<commit_message>
Updated links and fixed errors
</commit_message>
<xml_diff>
--- a/DSA_450_LoveBabbar.xlsx
+++ b/DSA_450_LoveBabbar.xlsx
@@ -198,10 +198,10 @@
     <t xml:space="preserve">Find a specific pair in matrix</t>
   </si>
   <si>
-    <t xml:space="preserve">sud</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kth smallest element in a row-cpumn wise sorted matrix</t>
+    <t xml:space="preserve">Rotate a matrix by 90deg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kth smallest element in a row-column wise sorted matrix</t>
   </si>
   <si>
     <t xml:space="preserve">Common elements in all rows of a given matrix</t>
@@ -1836,8 +1836,8 @@
   </sheetPr>
   <dimension ref="A1:D467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2438,7 +2438,7 @@
       </c>
       <c r="D48" s="12"/>
     </row>
-    <row r="49" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="n">
         <f aca="false">A48 + 1</f>
         <v>44</v>
@@ -7783,407 +7783,408 @@
     <hyperlink ref="C46" r:id="rId42" display="Print elements in sorted order using row-column wise sorted matrix (generalised form: MxN matrix)"/>
     <hyperlink ref="C47" r:id="rId43" display="Maximum size rectangle"/>
     <hyperlink ref="C48" r:id="rId44" display="Find a specific pair in matrix"/>
-    <hyperlink ref="C50" r:id="rId45" display="Kth smallest element in a row-cpumn wise sorted matrix"/>
-    <hyperlink ref="C51" r:id="rId46" display="Common elements in all rows of a given matrix"/>
-    <hyperlink ref="C52" r:id="rId47" display="Reverse a String"/>
-    <hyperlink ref="C53" r:id="rId48" display="Check whether a String is Palindrome or not"/>
-    <hyperlink ref="C54" r:id="rId49" display="Find Duplicate characters in a string"/>
-    <hyperlink ref="C56" r:id="rId50" display="Write a Code to check whether one string is a rotation of another"/>
-    <hyperlink ref="C57" r:id="rId51" display="Write a Program to check whether a string is a valid shuffle of two strings or not"/>
-    <hyperlink ref="C58" r:id="rId52" display="Count and Say problem"/>
-    <hyperlink ref="C59" r:id="rId53" display="Write a program to find the longest Palindrome in a string.[ Longest palindromic Substring]"/>
-    <hyperlink ref="C60" r:id="rId54" display="Find Longest Recurring Subsequence in String"/>
-    <hyperlink ref="C61" r:id="rId55" display="Print all Subsequences of a string."/>
-    <hyperlink ref="C62" r:id="rId56" display="Print all the permutations of the given string"/>
-    <hyperlink ref="C63" r:id="rId57" display="Split the Binary string into two substring with equal 0’s and 1’s"/>
-    <hyperlink ref="C64" r:id="rId58" display="Word Wrap Problem [VERY IMP]."/>
-    <hyperlink ref="C65" r:id="rId59" display="EDIT Distance [Very Imp]"/>
-    <hyperlink ref="C66" r:id="rId60" display="Find next greater number with same set of digits. [Very Very IMP]"/>
-    <hyperlink ref="C67" r:id="rId61" display="Balanced Parenthesis problem.[Imp]"/>
-    <hyperlink ref="C68" r:id="rId62" display="Word break Problem[ Very Imp]"/>
-    <hyperlink ref="C69" r:id="rId63" display="Rabin Karp Algo"/>
-    <hyperlink ref="C70" r:id="rId64" display="KMP Algo"/>
-    <hyperlink ref="C71" r:id="rId65" display="Convert a Sentence into its equivalent mobile numeric keypad sequence."/>
-    <hyperlink ref="C72" r:id="rId66" display="Minimum number of bracket reversals needed to make an expression balanced."/>
-    <hyperlink ref="C73" r:id="rId67" display="Count All Palindromic Subsequence in a given String."/>
-    <hyperlink ref="C74" r:id="rId68" display="Count of number of given string in 2D character array"/>
-    <hyperlink ref="C75" r:id="rId69" display="Search a Word in a 2D Grid of characters."/>
-    <hyperlink ref="C76" r:id="rId70" display="Boyer Moore Algorithm for Pattern Searching."/>
-    <hyperlink ref="C77" r:id="rId71" display="Converting Roman Numerals to Decimal"/>
-    <hyperlink ref="C78" r:id="rId72" display="Longest Common Prefix"/>
-    <hyperlink ref="C79" r:id="rId73" display="Number of flips to make binary string alternate"/>
-    <hyperlink ref="C80" r:id="rId74" display="Find the first repeated word in string."/>
-    <hyperlink ref="C81" r:id="rId75" display="Minimum number of swaps for bracket balancing."/>
-    <hyperlink ref="C82" r:id="rId76" display="Find the longest common subsequence between two strings."/>
-    <hyperlink ref="C83" r:id="rId77" display="Program to generate all possible valid IP addresses from given  string."/>
-    <hyperlink ref="C84" r:id="rId78" display="Write a program tofind the smallest window that contains all characters of string itself."/>
-    <hyperlink ref="C85" r:id="rId79" display="Rearrange characters in a string such that no two adjacent are same"/>
-    <hyperlink ref="C86" r:id="rId80" display="Minimum characters to be added at front to make string palindrome"/>
-    <hyperlink ref="C87" r:id="rId81" display="Given a sequence of words, print all anagrams together"/>
-    <hyperlink ref="C88" r:id="rId82" display="Find the smallest window in a string containing all characters of another string"/>
-    <hyperlink ref="C89" r:id="rId83" display="Recursively remove all adjacent duplicates"/>
-    <hyperlink ref="C90" r:id="rId84" display="String matching where one string contains wildcard characters"/>
-    <hyperlink ref="C91" r:id="rId85" display="Function to find Number of customers who could not get a computer"/>
-    <hyperlink ref="C92" r:id="rId86" display="Transform One String to Another using Minimum Number of Given Operation"/>
-    <hyperlink ref="C93" r:id="rId87" display="Check if two given strings are isomorphic to each other"/>
-    <hyperlink ref="C94" r:id="rId88" display="Recursively print all sentences that can be formed from list of word lists"/>
-    <hyperlink ref="C95" r:id="rId89" display="Find first and last positions of an element in a sorted array"/>
-    <hyperlink ref="C96" r:id="rId90" display="Find a Fixed Point (Value equal to index) in a given array"/>
-    <hyperlink ref="C97" r:id="rId91" display="Search in a rotated sorted array"/>
-    <hyperlink ref="C98" r:id="rId92" display="square root of an integer"/>
-    <hyperlink ref="C99" r:id="rId93" display="Maximum and minimum of an array using minimum number of comparisons"/>
-    <hyperlink ref="C100" r:id="rId94" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." display="Optimum location of point to minimize total distance"/>
-    <hyperlink ref="C101" r:id="rId95" display="Find the repeating and the missing"/>
-    <hyperlink ref="C102" r:id="rId96" display="find majority element"/>
-    <hyperlink ref="C103" r:id="rId97" display="Searching in an array where adjacent differ by at most k"/>
-    <hyperlink ref="C104" r:id="rId98" display="find a pair with a given difference"/>
-    <hyperlink ref="C105" r:id="rId99" display="find four elements that sum to a given value"/>
-    <hyperlink ref="C106" r:id="rId100" display="maximum sum such that no 2 elements are adjacent"/>
-    <hyperlink ref="C107" r:id="rId101" display="Count triplet with sum smaller than a given value"/>
-    <hyperlink ref="C108" r:id="rId102" display="merge 2 sorted arrays"/>
-    <hyperlink ref="C109" r:id="rId103" display="print all subarrays with 0 sum"/>
-    <hyperlink ref="C110" r:id="rId104" display="Product array Puzzle"/>
-    <hyperlink ref="C111" r:id="rId105" display="Sort array according to count of set bits"/>
-    <hyperlink ref="C112" r:id="rId106" display="minimum no. of swaps required to sort the array"/>
-    <hyperlink ref="C113" r:id="rId107" display="Bishu and Soldiers"/>
-    <hyperlink ref="C114" r:id="rId108" display="Rasta and Kheshtak"/>
-    <hyperlink ref="C115" r:id="rId109" display="Kth smallest number again"/>
-    <hyperlink ref="C116" r:id="rId110" display="Find pivot element in a sorted array"/>
-    <hyperlink ref="C117" r:id="rId111" display="K-th Element of Two Sorted Arrays"/>
-    <hyperlink ref="C118" r:id="rId112" display="Aggressive cows"/>
-    <hyperlink ref="C119" r:id="rId113" display="Book Allocation Problem"/>
-    <hyperlink ref="C120" r:id="rId114" display="EKOSPOJ:"/>
-    <hyperlink ref="C121" r:id="rId115" display="Job Scheduling Algo"/>
-    <hyperlink ref="C122" r:id="rId116" display="Missing Number in AP"/>
-    <hyperlink ref="C123" r:id="rId117" display="Smallest number with atleastn trailing zeroes infactorial"/>
-    <hyperlink ref="C124" r:id="rId118" display="Painters Partition Problem:"/>
-    <hyperlink ref="C125" r:id="rId119" display="ROTI-Prata SPOJ"/>
-    <hyperlink ref="C126" r:id="rId120" display="DoubleHelix SPOJ"/>
-    <hyperlink ref="C127" r:id="rId121" display="Subset Sums"/>
-    <hyperlink ref="C128" r:id="rId122" display="Findthe inversion count"/>
-    <hyperlink ref="C129" r:id="rId123" display="Implement Merge-sort in-place"/>
-    <hyperlink ref="C130" r:id="rId124" display="Partitioning and Sorting Arrays with Many Repeated Entries"/>
-    <hyperlink ref="C131" r:id="rId125" display="Write a Program to reverse the Linked List. (Both Iterative and recursive)"/>
-    <hyperlink ref="C132" r:id="rId126" display="Reverse a Linked List in group of Given Size. [Very Imp]"/>
-    <hyperlink ref="C133" r:id="rId127" display="Write a program to Detect loop in a linked list."/>
-    <hyperlink ref="C134" r:id="rId128" display="Write a program to Delete loop in a linked list."/>
-    <hyperlink ref="C135" r:id="rId129" display="Find the starting point of the loop. "/>
-    <hyperlink ref="C136" r:id="rId130" display="Remove Duplicates in a sorted Linked List."/>
-    <hyperlink ref="C137" r:id="rId131" display="Remove Duplicates in a Un-sorted Linked List."/>
-    <hyperlink ref="C138" r:id="rId132" display="Write a Program to Move the last element to Front in a Linked List."/>
-    <hyperlink ref="C139" r:id="rId133" display="Add “1” to a number represented as a Linked List."/>
-    <hyperlink ref="C140" r:id="rId134" display="Add two numbers represented by linked lists."/>
-    <hyperlink ref="C141" r:id="rId135" display="Intersection of two Sorted Linked List."/>
-    <hyperlink ref="C142" r:id="rId136" display="Intersection Point of two Linked Lists."/>
-    <hyperlink ref="C143" r:id="rId137" display="Merge Sort For Linked lists.[Very Important]"/>
-    <hyperlink ref="C144" r:id="rId138" display="Quicksort for Linked Lists.[Very Important]"/>
-    <hyperlink ref="C145" r:id="rId139" display="Find the middle Element of a linked list."/>
-    <hyperlink ref="C146" r:id="rId140" display="Check if a linked list is a circular linked list."/>
-    <hyperlink ref="C147" r:id="rId141" display="Split a Circular linked list into two halves."/>
-    <hyperlink ref="C148" r:id="rId142" display="Write a Program to check whether the Singly Linked list is a palindrome or not."/>
-    <hyperlink ref="C149" r:id="rId143" display="Deletion from a Circular Linked List."/>
-    <hyperlink ref="C150" r:id="rId144" display="Reverse a Doubly Linked list."/>
-    <hyperlink ref="C151" r:id="rId145" display="Find pairs with a given sum in a DLL."/>
-    <hyperlink ref="C152" r:id="rId146" display="Count triplets in a sorted DLL whose sum is equal to given value “X”."/>
-    <hyperlink ref="C153" r:id="rId147" display="Sort a “k”sorted Doubly Linked list.[Very IMP]"/>
-    <hyperlink ref="C154" r:id="rId148" display="Rotate DoublyLinked list by N nodes."/>
-    <hyperlink ref="C155" r:id="rId149" display="Rotate a Doubly Linked list in group of Given Size.[Very IMP]"/>
-    <hyperlink ref="C158" r:id="rId150" display="Flatten a Linked List"/>
-    <hyperlink ref="C159" r:id="rId151" display="Sort a LL of 0's, 1's and 2's"/>
-    <hyperlink ref="C160" r:id="rId152" display="Clone a linked list with next and random pointer"/>
-    <hyperlink ref="C161" r:id="rId153" display="Merge K sorted Linked list"/>
-    <hyperlink ref="C162" r:id="rId154" display="Multiply 2 no. represented by LL"/>
-    <hyperlink ref="C163" r:id="rId155" display="Delete nodes which have a greater value on right side"/>
-    <hyperlink ref="C164" r:id="rId156" display="Segregate even and odd nodes in a Linked List"/>
-    <hyperlink ref="C165" r:id="rId157" display="Program for n’th node from the end of a Linked List"/>
-    <hyperlink ref="C166" r:id="rId158" display="Find the first non-repeating character from a stream of characters"/>
-    <hyperlink ref="C167" r:id="rId159" display="level order traversal"/>
-    <hyperlink ref="C168" r:id="rId160" display="Reverse Level Order traversal"/>
-    <hyperlink ref="C169" r:id="rId161" display="Height of a tree"/>
-    <hyperlink ref="C170" r:id="rId162" display="Diameter of a tree"/>
-    <hyperlink ref="C171" r:id="rId163" display="Mirror of a tree"/>
-    <hyperlink ref="C172" r:id="rId164" display="Inorder Traversal of a tree both using recursion and Iteration"/>
-    <hyperlink ref="C173" r:id="rId165" display="Preorder Traversal of a tree both using recursion and Iteration"/>
-    <hyperlink ref="C174" r:id="rId166" display="Postorder Traversal of a tree both using recursion and Iteration"/>
-    <hyperlink ref="C175" r:id="rId167" display="Left View of a tree"/>
-    <hyperlink ref="C176" r:id="rId168" display="Right View of Tree"/>
-    <hyperlink ref="C177" r:id="rId169" display="Top View of a tree"/>
-    <hyperlink ref="C178" r:id="rId170" display="Bottom View of a tree"/>
-    <hyperlink ref="C179" r:id="rId171" display="Zig-Zag traversal of a binary tree"/>
-    <hyperlink ref="C180" r:id="rId172" display="Check if a tree is balanced or not"/>
-    <hyperlink ref="C181" r:id="rId173" display="Diagnol Traversal of a Binary tree"/>
-    <hyperlink ref="C182" r:id="rId174" display="Boundary traversal of a Binary tree"/>
-    <hyperlink ref="C183" r:id="rId175" display="Construct Binary Tree from String with Bracket Representation"/>
-    <hyperlink ref="C184" r:id="rId176" display="Convert Binary tree into Doubly Linked List"/>
-    <hyperlink ref="C185" r:id="rId177" display="Convert Binary tree into Sum tree"/>
-    <hyperlink ref="C186" r:id="rId178" display="Construct Binary tree from Inorder and preorder traversal"/>
-    <hyperlink ref="C187" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." display="Find minimum swaps required to convert a Binary tree into BST"/>
-    <hyperlink ref="C188" r:id="rId180" display="Check if Binary tree is Sum tree or not"/>
-    <hyperlink ref="C189" r:id="rId181" display="Check if all leaf nodes are at same level or not"/>
-    <hyperlink ref="C190" r:id="rId182" display="Check if a Binary Tree contains duplicate subtrees of size 2 or more [ IMP ]"/>
-    <hyperlink ref="C191" r:id="rId183" display="Check if 2 trees are mirror or not"/>
-    <hyperlink ref="C192" r:id="rId184" display="Sum of Nodes on the Longest path from root to leaf node "/>
-    <hyperlink ref="C193" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." display="Check if given graph is tree or not.  [ IMP ]"/>
-    <hyperlink ref="C194" r:id="rId186" display="Find Largest subtree sum in a tree"/>
-    <hyperlink ref="C195" r:id="rId187" display="Maximum Sum of nodes in Binary tree such that no two are adjacent "/>
-    <hyperlink ref="C196" r:id="rId188" display="Print all &quot;K&quot; Sum paths in a Binary tree"/>
-    <hyperlink ref="C197" r:id="rId189" display="Find LCA in a Binary tree"/>
-    <hyperlink ref="C198" r:id="rId190" display="Find distance between 2 nodes in a Binary tree"/>
-    <hyperlink ref="C199" r:id="rId191" display="Kth Ancestor of node in a Binary tree"/>
-    <hyperlink ref="C200" r:id="rId192" display="Find all Duplicate subtrees in a Binary tree [ IMP ]"/>
-    <hyperlink ref="C201" r:id="rId193" display="Tree Isomorphism Problem"/>
-    <hyperlink ref="C202" r:id="rId194" display="Fina a value in a BST"/>
-    <hyperlink ref="C203" r:id="rId195" display="Deletion of a node in a BST"/>
-    <hyperlink ref="C204" r:id="rId196" display="Find min and max value in a BST"/>
-    <hyperlink ref="C205" r:id="rId197" display="Find inorder successor and inorder predecessor in a BST"/>
-    <hyperlink ref="C206" r:id="rId198" display="Check if a tree is a BST or not "/>
-    <hyperlink ref="C207" r:id="rId199" display="Populate Inorder successor of all nodes"/>
-    <hyperlink ref="C208" r:id="rId200" display="Find LCA  of 2 nodes in a BST"/>
-    <hyperlink ref="C209" r:id="rId201" display="Construct BST from preorder traversal"/>
-    <hyperlink ref="C210" r:id="rId202" display="Convert Binary tree into BST"/>
-    <hyperlink ref="C211" r:id="rId203" display="Convert a normal BST into a Balanced BST"/>
-    <hyperlink ref="C212" r:id="rId204" display="Merge two BST [ V.V.V&gt;IMP ]"/>
-    <hyperlink ref="C213" r:id="rId205" display="Find Kth largest element in a BST"/>
-    <hyperlink ref="C214" r:id="rId206" display="Find Kth smallest element in a BST"/>
-    <hyperlink ref="C215" r:id="rId207" display="Count pairs from 2 BST whose sum is equal to given value &quot;X&quot;"/>
-    <hyperlink ref="C216" r:id="rId208" display="Find the median of BST in O(n) time and O(1) space"/>
-    <hyperlink ref="C217" r:id="rId209" display="Count BST ndoes that lie in a given range"/>
-    <hyperlink ref="C218" r:id="rId210" display="Replace every element with the least greater element on its right"/>
-    <hyperlink ref="C219" r:id="rId211" display="Given &quot;n&quot; appointments, find the conflicting appointments"/>
-    <hyperlink ref="C220" r:id="rId212" display="Check preorder is valid or not"/>
-    <hyperlink ref="C221" r:id="rId213" display="Check whether BST contains Dead end"/>
-    <hyperlink ref="C222" r:id="rId214" display="Largest BST in a Binary Tree [ V.V.V.V.V IMP ]"/>
-    <hyperlink ref="C223" r:id="rId215" display="Flatten BST to sorted list"/>
-    <hyperlink ref="C224" r:id="rId216" display="Activity Selection Problem"/>
-    <hyperlink ref="C225" r:id="rId217" display="Job SequencingProblem"/>
-    <hyperlink ref="C226" r:id="rId218" display="Huffman Coding"/>
-    <hyperlink ref="C227" r:id="rId219" display="Water Connection Problem"/>
-    <hyperlink ref="C228" r:id="rId220" display="Fractional Knapsack Problem"/>
-    <hyperlink ref="C229" r:id="rId221" display="Greedy Algorithm to find Minimum number of Coins"/>
-    <hyperlink ref="C230" r:id="rId222" display="Maximum trains for which stoppage can be provided"/>
-    <hyperlink ref="C231" r:id="rId223" display="Minimum Platforms Problem"/>
-    <hyperlink ref="C232" r:id="rId224" display="Buy Maximum Stocks if i stocks can be bought on i-th day"/>
-    <hyperlink ref="C233" r:id="rId225" display="Find the minimum and maximum amount to buy all N candies"/>
-    <hyperlink ref="C234" r:id="rId226" display="Minimize Cash Flow among a given set of friends who have borrowed money from each other"/>
-    <hyperlink ref="C235" r:id="rId227" display="Minimum Cost to cut a board into squares"/>
-    <hyperlink ref="C236" r:id="rId228" display="Check if it is possible to survive on Island"/>
-    <hyperlink ref="C237" r:id="rId229" display="Find maximum meetings in one room"/>
-    <hyperlink ref="C238" r:id="rId230" display="Maximum product subset of an array"/>
-    <hyperlink ref="C239" r:id="rId231" display="Maximize array sum after K negations"/>
-    <hyperlink ref="C240" r:id="rId232" display="Maximize the sum of arr[i]*i"/>
-    <hyperlink ref="C241" r:id="rId233" display="Maximum sum of absolute difference of an array"/>
-    <hyperlink ref="C242" r:id="rId234" display="Maximize sum of consecutive differences in a circular array"/>
-    <hyperlink ref="C243" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." display="Minimum sum of absolute difference of pairs of two arrays"/>
-    <hyperlink ref="C244" r:id="rId236" display="Program for Shortest Job First (or SJF) CPU Scheduling"/>
-    <hyperlink ref="C245" r:id="rId237" display="Program for Least Recently Used (LRU) Page Replacement algorithm"/>
-    <hyperlink ref="C246" r:id="rId238" display="Smallest subset with sum greater than all other elements"/>
-    <hyperlink ref="C247" r:id="rId239" display="Chocolate Distribution Problem"/>
-    <hyperlink ref="C248" r:id="rId240" display="DEFKIN -Defense of a Kingdom"/>
-    <hyperlink ref="C249" r:id="rId241" display="DIEHARD -DIE HARD"/>
-    <hyperlink ref="C250" r:id="rId242" display="GERGOVIA -Wine trading in Gergovia"/>
-    <hyperlink ref="C251" r:id="rId243" display="Picking Up Chicks"/>
-    <hyperlink ref="C252" r:id="rId244" display="CHOCOLA –Chocolate"/>
-    <hyperlink ref="C253" r:id="rId245" display="ARRANGE -Arranging Amplifiers"/>
-    <hyperlink ref="C254" r:id="rId246" display="K Centers Problem"/>
-    <hyperlink ref="C255" r:id="rId247" display="Minimum Cost of ropes"/>
-    <hyperlink ref="C256" r:id="rId248" display="Find smallest number with given number of digits and sum of digits"/>
-    <hyperlink ref="C257" r:id="rId249" display="Rearrange characters in a string such that no two adjacent are same"/>
-    <hyperlink ref="C258" r:id="rId250" display="Find maximum sum possible equal sum of three stacks"/>
-    <hyperlink ref="C259" r:id="rId251" display="Rat in a maze Problem"/>
-    <hyperlink ref="C260" r:id="rId252" display="Printing all solutions in N-Queen Problem"/>
-    <hyperlink ref="C261" r:id="rId253" display="Word Break Problem using Backtracking"/>
-    <hyperlink ref="C262" r:id="rId254" display="Remove Invalid Parentheses"/>
-    <hyperlink ref="C263" r:id="rId255" display="Sudoku Solver"/>
-    <hyperlink ref="C264" r:id="rId256" display="m Coloring Problem"/>
-    <hyperlink ref="C265" r:id="rId257" display="Print all palindromic partitions of a string"/>
-    <hyperlink ref="C266" r:id="rId258" display="Subset Sum Problem"/>
-    <hyperlink ref="C267" r:id="rId259" display="The Knight’s tour problem"/>
-    <hyperlink ref="C268" r:id="rId260" display="Tug of War"/>
-    <hyperlink ref="C269" r:id="rId261" display="Find shortest safe route in a path with landmines"/>
-    <hyperlink ref="C270" r:id="rId262" display="Combinational Sum"/>
-    <hyperlink ref="C271" r:id="rId263" display="Find Maximum number possible by doing at-most K swaps"/>
-    <hyperlink ref="C272" r:id="rId264" display="Print all permutations of a string "/>
-    <hyperlink ref="C273" r:id="rId265" display="Find if there is a path of more than k length from a source"/>
-    <hyperlink ref="C274" r:id="rId266" display="Longest Possible Route in a Matrix with Hurdles"/>
-    <hyperlink ref="C275" r:id="rId267" display="Print all possible paths from top left to bottom right of a mXn matrix"/>
-    <hyperlink ref="C276" r:id="rId268" display="Partition of a set intoK subsets with equal sum"/>
-    <hyperlink ref="C277" r:id="rId269" display="Find the K-th Permutation Sequence of first N natural numbers"/>
-    <hyperlink ref="C278" r:id="rId270" display=" Implement Stack from Scratch"/>
-    <hyperlink ref="C279" r:id="rId271" display=" Implement Queue from Scratch"/>
-    <hyperlink ref="C280" r:id="rId272" display="Implement 2 stack in an array"/>
-    <hyperlink ref="C281" r:id="rId273" display="find the middle element of a stack"/>
-    <hyperlink ref="C282" r:id="rId274" display="Implement &quot;N&quot; stacks in an Array"/>
-    <hyperlink ref="C283" r:id="rId275" display="Check the expression has valid or Balanced parenthesis or not."/>
-    <hyperlink ref="C284" r:id="rId276" display="Reverse a String using Stack"/>
-    <hyperlink ref="C285" r:id="rId277" display="Design a Stack that supports getMin() in O(1) time and O(1) extra space."/>
-    <hyperlink ref="C286" r:id="rId278" display="Find the next Greater element"/>
-    <hyperlink ref="C287" r:id="rId279" display="The celebrity Problem"/>
-    <hyperlink ref="C288" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." display="Arithmetic Expression evaluation"/>
-    <hyperlink ref="C289" r:id="rId281" display="Evaluation of Postfix expression"/>
-    <hyperlink ref="C290" r:id="rId282" display="Implement a method to insert an element at its bottom without using any other data structure."/>
-    <hyperlink ref="C291" r:id="rId283" display="Reverse a stack using recursion"/>
-    <hyperlink ref="C292" r:id="rId284" display="Sort a Stack using recursion"/>
-    <hyperlink ref="C293" r:id="rId285" display="Merge Overlapping Intervals"/>
-    <hyperlink ref="C294" r:id="rId286" display="Largest rectangular Area in Histogram"/>
-    <hyperlink ref="C295" r:id="rId287" display="Length of the Longest Valid Substring"/>
-    <hyperlink ref="C296" r:id="rId288" display="Expression contains redundant bracket or not"/>
-    <hyperlink ref="C297" r:id="rId289" display="Implement Stack using Queue"/>
-    <hyperlink ref="C298" r:id="rId290" display="Implement Stack using Deque"/>
-    <hyperlink ref="C299" r:id="rId291" display="Stack Permutations (Check if an array is stack permutation of other)"/>
-    <hyperlink ref="C300" r:id="rId292" display="Implement Queue using Stack  "/>
-    <hyperlink ref="C301" r:id="rId293" display="Implement &quot;n&quot; queue in an array"/>
-    <hyperlink ref="C302" r:id="rId294" display="Implement a Circular queue"/>
-    <hyperlink ref="C303" r:id="rId295" display="LRU Cache Implementationa"/>
-    <hyperlink ref="C304" r:id="rId296" display="Reverse a Queue using recursion"/>
-    <hyperlink ref="C305" r:id="rId297" display="Reverse the first “K” elements of a queue"/>
-    <hyperlink ref="C306" r:id="rId298" display="Interleave the first half of the queue with second half"/>
-    <hyperlink ref="C307" r:id="rId299" display="Find the first circular tour that visits all Petrol Pumps"/>
-    <hyperlink ref="C308" r:id="rId300" display="Minimum time required to rot all oranges"/>
-    <hyperlink ref="C309" r:id="rId301" display="Distance of nearest cell having 1 in a binary matrix"/>
-    <hyperlink ref="C310" r:id="rId302" display="First negative integer in every window of size “k”"/>
-    <hyperlink ref="C311" r:id="rId303" display="Check if all levels of two trees are anagrams or not."/>
-    <hyperlink ref="C312" r:id="rId304" display="Sum of minimum and maximum elements of all subarrays of size “k”."/>
-    <hyperlink ref="C313" r:id="rId305" display="Minimum sum of squares of character counts in a given string after removing “k” characters."/>
-    <hyperlink ref="C314" r:id="rId306" display="Queue based approach or first non-repeating character in a stream."/>
-    <hyperlink ref="C315" r:id="rId307" display="Next Smaller Element"/>
-    <hyperlink ref="C316" r:id="rId308" display="Implement a Maxheap/MinHeap using arrays and recursion."/>
-    <hyperlink ref="C317" r:id="rId309" display="Sort an Array using heap. (HeapSort)"/>
-    <hyperlink ref="C318" r:id="rId310" display="Maximum of all subarrays of size k."/>
-    <hyperlink ref="C319" r:id="rId311" display="“k” largest element in an array"/>
-    <hyperlink ref="C320" r:id="rId312" display="Kth smallest and largest element in an unsorted array"/>
-    <hyperlink ref="C321" r:id="rId313" display="Merge “K” sorted arrays. [ IMP ]"/>
-    <hyperlink ref="C322" r:id="rId314" display="Merge 2 Binary Max Heaps"/>
-    <hyperlink ref="C323" r:id="rId315" display="Kth largest sum continuous subarrays"/>
-    <hyperlink ref="C324" r:id="rId316" display="Leetcode- reorganize strings"/>
-    <hyperlink ref="C325" r:id="rId317" display="Merge “K” Sorted Linked Lists [V.IMP]"/>
-    <hyperlink ref="C326" r:id="rId318" display="Smallest range in “K” Lists"/>
-    <hyperlink ref="C327" r:id="rId319" display="Median in a stream of Integers"/>
-    <hyperlink ref="C328" r:id="rId320" display="Check if a Binary Tree is Heap"/>
-    <hyperlink ref="C329" r:id="rId321" display="Connect “n” ropes with minimum cost"/>
-    <hyperlink ref="C330" r:id="rId322" display="Convert BST to Min Heap"/>
-    <hyperlink ref="C331" r:id="rId323" display="Convert min heap to max heap"/>
-    <hyperlink ref="C332" r:id="rId324" display="Rearrange characters in a string such that no two adjacent are same."/>
-    <hyperlink ref="C333" r:id="rId325" display="Minimum sum of two numbers formed from digits of an array"/>
-    <hyperlink ref="C334" r:id="rId326" display="Create a Graph, print it"/>
-    <hyperlink ref="C335" r:id="rId327" display="Implement BFS algorithm "/>
-    <hyperlink ref="C336" r:id="rId328" display="Implement DFS Algo "/>
-    <hyperlink ref="C337" r:id="rId329" display="Detect Cycle in Directed Graph using BFS/DFS Algo "/>
-    <hyperlink ref="C338" r:id="rId330" display="Detect Cycle in UnDirected Graph using BFS/DFS Algo "/>
-    <hyperlink ref="C339" r:id="rId331" display="Search in a Maze"/>
-    <hyperlink ref="C340" r:id="rId332" display="Minimum Step by Knight"/>
-    <hyperlink ref="C341" r:id="rId333" display="flood fill algo"/>
-    <hyperlink ref="C342" r:id="rId334" display="Clone a graph"/>
-    <hyperlink ref="C343" r:id="rId335" display="Making wired Connections"/>
-    <hyperlink ref="C344" r:id="rId336" display="word Ladder "/>
-    <hyperlink ref="C345" r:id="rId337" display="Dijkstra algo"/>
-    <hyperlink ref="C346" r:id="rId338" display="Implement Topological Sort "/>
-    <hyperlink ref="C347" r:id="rId339" display="Minimum time taken by each job to be completed given by a Directed Acyclic Graph"/>
-    <hyperlink ref="C348" r:id="rId340" display="Find whether it is possible to finish all tasks or not from given dependencies"/>
-    <hyperlink ref="C349" r:id="rId341" display="Find the no. of Isalnds"/>
-    <hyperlink ref="C350" r:id="rId342" display="Given a sorted Dictionary of an Alien Language, find order of characters"/>
-    <hyperlink ref="C351" r:id="rId343" display="Implement Kruksal’sAlgorithm"/>
-    <hyperlink ref="C352" r:id="rId344" display="Implement Prim’s Algorithm"/>
-    <hyperlink ref="C353" r:id="rId345" display="Total no. of Spanning tree in a graph"/>
-    <hyperlink ref="C354" r:id="rId346" display="Implement Bellman Ford Algorithm"/>
-    <hyperlink ref="C355" r:id="rId347" display="Implement Floyd warshallAlgorithm"/>
-    <hyperlink ref="C356" r:id="rId348" display="Travelling Salesman Problem"/>
-    <hyperlink ref="C357" r:id="rId349" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." display="Graph ColouringProblem"/>
-    <hyperlink ref="C358" r:id="rId350" display="Snake and Ladders Problem"/>
-    <hyperlink ref="C359" r:id="rId351" display="Find bridge in a graph"/>
-    <hyperlink ref="C360" r:id="rId352" display="Count Strongly connected Components(Kosaraju Algo)"/>
-    <hyperlink ref="C361" r:id="rId353" display="Check whether a graph is Bipartite or Not"/>
-    <hyperlink ref="C362" r:id="rId354" display="Detect Negative cycle in a graph"/>
-    <hyperlink ref="C363" r:id="rId355" display="Longest path in a Directed Acyclic Graph"/>
-    <hyperlink ref="C364" r:id="rId356" display="Journey to the Moon"/>
-    <hyperlink ref="C365" r:id="rId357" display="Cheapest Flights Within K Stops"/>
-    <hyperlink ref="C366" r:id="rId358" display="Oliver and the Game"/>
-    <hyperlink ref="C367" r:id="rId359" display="Water Jug problem using BFS"/>
-    <hyperlink ref="C368" r:id="rId360" display="Water Jug problem using BFS"/>
-    <hyperlink ref="C369" r:id="rId361" display="Find if there is a path of more thank length from a source"/>
-    <hyperlink ref="C370" r:id="rId362" display="M-ColouringProblem"/>
-    <hyperlink ref="C371" r:id="rId363" display="Minimum edges to reverse o make path from source to destination"/>
-    <hyperlink ref="C372" r:id="rId364" display="Paths to travel each nodes using each edge(Seven Bridges)"/>
-    <hyperlink ref="C373" r:id="rId365" display="Vertex Cover Problem"/>
-    <hyperlink ref="C374" r:id="rId366" display="Chinese Postman or Route Inspection"/>
-    <hyperlink ref="C375" r:id="rId367" display="Number of Triangles in a Directed and Undirected Graph"/>
-    <hyperlink ref="C376" r:id="rId368" display="Minimise the cashflow among a given set of friends who have borrowed money from each other"/>
-    <hyperlink ref="C377" r:id="rId369" display="Two Clique Problem"/>
-    <hyperlink ref="C378" r:id="rId370" display="Construct a trie from scratch"/>
-    <hyperlink ref="C379" r:id="rId371" display="Find shortest unique prefix for every word in a given list"/>
-    <hyperlink ref="C380" r:id="rId372" display="Word Break Problem | (Trie solution)"/>
-    <hyperlink ref="C381" r:id="rId373" display="Given a sequence of words, print all anagrams together"/>
-    <hyperlink ref="C382" r:id="rId374" display="Implement a Phone Directory"/>
-    <hyperlink ref="C383" r:id="rId375" display="Print unique rows in a given boolean matrix"/>
-    <hyperlink ref="C384" r:id="rId376" display="Coin ChangeProblem"/>
-    <hyperlink ref="C385" r:id="rId377" display="Knapsack Problem"/>
-    <hyperlink ref="C386" r:id="rId378" display="Binomial CoefficientProblem"/>
-    <hyperlink ref="C387" r:id="rId379" display="Permutation CoefficientProblem"/>
-    <hyperlink ref="C388" r:id="rId380" display="Program for nth Catalan Number"/>
-    <hyperlink ref="C389" r:id="rId381" display="Matrix Chain Multiplication "/>
-    <hyperlink ref="C390" r:id="rId382" display="Edit Distance"/>
-    <hyperlink ref="C391" r:id="rId383" display="Subset Sum Problem"/>
-    <hyperlink ref="C392" r:id="rId384" display="Friends Pairing Problem"/>
-    <hyperlink ref="C393" r:id="rId385" display="Gold Mine Problem"/>
-    <hyperlink ref="C394" r:id="rId386" display="Assembly Line SchedulingProblem"/>
-    <hyperlink ref="C395" r:id="rId387" display="Painting the Fenceproblem"/>
-    <hyperlink ref="C396" r:id="rId388" display="Maximize The Cut Segments"/>
-    <hyperlink ref="C397" r:id="rId389" display="Longest Common Subsequence"/>
-    <hyperlink ref="C398" r:id="rId390" display="Longest Repeated Subsequence"/>
-    <hyperlink ref="C399" r:id="rId391" display="Longest Increasing Subsequence"/>
-    <hyperlink ref="C400" r:id="rId392" display="Space Optimized Solution of LCS"/>
-    <hyperlink ref="C401" r:id="rId393" display="LCS (Longest Common Subsequence) of three strings"/>
-    <hyperlink ref="C402" r:id="rId394" display="Maximum Sum Increasing Subsequence"/>
-    <hyperlink ref="C403" r:id="rId395" display="Count all subsequences having product less than K"/>
-    <hyperlink ref="C404" r:id="rId396" display="Longest subsequence such that difference between adjacent is one"/>
-    <hyperlink ref="C405" r:id="rId397" display="Maximum subsequence sum such that no three are consecutive"/>
-    <hyperlink ref="C406" r:id="rId398" display="Egg Dropping Problem"/>
-    <hyperlink ref="C407" r:id="rId399" display="Maximum Length Chain of Pairs"/>
-    <hyperlink ref="C408" r:id="rId400" display="Maximum size square sub-matrix with all 1s"/>
-    <hyperlink ref="C409" r:id="rId401" display="Maximum sum of pairs with specific difference"/>
-    <hyperlink ref="C410" r:id="rId402" display="Min Cost PathProblem"/>
-    <hyperlink ref="C411" r:id="rId403" display="Maximum difference of zeros and ones in binary string"/>
-    <hyperlink ref="C412" r:id="rId404" display="Minimum number of jumps to reach end"/>
-    <hyperlink ref="C413" r:id="rId405" display="Minimum cost to fill given weight in a bag"/>
-    <hyperlink ref="C414" r:id="rId406" display="Minimum removals from array to make max –min &lt;= K"/>
-    <hyperlink ref="C415" r:id="rId407" display="Longest Common Substring"/>
-    <hyperlink ref="C416" r:id="rId408" display="Count number of ways to reacha given score in a game"/>
-    <hyperlink ref="C417" r:id="rId409" display="Count Balanced Binary Trees of Height h"/>
-    <hyperlink ref="C418" r:id="rId410" display="LargestSum Contiguous Subarray [V&gt;V&gt;V&gt;V IMP ]"/>
-    <hyperlink ref="C419" r:id="rId411" display="Smallest sum contiguous subarray"/>
-    <hyperlink ref="C420" r:id="rId412" display="Unbounded Knapsack (Repetition of items allowed)"/>
-    <hyperlink ref="C421" r:id="rId413" display="Word Break Problem"/>
-    <hyperlink ref="C422" r:id="rId414" display="Largest Independent Set Problem"/>
-    <hyperlink ref="C423" r:id="rId415" display="Partition problem"/>
-    <hyperlink ref="C424" r:id="rId416" display="Longest Palindromic Subsequence"/>
-    <hyperlink ref="C425" r:id="rId417" display="Count All Palindromic Subsequence in a given String"/>
-    <hyperlink ref="C426" r:id="rId418" display="Longest Palindromic Substring"/>
-    <hyperlink ref="C427" r:id="rId419" display="Longest alternating subsequence"/>
-    <hyperlink ref="C428" r:id="rId420" display="Weighted Job Scheduling"/>
-    <hyperlink ref="C429" r:id="rId421" display="Coin game winner where every player has three choices"/>
-    <hyperlink ref="C430" r:id="rId422" display="Count Derangements (Permutation such that no element appears in its original position) [ IMPORTANT ]"/>
-    <hyperlink ref="C431" r:id="rId423" display="Maximum profit by buying and selling a share at most twice [ IMP ]"/>
-    <hyperlink ref="C432" r:id="rId424" display="Optimal Strategy for a Game"/>
-    <hyperlink ref="C433" r:id="rId425" display="Optimal Binary Search Tree"/>
-    <hyperlink ref="C434" r:id="rId426" display="Palindrome PartitioningProblem"/>
-    <hyperlink ref="C435" r:id="rId427" display="Word Wrap Problem"/>
-    <hyperlink ref="C436" r:id="rId428" display="Mobile Numeric Keypad Problem [ IMP ]"/>
-    <hyperlink ref="C437" r:id="rId429" display="Boolean Parenthesization Problem"/>
-    <hyperlink ref="C438" r:id="rId430" display="Largest rectangular sub-matrix whose sum is 0"/>
-    <hyperlink ref="C439" r:id="rId431" display="Largest area rectangular sub-matrix with equal number of 1’s and 0’s [ IMP ]"/>
-    <hyperlink ref="C440" r:id="rId432" display="Maximum sum rectangle in a 2D matrix"/>
-    <hyperlink ref="C441" r:id="rId433" display="Maximum profit by buying and selling a share at most k times"/>
-    <hyperlink ref="C442" r:id="rId434" display="Find if a string is interleaved of two other strings"/>
-    <hyperlink ref="C443" r:id="rId435" display="Maximum Length of Pair Chain"/>
-    <hyperlink ref="C444" r:id="rId436" display="Count set bits in an integer"/>
-    <hyperlink ref="C445" r:id="rId437" display="Find the two non-repeating elements in an array of repeating elements"/>
-    <hyperlink ref="C446" r:id="rId438" display="Count number of bits to be flipped to convert A to B"/>
-    <hyperlink ref="C447" r:id="rId439" display="Count total set bits in all numbers from 1 to n"/>
-    <hyperlink ref="C448" r:id="rId440" display="Program to find whether a no is power of two"/>
-    <hyperlink ref="C449" r:id="rId441" display="Find position of the only set bit"/>
-    <hyperlink ref="C450" r:id="rId442" display="Copy set bits in a range"/>
-    <hyperlink ref="C451" r:id="rId443" display="Divide two integers without using multiplication, division and mod operator"/>
-    <hyperlink ref="C452" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." display="Calculate square of a number without using *, / and pow()"/>
-    <hyperlink ref="C453" r:id="rId445" display="Power Set"/>
+    <hyperlink ref="C49" r:id="rId45" display="Rotate a matrix by 90deg"/>
+    <hyperlink ref="C50" r:id="rId46" display="Kth smallest element in a row-column wise sorted matrix"/>
+    <hyperlink ref="C51" r:id="rId47" display="Common elements in all rows of a given matrix"/>
+    <hyperlink ref="C52" r:id="rId48" display="Reverse a String"/>
+    <hyperlink ref="C53" r:id="rId49" display="Check whether a String is Palindrome or not"/>
+    <hyperlink ref="C54" r:id="rId50" display="Find Duplicate characters in a string"/>
+    <hyperlink ref="C56" r:id="rId51" display="Write a Code to check whether one string is a rotation of another"/>
+    <hyperlink ref="C57" r:id="rId52" display="Write a Program to check whether a string is a valid shuffle of two strings or not"/>
+    <hyperlink ref="C58" r:id="rId53" display="Count and Say problem"/>
+    <hyperlink ref="C59" r:id="rId54" display="Write a program to find the longest Palindrome in a string.[ Longest palindromic Substring]"/>
+    <hyperlink ref="C60" r:id="rId55" display="Find Longest Recurring Subsequence in String"/>
+    <hyperlink ref="C61" r:id="rId56" display="Print all Subsequences of a string."/>
+    <hyperlink ref="C62" r:id="rId57" display="Print all the permutations of the given string"/>
+    <hyperlink ref="C63" r:id="rId58" display="Split the Binary string into two substring with equal 0’s and 1’s"/>
+    <hyperlink ref="C64" r:id="rId59" display="Word Wrap Problem [VERY IMP]."/>
+    <hyperlink ref="C65" r:id="rId60" display="EDIT Distance [Very Imp]"/>
+    <hyperlink ref="C66" r:id="rId61" display="Find next greater number with same set of digits. [Very Very IMP]"/>
+    <hyperlink ref="C67" r:id="rId62" display="Balanced Parenthesis problem.[Imp]"/>
+    <hyperlink ref="C68" r:id="rId63" display="Word break Problem[ Very Imp]"/>
+    <hyperlink ref="C69" r:id="rId64" display="Rabin Karp Algo"/>
+    <hyperlink ref="C70" r:id="rId65" display="KMP Algo"/>
+    <hyperlink ref="C71" r:id="rId66" display="Convert a Sentence into its equivalent mobile numeric keypad sequence."/>
+    <hyperlink ref="C72" r:id="rId67" display="Minimum number of bracket reversals needed to make an expression balanced."/>
+    <hyperlink ref="C73" r:id="rId68" display="Count All Palindromic Subsequence in a given String."/>
+    <hyperlink ref="C74" r:id="rId69" display="Count of number of given string in 2D character array"/>
+    <hyperlink ref="C75" r:id="rId70" display="Search a Word in a 2D Grid of characters."/>
+    <hyperlink ref="C76" r:id="rId71" display="Boyer Moore Algorithm for Pattern Searching."/>
+    <hyperlink ref="C77" r:id="rId72" display="Converting Roman Numerals to Decimal"/>
+    <hyperlink ref="C78" r:id="rId73" display="Longest Common Prefix"/>
+    <hyperlink ref="C79" r:id="rId74" display="Number of flips to make binary string alternate"/>
+    <hyperlink ref="C80" r:id="rId75" display="Find the first repeated word in string."/>
+    <hyperlink ref="C81" r:id="rId76" display="Minimum number of swaps for bracket balancing."/>
+    <hyperlink ref="C82" r:id="rId77" display="Find the longest common subsequence between two strings."/>
+    <hyperlink ref="C83" r:id="rId78" display="Program to generate all possible valid IP addresses from given  string."/>
+    <hyperlink ref="C84" r:id="rId79" display="Write a program tofind the smallest window that contains all characters of string itself."/>
+    <hyperlink ref="C85" r:id="rId80" display="Rearrange characters in a string such that no two adjacent are same"/>
+    <hyperlink ref="C86" r:id="rId81" display="Minimum characters to be added at front to make string palindrome"/>
+    <hyperlink ref="C87" r:id="rId82" display="Given a sequence of words, print all anagrams together"/>
+    <hyperlink ref="C88" r:id="rId83" display="Find the smallest window in a string containing all characters of another string"/>
+    <hyperlink ref="C89" r:id="rId84" display="Recursively remove all adjacent duplicates"/>
+    <hyperlink ref="C90" r:id="rId85" display="String matching where one string contains wildcard characters"/>
+    <hyperlink ref="C91" r:id="rId86" display="Function to find Number of customers who could not get a computer"/>
+    <hyperlink ref="C92" r:id="rId87" display="Transform One String to Another using Minimum Number of Given Operation"/>
+    <hyperlink ref="C93" r:id="rId88" display="Check if two given strings are isomorphic to each other"/>
+    <hyperlink ref="C94" r:id="rId89" display="Recursively print all sentences that can be formed from list of word lists"/>
+    <hyperlink ref="C95" r:id="rId90" display="Find first and last positions of an element in a sorted array"/>
+    <hyperlink ref="C96" r:id="rId91" display="Find a Fixed Point (Value equal to index) in a given array"/>
+    <hyperlink ref="C97" r:id="rId92" display="Search in a rotated sorted array"/>
+    <hyperlink ref="C98" r:id="rId93" display="square root of an integer"/>
+    <hyperlink ref="C99" r:id="rId94" display="Maximum and minimum of an array using minimum number of comparisons"/>
+    <hyperlink ref="C100" r:id="rId95" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." display="Optimum location of point to minimize total distance"/>
+    <hyperlink ref="C101" r:id="rId96" display="Find the repeating and the missing"/>
+    <hyperlink ref="C102" r:id="rId97" display="find majority element"/>
+    <hyperlink ref="C103" r:id="rId98" display="Searching in an array where adjacent differ by at most k"/>
+    <hyperlink ref="C104" r:id="rId99" display="find a pair with a given difference"/>
+    <hyperlink ref="C105" r:id="rId100" display="find four elements that sum to a given value"/>
+    <hyperlink ref="C106" r:id="rId101" display="maximum sum such that no 2 elements are adjacent"/>
+    <hyperlink ref="C107" r:id="rId102" display="Count triplet with sum smaller than a given value"/>
+    <hyperlink ref="C108" r:id="rId103" display="merge 2 sorted arrays"/>
+    <hyperlink ref="C109" r:id="rId104" display="print all subarrays with 0 sum"/>
+    <hyperlink ref="C110" r:id="rId105" display="Product array Puzzle"/>
+    <hyperlink ref="C111" r:id="rId106" display="Sort array according to count of set bits"/>
+    <hyperlink ref="C112" r:id="rId107" display="minimum no. of swaps required to sort the array"/>
+    <hyperlink ref="C113" r:id="rId108" display="Bishu and Soldiers"/>
+    <hyperlink ref="C114" r:id="rId109" display="Rasta and Kheshtak"/>
+    <hyperlink ref="C115" r:id="rId110" display="Kth smallest number again"/>
+    <hyperlink ref="C116" r:id="rId111" display="Find pivot element in a sorted array"/>
+    <hyperlink ref="C117" r:id="rId112" display="K-th Element of Two Sorted Arrays"/>
+    <hyperlink ref="C118" r:id="rId113" display="Aggressive cows"/>
+    <hyperlink ref="C119" r:id="rId114" display="Book Allocation Problem"/>
+    <hyperlink ref="C120" r:id="rId115" display="EKOSPOJ:"/>
+    <hyperlink ref="C121" r:id="rId116" display="Job Scheduling Algo"/>
+    <hyperlink ref="C122" r:id="rId117" display="Missing Number in AP"/>
+    <hyperlink ref="C123" r:id="rId118" display="Smallest number with atleastn trailing zeroes infactorial"/>
+    <hyperlink ref="C124" r:id="rId119" display="Painters Partition Problem:"/>
+    <hyperlink ref="C125" r:id="rId120" display="ROTI-Prata SPOJ"/>
+    <hyperlink ref="C126" r:id="rId121" display="DoubleHelix SPOJ"/>
+    <hyperlink ref="C127" r:id="rId122" display="Subset Sums"/>
+    <hyperlink ref="C128" r:id="rId123" display="Findthe inversion count"/>
+    <hyperlink ref="C129" r:id="rId124" display="Implement Merge-sort in-place"/>
+    <hyperlink ref="C130" r:id="rId125" display="Partitioning and Sorting Arrays with Many Repeated Entries"/>
+    <hyperlink ref="C131" r:id="rId126" display="Write a Program to reverse the Linked List. (Both Iterative and recursive)"/>
+    <hyperlink ref="C132" r:id="rId127" display="Reverse a Linked List in group of Given Size. [Very Imp]"/>
+    <hyperlink ref="C133" r:id="rId128" display="Write a program to Detect loop in a linked list."/>
+    <hyperlink ref="C134" r:id="rId129" display="Write a program to Delete loop in a linked list."/>
+    <hyperlink ref="C135" r:id="rId130" display="Find the starting point of the loop. "/>
+    <hyperlink ref="C136" r:id="rId131" display="Remove Duplicates in a sorted Linked List."/>
+    <hyperlink ref="C137" r:id="rId132" display="Remove Duplicates in a Un-sorted Linked List."/>
+    <hyperlink ref="C138" r:id="rId133" display="Write a Program to Move the last element to Front in a Linked List."/>
+    <hyperlink ref="C139" r:id="rId134" display="Add “1” to a number represented as a Linked List."/>
+    <hyperlink ref="C140" r:id="rId135" display="Add two numbers represented by linked lists."/>
+    <hyperlink ref="C141" r:id="rId136" display="Intersection of two Sorted Linked List."/>
+    <hyperlink ref="C142" r:id="rId137" display="Intersection Point of two Linked Lists."/>
+    <hyperlink ref="C143" r:id="rId138" display="Merge Sort For Linked lists.[Very Important]"/>
+    <hyperlink ref="C144" r:id="rId139" display="Quicksort for Linked Lists.[Very Important]"/>
+    <hyperlink ref="C145" r:id="rId140" display="Find the middle Element of a linked list."/>
+    <hyperlink ref="C146" r:id="rId141" display="Check if a linked list is a circular linked list."/>
+    <hyperlink ref="C147" r:id="rId142" display="Split a Circular linked list into two halves."/>
+    <hyperlink ref="C148" r:id="rId143" display="Write a Program to check whether the Singly Linked list is a palindrome or not."/>
+    <hyperlink ref="C149" r:id="rId144" display="Deletion from a Circular Linked List."/>
+    <hyperlink ref="C150" r:id="rId145" display="Reverse a Doubly Linked list."/>
+    <hyperlink ref="C151" r:id="rId146" display="Find pairs with a given sum in a DLL."/>
+    <hyperlink ref="C152" r:id="rId147" display="Count triplets in a sorted DLL whose sum is equal to given value “X”."/>
+    <hyperlink ref="C153" r:id="rId148" display="Sort a “k”sorted Doubly Linked list.[Very IMP]"/>
+    <hyperlink ref="C154" r:id="rId149" display="Rotate DoublyLinked list by N nodes."/>
+    <hyperlink ref="C155" r:id="rId150" display="Rotate a Doubly Linked list in group of Given Size.[Very IMP]"/>
+    <hyperlink ref="C158" r:id="rId151" display="Flatten a Linked List"/>
+    <hyperlink ref="C159" r:id="rId152" display="Sort a LL of 0's, 1's and 2's"/>
+    <hyperlink ref="C160" r:id="rId153" display="Clone a linked list with next and random pointer"/>
+    <hyperlink ref="C161" r:id="rId154" display="Merge K sorted Linked list"/>
+    <hyperlink ref="C162" r:id="rId155" display="Multiply 2 no. represented by LL"/>
+    <hyperlink ref="C163" r:id="rId156" display="Delete nodes which have a greater value on right side"/>
+    <hyperlink ref="C164" r:id="rId157" display="Segregate even and odd nodes in a Linked List"/>
+    <hyperlink ref="C165" r:id="rId158" display="Program for n’th node from the end of a Linked List"/>
+    <hyperlink ref="C166" r:id="rId159" display="Find the first non-repeating character from a stream of characters"/>
+    <hyperlink ref="C167" r:id="rId160" display="level order traversal"/>
+    <hyperlink ref="C168" r:id="rId161" display="Reverse Level Order traversal"/>
+    <hyperlink ref="C169" r:id="rId162" display="Height of a tree"/>
+    <hyperlink ref="C170" r:id="rId163" display="Diameter of a tree"/>
+    <hyperlink ref="C171" r:id="rId164" display="Mirror of a tree"/>
+    <hyperlink ref="C172" r:id="rId165" display="Inorder Traversal of a tree both using recursion and Iteration"/>
+    <hyperlink ref="C173" r:id="rId166" display="Preorder Traversal of a tree both using recursion and Iteration"/>
+    <hyperlink ref="C174" r:id="rId167" display="Postorder Traversal of a tree both using recursion and Iteration"/>
+    <hyperlink ref="C175" r:id="rId168" display="Left View of a tree"/>
+    <hyperlink ref="C176" r:id="rId169" display="Right View of Tree"/>
+    <hyperlink ref="C177" r:id="rId170" display="Top View of a tree"/>
+    <hyperlink ref="C178" r:id="rId171" display="Bottom View of a tree"/>
+    <hyperlink ref="C179" r:id="rId172" display="Zig-Zag traversal of a binary tree"/>
+    <hyperlink ref="C180" r:id="rId173" display="Check if a tree is balanced or not"/>
+    <hyperlink ref="C181" r:id="rId174" display="Diagnol Traversal of a Binary tree"/>
+    <hyperlink ref="C182" r:id="rId175" display="Boundary traversal of a Binary tree"/>
+    <hyperlink ref="C183" r:id="rId176" display="Construct Binary Tree from String with Bracket Representation"/>
+    <hyperlink ref="C184" r:id="rId177" display="Convert Binary tree into Doubly Linked List"/>
+    <hyperlink ref="C185" r:id="rId178" display="Convert Binary tree into Sum tree"/>
+    <hyperlink ref="C186" r:id="rId179" display="Construct Binary tree from Inorder and preorder traversal"/>
+    <hyperlink ref="C187" r:id="rId180" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." display="Find minimum swaps required to convert a Binary tree into BST"/>
+    <hyperlink ref="C188" r:id="rId181" display="Check if Binary tree is Sum tree or not"/>
+    <hyperlink ref="C189" r:id="rId182" display="Check if all leaf nodes are at same level or not"/>
+    <hyperlink ref="C190" r:id="rId183" display="Check if a Binary Tree contains duplicate subtrees of size 2 or more [ IMP ]"/>
+    <hyperlink ref="C191" r:id="rId184" display="Check if 2 trees are mirror or not"/>
+    <hyperlink ref="C192" r:id="rId185" display="Sum of Nodes on the Longest path from root to leaf node "/>
+    <hyperlink ref="C193" r:id="rId186" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." display="Check if given graph is tree or not.  [ IMP ]"/>
+    <hyperlink ref="C194" r:id="rId187" display="Find Largest subtree sum in a tree"/>
+    <hyperlink ref="C195" r:id="rId188" display="Maximum Sum of nodes in Binary tree such that no two are adjacent "/>
+    <hyperlink ref="C196" r:id="rId189" display="Print all &quot;K&quot; Sum paths in a Binary tree"/>
+    <hyperlink ref="C197" r:id="rId190" display="Find LCA in a Binary tree"/>
+    <hyperlink ref="C198" r:id="rId191" display="Find distance between 2 nodes in a Binary tree"/>
+    <hyperlink ref="C199" r:id="rId192" display="Kth Ancestor of node in a Binary tree"/>
+    <hyperlink ref="C200" r:id="rId193" display="Find all Duplicate subtrees in a Binary tree [ IMP ]"/>
+    <hyperlink ref="C201" r:id="rId194" display="Tree Isomorphism Problem"/>
+    <hyperlink ref="C202" r:id="rId195" display="Fina a value in a BST"/>
+    <hyperlink ref="C203" r:id="rId196" display="Deletion of a node in a BST"/>
+    <hyperlink ref="C204" r:id="rId197" display="Find min and max value in a BST"/>
+    <hyperlink ref="C205" r:id="rId198" display="Find inorder successor and inorder predecessor in a BST"/>
+    <hyperlink ref="C206" r:id="rId199" display="Check if a tree is a BST or not "/>
+    <hyperlink ref="C207" r:id="rId200" display="Populate Inorder successor of all nodes"/>
+    <hyperlink ref="C208" r:id="rId201" display="Find LCA  of 2 nodes in a BST"/>
+    <hyperlink ref="C209" r:id="rId202" display="Construct BST from preorder traversal"/>
+    <hyperlink ref="C210" r:id="rId203" display="Convert Binary tree into BST"/>
+    <hyperlink ref="C211" r:id="rId204" display="Convert a normal BST into a Balanced BST"/>
+    <hyperlink ref="C212" r:id="rId205" display="Merge two BST [ V.V.V&gt;IMP ]"/>
+    <hyperlink ref="C213" r:id="rId206" display="Find Kth largest element in a BST"/>
+    <hyperlink ref="C214" r:id="rId207" display="Find Kth smallest element in a BST"/>
+    <hyperlink ref="C215" r:id="rId208" display="Count pairs from 2 BST whose sum is equal to given value &quot;X&quot;"/>
+    <hyperlink ref="C216" r:id="rId209" display="Find the median of BST in O(n) time and O(1) space"/>
+    <hyperlink ref="C217" r:id="rId210" display="Count BST ndoes that lie in a given range"/>
+    <hyperlink ref="C218" r:id="rId211" display="Replace every element with the least greater element on its right"/>
+    <hyperlink ref="C219" r:id="rId212" display="Given &quot;n&quot; appointments, find the conflicting appointments"/>
+    <hyperlink ref="C220" r:id="rId213" display="Check preorder is valid or not"/>
+    <hyperlink ref="C221" r:id="rId214" display="Check whether BST contains Dead end"/>
+    <hyperlink ref="C222" r:id="rId215" display="Largest BST in a Binary Tree [ V.V.V.V.V IMP ]"/>
+    <hyperlink ref="C223" r:id="rId216" display="Flatten BST to sorted list"/>
+    <hyperlink ref="C224" r:id="rId217" display="Activity Selection Problem"/>
+    <hyperlink ref="C225" r:id="rId218" display="Job SequencingProblem"/>
+    <hyperlink ref="C226" r:id="rId219" display="Huffman Coding"/>
+    <hyperlink ref="C227" r:id="rId220" display="Water Connection Problem"/>
+    <hyperlink ref="C228" r:id="rId221" display="Fractional Knapsack Problem"/>
+    <hyperlink ref="C229" r:id="rId222" display="Greedy Algorithm to find Minimum number of Coins"/>
+    <hyperlink ref="C230" r:id="rId223" display="Maximum trains for which stoppage can be provided"/>
+    <hyperlink ref="C231" r:id="rId224" display="Minimum Platforms Problem"/>
+    <hyperlink ref="C232" r:id="rId225" display="Buy Maximum Stocks if i stocks can be bought on i-th day"/>
+    <hyperlink ref="C233" r:id="rId226" display="Find the minimum and maximum amount to buy all N candies"/>
+    <hyperlink ref="C234" r:id="rId227" display="Minimize Cash Flow among a given set of friends who have borrowed money from each other"/>
+    <hyperlink ref="C235" r:id="rId228" display="Minimum Cost to cut a board into squares"/>
+    <hyperlink ref="C236" r:id="rId229" display="Check if it is possible to survive on Island"/>
+    <hyperlink ref="C237" r:id="rId230" display="Find maximum meetings in one room"/>
+    <hyperlink ref="C238" r:id="rId231" display="Maximum product subset of an array"/>
+    <hyperlink ref="C239" r:id="rId232" display="Maximize array sum after K negations"/>
+    <hyperlink ref="C240" r:id="rId233" display="Maximize the sum of arr[i]*i"/>
+    <hyperlink ref="C241" r:id="rId234" display="Maximum sum of absolute difference of an array"/>
+    <hyperlink ref="C242" r:id="rId235" display="Maximize sum of consecutive differences in a circular array"/>
+    <hyperlink ref="C243" r:id="rId236" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." display="Minimum sum of absolute difference of pairs of two arrays"/>
+    <hyperlink ref="C244" r:id="rId237" display="Program for Shortest Job First (or SJF) CPU Scheduling"/>
+    <hyperlink ref="C245" r:id="rId238" display="Program for Least Recently Used (LRU) Page Replacement algorithm"/>
+    <hyperlink ref="C246" r:id="rId239" display="Smallest subset with sum greater than all other elements"/>
+    <hyperlink ref="C247" r:id="rId240" display="Chocolate Distribution Problem"/>
+    <hyperlink ref="C248" r:id="rId241" display="DEFKIN -Defense of a Kingdom"/>
+    <hyperlink ref="C249" r:id="rId242" display="DIEHARD -DIE HARD"/>
+    <hyperlink ref="C250" r:id="rId243" display="GERGOVIA -Wine trading in Gergovia"/>
+    <hyperlink ref="C251" r:id="rId244" display="Picking Up Chicks"/>
+    <hyperlink ref="C252" r:id="rId245" display="CHOCOLA –Chocolate"/>
+    <hyperlink ref="C253" r:id="rId246" display="ARRANGE -Arranging Amplifiers"/>
+    <hyperlink ref="C254" r:id="rId247" display="K Centers Problem"/>
+    <hyperlink ref="C255" r:id="rId248" display="Minimum Cost of ropes"/>
+    <hyperlink ref="C256" r:id="rId249" display="Find smallest number with given number of digits and sum of digits"/>
+    <hyperlink ref="C257" r:id="rId250" display="Rearrange characters in a string such that no two adjacent are same"/>
+    <hyperlink ref="C258" r:id="rId251" display="Find maximum sum possible equal sum of three stacks"/>
+    <hyperlink ref="C259" r:id="rId252" display="Rat in a maze Problem"/>
+    <hyperlink ref="C260" r:id="rId253" display="Printing all solutions in N-Queen Problem"/>
+    <hyperlink ref="C261" r:id="rId254" display="Word Break Problem using Backtracking"/>
+    <hyperlink ref="C262" r:id="rId255" display="Remove Invalid Parentheses"/>
+    <hyperlink ref="C263" r:id="rId256" display="Sudoku Solver"/>
+    <hyperlink ref="C264" r:id="rId257" display="m Coloring Problem"/>
+    <hyperlink ref="C265" r:id="rId258" display="Print all palindromic partitions of a string"/>
+    <hyperlink ref="C266" r:id="rId259" display="Subset Sum Problem"/>
+    <hyperlink ref="C267" r:id="rId260" display="The Knight’s tour problem"/>
+    <hyperlink ref="C268" r:id="rId261" display="Tug of War"/>
+    <hyperlink ref="C269" r:id="rId262" display="Find shortest safe route in a path with landmines"/>
+    <hyperlink ref="C270" r:id="rId263" display="Combinational Sum"/>
+    <hyperlink ref="C271" r:id="rId264" display="Find Maximum number possible by doing at-most K swaps"/>
+    <hyperlink ref="C272" r:id="rId265" display="Print all permutations of a string "/>
+    <hyperlink ref="C273" r:id="rId266" display="Find if there is a path of more than k length from a source"/>
+    <hyperlink ref="C274" r:id="rId267" display="Longest Possible Route in a Matrix with Hurdles"/>
+    <hyperlink ref="C275" r:id="rId268" display="Print all possible paths from top left to bottom right of a mXn matrix"/>
+    <hyperlink ref="C276" r:id="rId269" display="Partition of a set intoK subsets with equal sum"/>
+    <hyperlink ref="C277" r:id="rId270" display="Find the K-th Permutation Sequence of first N natural numbers"/>
+    <hyperlink ref="C278" r:id="rId271" display=" Implement Stack from Scratch"/>
+    <hyperlink ref="C279" r:id="rId272" display=" Implement Queue from Scratch"/>
+    <hyperlink ref="C280" r:id="rId273" display="Implement 2 stack in an array"/>
+    <hyperlink ref="C281" r:id="rId274" display="find the middle element of a stack"/>
+    <hyperlink ref="C282" r:id="rId275" display="Implement &quot;N&quot; stacks in an Array"/>
+    <hyperlink ref="C283" r:id="rId276" display="Check the expression has valid or Balanced parenthesis or not."/>
+    <hyperlink ref="C284" r:id="rId277" display="Reverse a String using Stack"/>
+    <hyperlink ref="C285" r:id="rId278" display="Design a Stack that supports getMin() in O(1) time and O(1) extra space."/>
+    <hyperlink ref="C286" r:id="rId279" display="Find the next Greater element"/>
+    <hyperlink ref="C287" r:id="rId280" display="The celebrity Problem"/>
+    <hyperlink ref="C288" r:id="rId281" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." display="Arithmetic Expression evaluation"/>
+    <hyperlink ref="C289" r:id="rId282" display="Evaluation of Postfix expression"/>
+    <hyperlink ref="C290" r:id="rId283" display="Implement a method to insert an element at its bottom without using any other data structure."/>
+    <hyperlink ref="C291" r:id="rId284" display="Reverse a stack using recursion"/>
+    <hyperlink ref="C292" r:id="rId285" display="Sort a Stack using recursion"/>
+    <hyperlink ref="C293" r:id="rId286" display="Merge Overlapping Intervals"/>
+    <hyperlink ref="C294" r:id="rId287" display="Largest rectangular Area in Histogram"/>
+    <hyperlink ref="C295" r:id="rId288" display="Length of the Longest Valid Substring"/>
+    <hyperlink ref="C296" r:id="rId289" display="Expression contains redundant bracket or not"/>
+    <hyperlink ref="C297" r:id="rId290" display="Implement Stack using Queue"/>
+    <hyperlink ref="C298" r:id="rId291" display="Implement Stack using Deque"/>
+    <hyperlink ref="C299" r:id="rId292" display="Stack Permutations (Check if an array is stack permutation of other)"/>
+    <hyperlink ref="C300" r:id="rId293" display="Implement Queue using Stack  "/>
+    <hyperlink ref="C301" r:id="rId294" display="Implement &quot;n&quot; queue in an array"/>
+    <hyperlink ref="C302" r:id="rId295" display="Implement a Circular queue"/>
+    <hyperlink ref="C303" r:id="rId296" display="LRU Cache Implementationa"/>
+    <hyperlink ref="C304" r:id="rId297" display="Reverse a Queue using recursion"/>
+    <hyperlink ref="C305" r:id="rId298" display="Reverse the first “K” elements of a queue"/>
+    <hyperlink ref="C306" r:id="rId299" display="Interleave the first half of the queue with second half"/>
+    <hyperlink ref="C307" r:id="rId300" display="Find the first circular tour that visits all Petrol Pumps"/>
+    <hyperlink ref="C308" r:id="rId301" display="Minimum time required to rot all oranges"/>
+    <hyperlink ref="C309" r:id="rId302" display="Distance of nearest cell having 1 in a binary matrix"/>
+    <hyperlink ref="C310" r:id="rId303" display="First negative integer in every window of size “k”"/>
+    <hyperlink ref="C311" r:id="rId304" display="Check if all levels of two trees are anagrams or not."/>
+    <hyperlink ref="C312" r:id="rId305" display="Sum of minimum and maximum elements of all subarrays of size “k”."/>
+    <hyperlink ref="C313" r:id="rId306" display="Minimum sum of squares of character counts in a given string after removing “k” characters."/>
+    <hyperlink ref="C314" r:id="rId307" display="Queue based approach or first non-repeating character in a stream."/>
+    <hyperlink ref="C315" r:id="rId308" display="Next Smaller Element"/>
+    <hyperlink ref="C316" r:id="rId309" display="Implement a Maxheap/MinHeap using arrays and recursion."/>
+    <hyperlink ref="C317" r:id="rId310" display="Sort an Array using heap. (HeapSort)"/>
+    <hyperlink ref="C318" r:id="rId311" display="Maximum of all subarrays of size k."/>
+    <hyperlink ref="C319" r:id="rId312" display="“k” largest element in an array"/>
+    <hyperlink ref="C320" r:id="rId313" display="Kth smallest and largest element in an unsorted array"/>
+    <hyperlink ref="C321" r:id="rId314" display="Merge “K” sorted arrays. [ IMP ]"/>
+    <hyperlink ref="C322" r:id="rId315" display="Merge 2 Binary Max Heaps"/>
+    <hyperlink ref="C323" r:id="rId316" display="Kth largest sum continuous subarrays"/>
+    <hyperlink ref="C324" r:id="rId317" display="Leetcode- reorganize strings"/>
+    <hyperlink ref="C325" r:id="rId318" display="Merge “K” Sorted Linked Lists [V.IMP]"/>
+    <hyperlink ref="C326" r:id="rId319" display="Smallest range in “K” Lists"/>
+    <hyperlink ref="C327" r:id="rId320" display="Median in a stream of Integers"/>
+    <hyperlink ref="C328" r:id="rId321" display="Check if a Binary Tree is Heap"/>
+    <hyperlink ref="C329" r:id="rId322" display="Connect “n” ropes with minimum cost"/>
+    <hyperlink ref="C330" r:id="rId323" display="Convert BST to Min Heap"/>
+    <hyperlink ref="C331" r:id="rId324" display="Convert min heap to max heap"/>
+    <hyperlink ref="C332" r:id="rId325" display="Rearrange characters in a string such that no two adjacent are same."/>
+    <hyperlink ref="C333" r:id="rId326" display="Minimum sum of two numbers formed from digits of an array"/>
+    <hyperlink ref="C334" r:id="rId327" display="Create a Graph, print it"/>
+    <hyperlink ref="C335" r:id="rId328" display="Implement BFS algorithm "/>
+    <hyperlink ref="C336" r:id="rId329" display="Implement DFS Algo "/>
+    <hyperlink ref="C337" r:id="rId330" display="Detect Cycle in Directed Graph using BFS/DFS Algo "/>
+    <hyperlink ref="C338" r:id="rId331" display="Detect Cycle in UnDirected Graph using BFS/DFS Algo "/>
+    <hyperlink ref="C339" r:id="rId332" display="Search in a Maze"/>
+    <hyperlink ref="C340" r:id="rId333" display="Minimum Step by Knight"/>
+    <hyperlink ref="C341" r:id="rId334" display="flood fill algo"/>
+    <hyperlink ref="C342" r:id="rId335" display="Clone a graph"/>
+    <hyperlink ref="C343" r:id="rId336" display="Making wired Connections"/>
+    <hyperlink ref="C344" r:id="rId337" display="word Ladder "/>
+    <hyperlink ref="C345" r:id="rId338" display="Dijkstra algo"/>
+    <hyperlink ref="C346" r:id="rId339" display="Implement Topological Sort "/>
+    <hyperlink ref="C347" r:id="rId340" display="Minimum time taken by each job to be completed given by a Directed Acyclic Graph"/>
+    <hyperlink ref="C348" r:id="rId341" display="Find whether it is possible to finish all tasks or not from given dependencies"/>
+    <hyperlink ref="C349" r:id="rId342" display="Find the no. of Isalnds"/>
+    <hyperlink ref="C350" r:id="rId343" display="Given a sorted Dictionary of an Alien Language, find order of characters"/>
+    <hyperlink ref="C351" r:id="rId344" display="Implement Kruksal’sAlgorithm"/>
+    <hyperlink ref="C352" r:id="rId345" display="Implement Prim’s Algorithm"/>
+    <hyperlink ref="C353" r:id="rId346" display="Total no. of Spanning tree in a graph"/>
+    <hyperlink ref="C354" r:id="rId347" display="Implement Bellman Ford Algorithm"/>
+    <hyperlink ref="C355" r:id="rId348" display="Implement Floyd warshallAlgorithm"/>
+    <hyperlink ref="C356" r:id="rId349" display="Travelling Salesman Problem"/>
+    <hyperlink ref="C357" r:id="rId350" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." display="Graph ColouringProblem"/>
+    <hyperlink ref="C358" r:id="rId351" display="Snake and Ladders Problem"/>
+    <hyperlink ref="C359" r:id="rId352" display="Find bridge in a graph"/>
+    <hyperlink ref="C360" r:id="rId353" display="Count Strongly connected Components(Kosaraju Algo)"/>
+    <hyperlink ref="C361" r:id="rId354" display="Check whether a graph is Bipartite or Not"/>
+    <hyperlink ref="C362" r:id="rId355" display="Detect Negative cycle in a graph"/>
+    <hyperlink ref="C363" r:id="rId356" display="Longest path in a Directed Acyclic Graph"/>
+    <hyperlink ref="C364" r:id="rId357" display="Journey to the Moon"/>
+    <hyperlink ref="C365" r:id="rId358" display="Cheapest Flights Within K Stops"/>
+    <hyperlink ref="C366" r:id="rId359" display="Oliver and the Game"/>
+    <hyperlink ref="C367" r:id="rId360" display="Water Jug problem using BFS"/>
+    <hyperlink ref="C368" r:id="rId361" display="Water Jug problem using BFS"/>
+    <hyperlink ref="C369" r:id="rId362" display="Find if there is a path of more thank length from a source"/>
+    <hyperlink ref="C370" r:id="rId363" display="M-ColouringProblem"/>
+    <hyperlink ref="C371" r:id="rId364" display="Minimum edges to reverse o make path from source to destination"/>
+    <hyperlink ref="C372" r:id="rId365" display="Paths to travel each nodes using each edge(Seven Bridges)"/>
+    <hyperlink ref="C373" r:id="rId366" display="Vertex Cover Problem"/>
+    <hyperlink ref="C374" r:id="rId367" display="Chinese Postman or Route Inspection"/>
+    <hyperlink ref="C375" r:id="rId368" display="Number of Triangles in a Directed and Undirected Graph"/>
+    <hyperlink ref="C376" r:id="rId369" display="Minimise the cashflow among a given set of friends who have borrowed money from each other"/>
+    <hyperlink ref="C377" r:id="rId370" display="Two Clique Problem"/>
+    <hyperlink ref="C378" r:id="rId371" display="Construct a trie from scratch"/>
+    <hyperlink ref="C379" r:id="rId372" display="Find shortest unique prefix for every word in a given list"/>
+    <hyperlink ref="C380" r:id="rId373" display="Word Break Problem | (Trie solution)"/>
+    <hyperlink ref="C381" r:id="rId374" display="Given a sequence of words, print all anagrams together"/>
+    <hyperlink ref="C382" r:id="rId375" display="Implement a Phone Directory"/>
+    <hyperlink ref="C383" r:id="rId376" display="Print unique rows in a given boolean matrix"/>
+    <hyperlink ref="C384" r:id="rId377" display="Coin ChangeProblem"/>
+    <hyperlink ref="C385" r:id="rId378" display="Knapsack Problem"/>
+    <hyperlink ref="C386" r:id="rId379" display="Binomial CoefficientProblem"/>
+    <hyperlink ref="C387" r:id="rId380" display="Permutation CoefficientProblem"/>
+    <hyperlink ref="C388" r:id="rId381" display="Program for nth Catalan Number"/>
+    <hyperlink ref="C389" r:id="rId382" display="Matrix Chain Multiplication "/>
+    <hyperlink ref="C390" r:id="rId383" display="Edit Distance"/>
+    <hyperlink ref="C391" r:id="rId384" display="Subset Sum Problem"/>
+    <hyperlink ref="C392" r:id="rId385" display="Friends Pairing Problem"/>
+    <hyperlink ref="C393" r:id="rId386" display="Gold Mine Problem"/>
+    <hyperlink ref="C394" r:id="rId387" display="Assembly Line SchedulingProblem"/>
+    <hyperlink ref="C395" r:id="rId388" display="Painting the Fenceproblem"/>
+    <hyperlink ref="C396" r:id="rId389" display="Maximize The Cut Segments"/>
+    <hyperlink ref="C397" r:id="rId390" display="Longest Common Subsequence"/>
+    <hyperlink ref="C398" r:id="rId391" display="Longest Repeated Subsequence"/>
+    <hyperlink ref="C399" r:id="rId392" display="Longest Increasing Subsequence"/>
+    <hyperlink ref="C400" r:id="rId393" display="Space Optimized Solution of LCS"/>
+    <hyperlink ref="C401" r:id="rId394" display="LCS (Longest Common Subsequence) of three strings"/>
+    <hyperlink ref="C402" r:id="rId395" display="Maximum Sum Increasing Subsequence"/>
+    <hyperlink ref="C403" r:id="rId396" display="Count all subsequences having product less than K"/>
+    <hyperlink ref="C404" r:id="rId397" display="Longest subsequence such that difference between adjacent is one"/>
+    <hyperlink ref="C405" r:id="rId398" display="Maximum subsequence sum such that no three are consecutive"/>
+    <hyperlink ref="C406" r:id="rId399" display="Egg Dropping Problem"/>
+    <hyperlink ref="C407" r:id="rId400" display="Maximum Length Chain of Pairs"/>
+    <hyperlink ref="C408" r:id="rId401" display="Maximum size square sub-matrix with all 1s"/>
+    <hyperlink ref="C409" r:id="rId402" display="Maximum sum of pairs with specific difference"/>
+    <hyperlink ref="C410" r:id="rId403" display="Min Cost PathProblem"/>
+    <hyperlink ref="C411" r:id="rId404" display="Maximum difference of zeros and ones in binary string"/>
+    <hyperlink ref="C412" r:id="rId405" display="Minimum number of jumps to reach end"/>
+    <hyperlink ref="C413" r:id="rId406" display="Minimum cost to fill given weight in a bag"/>
+    <hyperlink ref="C414" r:id="rId407" display="Minimum removals from array to make max –min &lt;= K"/>
+    <hyperlink ref="C415" r:id="rId408" display="Longest Common Substring"/>
+    <hyperlink ref="C416" r:id="rId409" display="Count number of ways to reacha given score in a game"/>
+    <hyperlink ref="C417" r:id="rId410" display="Count Balanced Binary Trees of Height h"/>
+    <hyperlink ref="C418" r:id="rId411" display="LargestSum Contiguous Subarray [V&gt;V&gt;V&gt;V IMP ]"/>
+    <hyperlink ref="C419" r:id="rId412" display="Smallest sum contiguous subarray"/>
+    <hyperlink ref="C420" r:id="rId413" display="Unbounded Knapsack (Repetition of items allowed)"/>
+    <hyperlink ref="C421" r:id="rId414" display="Word Break Problem"/>
+    <hyperlink ref="C422" r:id="rId415" display="Largest Independent Set Problem"/>
+    <hyperlink ref="C423" r:id="rId416" display="Partition problem"/>
+    <hyperlink ref="C424" r:id="rId417" display="Longest Palindromic Subsequence"/>
+    <hyperlink ref="C425" r:id="rId418" display="Count All Palindromic Subsequence in a given String"/>
+    <hyperlink ref="C426" r:id="rId419" display="Longest Palindromic Substring"/>
+    <hyperlink ref="C427" r:id="rId420" display="Longest alternating subsequence"/>
+    <hyperlink ref="C428" r:id="rId421" display="Weighted Job Scheduling"/>
+    <hyperlink ref="C429" r:id="rId422" display="Coin game winner where every player has three choices"/>
+    <hyperlink ref="C430" r:id="rId423" display="Count Derangements (Permutation such that no element appears in its original position) [ IMPORTANT ]"/>
+    <hyperlink ref="C431" r:id="rId424" display="Maximum profit by buying and selling a share at most twice [ IMP ]"/>
+    <hyperlink ref="C432" r:id="rId425" display="Optimal Strategy for a Game"/>
+    <hyperlink ref="C433" r:id="rId426" display="Optimal Binary Search Tree"/>
+    <hyperlink ref="C434" r:id="rId427" display="Palindrome PartitioningProblem"/>
+    <hyperlink ref="C435" r:id="rId428" display="Word Wrap Problem"/>
+    <hyperlink ref="C436" r:id="rId429" display="Mobile Numeric Keypad Problem [ IMP ]"/>
+    <hyperlink ref="C437" r:id="rId430" display="Boolean Parenthesization Problem"/>
+    <hyperlink ref="C438" r:id="rId431" display="Largest rectangular sub-matrix whose sum is 0"/>
+    <hyperlink ref="C439" r:id="rId432" display="Largest area rectangular sub-matrix with equal number of 1’s and 0’s [ IMP ]"/>
+    <hyperlink ref="C440" r:id="rId433" display="Maximum sum rectangle in a 2D matrix"/>
+    <hyperlink ref="C441" r:id="rId434" display="Maximum profit by buying and selling a share at most k times"/>
+    <hyperlink ref="C442" r:id="rId435" display="Find if a string is interleaved of two other strings"/>
+    <hyperlink ref="C443" r:id="rId436" display="Maximum Length of Pair Chain"/>
+    <hyperlink ref="C444" r:id="rId437" display="Count set bits in an integer"/>
+    <hyperlink ref="C445" r:id="rId438" display="Find the two non-repeating elements in an array of repeating elements"/>
+    <hyperlink ref="C446" r:id="rId439" display="Count number of bits to be flipped to convert A to B"/>
+    <hyperlink ref="C447" r:id="rId440" display="Count total set bits in all numbers from 1 to n"/>
+    <hyperlink ref="C448" r:id="rId441" display="Program to find whether a no is power of two"/>
+    <hyperlink ref="C449" r:id="rId442" display="Find position of the only set bit"/>
+    <hyperlink ref="C450" r:id="rId443" display="Copy set bits in a range"/>
+    <hyperlink ref="C451" r:id="rId444" display="Divide two integers without using multiplication, division and mod operator"/>
+    <hyperlink ref="C452" r:id="rId445" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." display="Calculate square of a number without using *, / and pow()"/>
+    <hyperlink ref="C453" r:id="rId446" display="Power Set"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
fixed links and question typos
</commit_message>
<xml_diff>
--- a/DSA_450_LoveBabbar.xlsx
+++ b/DSA_450_LoveBabbar.xlsx
@@ -1836,11 +1836,11 @@
   </sheetPr>
   <dimension ref="A1:D467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.24"/>

</xml_diff>

<commit_message>
done Q47 reverse a string(using java for practice)
</commit_message>
<xml_diff>
--- a/DSA_450_LoveBabbar.xlsx
+++ b/DSA_450_LoveBabbar.xlsx
@@ -1839,11 +1839,11 @@
   </sheetPr>
   <dimension ref="A1:D467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.24"/>
@@ -2490,7 +2490,7 @@
       <c r="B52" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C52" s="20" t="s">
+      <c r="C52" s="13" t="s">
         <v>57</v>
       </c>
       <c r="D52" s="12"/>

</xml_diff>

<commit_message>
done Q57 print all permutations of a string
</commit_message>
<xml_diff>
--- a/DSA_450_LoveBabbar.xlsx
+++ b/DSA_450_LoveBabbar.xlsx
@@ -1860,11 +1860,11 @@
   </sheetPr>
   <dimension ref="A1:D467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D59" activeCellId="0" sqref="D59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C62" activeCellId="0" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.24"/>
@@ -2606,7 +2606,7 @@
       <c r="B59" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="22" t="s">
+      <c r="C59" s="11" t="s">
         <v>66</v>
       </c>
       <c r="D59" s="12"/>
@@ -2619,7 +2619,7 @@
       <c r="B60" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C60" s="22" t="s">
+      <c r="C60" s="11" t="s">
         <v>67</v>
       </c>
       <c r="D60" s="12"/>
@@ -2632,7 +2632,7 @@
       <c r="B61" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C61" s="22" t="s">
+      <c r="C61" s="13" t="s">
         <v>68</v>
       </c>
       <c r="D61" s="12"/>

</xml_diff>

<commit_message>
done Q60 min operations to convert a str1 to str2
</commit_message>
<xml_diff>
--- a/DSA_450_LoveBabbar.xlsx
+++ b/DSA_450_LoveBabbar.xlsx
@@ -287,7 +287,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">)</t>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF81D41A"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">However I will try the DP solution too</t>
     </r>
   </si>
   <si>
@@ -1489,7 +1499,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1601,6 +1611,13 @@
       <vertAlign val="superscript"/>
       <sz val="12"/>
       <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF81D41A"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1905,11 +1922,11 @@
   </sheetPr>
   <dimension ref="A1:D467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D63" activeCellId="0" sqref="D63"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C65" activeCellId="0" sqref="C65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.24"/>
@@ -2731,7 +2748,7 @@
       <c r="B65" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C65" s="23" t="s">
+      <c r="C65" s="11" t="s">
         <v>73</v>
       </c>
       <c r="D65" s="12"/>

</xml_diff>

<commit_message>
done Q62 balanced parantheses problem
</commit_message>
<xml_diff>
--- a/DSA_450_LoveBabbar.xlsx
+++ b/DSA_450_LoveBabbar.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="471">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t xml:space="preserve">Find next greater number with same set of digits. [Very Very IMP]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Repeated] - Array Q15</t>
   </si>
   <si>
     <t xml:space="preserve">Balanced Parenthesis problem.[Imp]</t>
@@ -1922,11 +1925,11 @@
   </sheetPr>
   <dimension ref="A1:D467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C65" activeCellId="0" sqref="C65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E66" activeCellId="0" sqref="E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.74609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.24"/>
@@ -2151,7 +2154,7 @@
       <c r="B20" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="11" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="12"/>
@@ -2748,7 +2751,7 @@
       <c r="B65" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="19" t="s">
         <v>73</v>
       </c>
       <c r="D65" s="12"/>
@@ -2764,7 +2767,9 @@
       <c r="C66" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="D66" s="12"/>
+      <c r="D66" s="12" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="n">
@@ -2774,8 +2779,8 @@
       <c r="B67" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C67" s="23" t="s">
-        <v>75</v>
+      <c r="C67" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="D67" s="12"/>
     </row>
@@ -2788,7 +2793,7 @@
         <v>56</v>
       </c>
       <c r="C68" s="23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D68" s="12"/>
     </row>
@@ -2801,7 +2806,7 @@
         <v>56</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D69" s="12"/>
     </row>
@@ -2814,7 +2819,7 @@
         <v>56</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D70" s="12"/>
     </row>
@@ -2827,7 +2832,7 @@
         <v>56</v>
       </c>
       <c r="C71" s="23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D71" s="12"/>
     </row>
@@ -2840,7 +2845,7 @@
         <v>56</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D72" s="12"/>
     </row>
@@ -2853,7 +2858,7 @@
         <v>56</v>
       </c>
       <c r="C73" s="23" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D73" s="12"/>
     </row>
@@ -2866,7 +2871,7 @@
         <v>56</v>
       </c>
       <c r="C74" s="23" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D74" s="12"/>
     </row>
@@ -2879,7 +2884,7 @@
         <v>56</v>
       </c>
       <c r="C75" s="23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D75" s="12"/>
     </row>
@@ -2892,7 +2897,7 @@
         <v>56</v>
       </c>
       <c r="C76" s="23" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D76" s="12"/>
     </row>
@@ -2905,7 +2910,7 @@
         <v>56</v>
       </c>
       <c r="C77" s="23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D77" s="12"/>
     </row>
@@ -2918,7 +2923,7 @@
         <v>56</v>
       </c>
       <c r="C78" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D78" s="12"/>
     </row>
@@ -2931,7 +2936,7 @@
         <v>56</v>
       </c>
       <c r="C79" s="23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D79" s="12"/>
     </row>
@@ -2944,7 +2949,7 @@
         <v>56</v>
       </c>
       <c r="C80" s="23" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D80" s="12"/>
     </row>
@@ -2957,7 +2962,7 @@
         <v>56</v>
       </c>
       <c r="C81" s="23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D81" s="12"/>
     </row>
@@ -2970,7 +2975,7 @@
         <v>56</v>
       </c>
       <c r="C82" s="23" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D82" s="12"/>
     </row>
@@ -2983,7 +2988,7 @@
         <v>56</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D83" s="12"/>
     </row>
@@ -2996,7 +3001,7 @@
         <v>56</v>
       </c>
       <c r="C84" s="23" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D84" s="12"/>
     </row>
@@ -3009,7 +3014,7 @@
         <v>56</v>
       </c>
       <c r="C85" s="23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D85" s="12"/>
     </row>
@@ -3022,7 +3027,7 @@
         <v>56</v>
       </c>
       <c r="C86" s="23" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D86" s="12"/>
     </row>
@@ -3035,7 +3040,7 @@
         <v>56</v>
       </c>
       <c r="C87" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D87" s="12"/>
     </row>
@@ -3048,7 +3053,7 @@
         <v>56</v>
       </c>
       <c r="C88" s="23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D88" s="12"/>
     </row>
@@ -3061,7 +3066,7 @@
         <v>56</v>
       </c>
       <c r="C89" s="23" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D89" s="12"/>
     </row>
@@ -3074,7 +3079,7 @@
         <v>56</v>
       </c>
       <c r="C90" s="23" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D90" s="12"/>
     </row>
@@ -3087,7 +3092,7 @@
         <v>56</v>
       </c>
       <c r="C91" s="23" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D91" s="12"/>
     </row>
@@ -3100,7 +3105,7 @@
         <v>56</v>
       </c>
       <c r="C92" s="23" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D92" s="12"/>
     </row>
@@ -3113,7 +3118,7 @@
         <v>56</v>
       </c>
       <c r="C93" s="23" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D93" s="12"/>
     </row>
@@ -3126,7 +3131,7 @@
         <v>56</v>
       </c>
       <c r="C94" s="23" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D94" s="12"/>
     </row>
@@ -3136,10 +3141,10 @@
         <v>90</v>
       </c>
       <c r="B95" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C95" s="23" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D95" s="12"/>
     </row>
@@ -3149,10 +3154,10 @@
         <v>91</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C96" s="23" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D96" s="12"/>
     </row>
@@ -3162,10 +3167,10 @@
         <v>92</v>
       </c>
       <c r="B97" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C97" s="23" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D97" s="12"/>
     </row>
@@ -3175,10 +3180,10 @@
         <v>93</v>
       </c>
       <c r="B98" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C98" s="23" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D98" s="12"/>
     </row>
@@ -3188,10 +3193,10 @@
         <v>94</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C99" s="23" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D99" s="12"/>
     </row>
@@ -3201,10 +3206,10 @@
         <v>95</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C100" s="23" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D100" s="12"/>
     </row>
@@ -3214,10 +3219,10 @@
         <v>96</v>
       </c>
       <c r="B101" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C101" s="23" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D101" s="12"/>
     </row>
@@ -3227,10 +3232,10 @@
         <v>97</v>
       </c>
       <c r="B102" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C102" s="23" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D102" s="12"/>
     </row>
@@ -3240,10 +3245,10 @@
         <v>98</v>
       </c>
       <c r="B103" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C103" s="23" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D103" s="12"/>
     </row>
@@ -3253,10 +3258,10 @@
         <v>99</v>
       </c>
       <c r="B104" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C104" s="23" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D104" s="12"/>
     </row>
@@ -3266,10 +3271,10 @@
         <v>100</v>
       </c>
       <c r="B105" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C105" s="23" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D105" s="12"/>
     </row>
@@ -3279,10 +3284,10 @@
         <v>101</v>
       </c>
       <c r="B106" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C106" s="23" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D106" s="12"/>
     </row>
@@ -3292,10 +3297,10 @@
         <v>102</v>
       </c>
       <c r="B107" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C107" s="23" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D107" s="12"/>
     </row>
@@ -3305,10 +3310,10 @@
         <v>103</v>
       </c>
       <c r="B108" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C108" s="23" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D108" s="12"/>
     </row>
@@ -3318,10 +3323,10 @@
         <v>104</v>
       </c>
       <c r="B109" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C109" s="23" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D109" s="12"/>
     </row>
@@ -3331,10 +3336,10 @@
         <v>105</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C110" s="23" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D110" s="12"/>
     </row>
@@ -3344,10 +3349,10 @@
         <v>106</v>
       </c>
       <c r="B111" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C111" s="23" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D111" s="12"/>
     </row>
@@ -3357,10 +3362,10 @@
         <v>107</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C112" s="23" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D112" s="12"/>
     </row>
@@ -3370,10 +3375,10 @@
         <v>108</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C113" s="23" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D113" s="12"/>
     </row>
@@ -3383,10 +3388,10 @@
         <v>109</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C114" s="23" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D114" s="12"/>
     </row>
@@ -3396,10 +3401,10 @@
         <v>110</v>
       </c>
       <c r="B115" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C115" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D115" s="12"/>
     </row>
@@ -3409,10 +3414,10 @@
         <v>111</v>
       </c>
       <c r="B116" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C116" s="23" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D116" s="12"/>
     </row>
@@ -3422,10 +3427,10 @@
         <v>112</v>
       </c>
       <c r="B117" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C117" s="23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D117" s="12"/>
     </row>
@@ -3435,10 +3440,10 @@
         <v>113</v>
       </c>
       <c r="B118" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C118" s="23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D118" s="12"/>
     </row>
@@ -3448,10 +3453,10 @@
         <v>114</v>
       </c>
       <c r="B119" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C119" s="23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D119" s="12"/>
     </row>
@@ -3461,10 +3466,10 @@
         <v>115</v>
       </c>
       <c r="B120" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C120" s="23" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D120" s="12"/>
     </row>
@@ -3474,10 +3479,10 @@
         <v>116</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C121" s="23" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D121" s="12"/>
     </row>
@@ -3487,10 +3492,10 @@
         <v>117</v>
       </c>
       <c r="B122" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C122" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D122" s="12"/>
     </row>
@@ -3500,10 +3505,10 @@
         <v>118</v>
       </c>
       <c r="B123" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C123" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D123" s="12"/>
     </row>
@@ -3513,10 +3518,10 @@
         <v>119</v>
       </c>
       <c r="B124" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C124" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D124" s="12"/>
     </row>
@@ -3526,10 +3531,10 @@
         <v>120</v>
       </c>
       <c r="B125" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C125" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D125" s="12"/>
     </row>
@@ -3539,10 +3544,10 @@
         <v>121</v>
       </c>
       <c r="B126" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C126" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D126" s="12"/>
     </row>
@@ -3552,10 +3557,10 @@
         <v>122</v>
       </c>
       <c r="B127" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C127" s="23" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D127" s="12"/>
     </row>
@@ -3565,10 +3570,10 @@
         <v>123</v>
       </c>
       <c r="B128" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C128" s="23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D128" s="12"/>
     </row>
@@ -3578,10 +3583,10 @@
         <v>124</v>
       </c>
       <c r="B129" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C129" s="23" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D129" s="12"/>
     </row>
@@ -3591,10 +3596,10 @@
         <v>125</v>
       </c>
       <c r="B130" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C130" s="23" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D130" s="12"/>
     </row>
@@ -3604,10 +3609,10 @@
         <v>126</v>
       </c>
       <c r="B131" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C131" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D131" s="12"/>
     </row>
@@ -3617,10 +3622,10 @@
         <v>127</v>
       </c>
       <c r="B132" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C132" s="23" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D132" s="12"/>
     </row>
@@ -3630,10 +3635,10 @@
         <v>128</v>
       </c>
       <c r="B133" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C133" s="23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D133" s="12"/>
     </row>
@@ -3643,10 +3648,10 @@
         <v>129</v>
       </c>
       <c r="B134" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C134" s="23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D134" s="12"/>
     </row>
@@ -3656,10 +3661,10 @@
         <v>130</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C135" s="23" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D135" s="12"/>
     </row>
@@ -3669,10 +3674,10 @@
         <v>131</v>
       </c>
       <c r="B136" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C136" s="23" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D136" s="12"/>
     </row>
@@ -3682,10 +3687,10 @@
         <v>132</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C137" s="23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D137" s="12"/>
     </row>
@@ -3695,10 +3700,10 @@
         <v>133</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C138" s="23" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D138" s="12"/>
     </row>
@@ -3708,10 +3713,10 @@
         <v>134</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C139" s="23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D139" s="12"/>
     </row>
@@ -3721,10 +3726,10 @@
         <v>135</v>
       </c>
       <c r="B140" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C140" s="23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D140" s="12"/>
     </row>
@@ -3734,10 +3739,10 @@
         <v>136</v>
       </c>
       <c r="B141" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C141" s="23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D141" s="12"/>
     </row>
@@ -3747,10 +3752,10 @@
         <v>137</v>
       </c>
       <c r="B142" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C142" s="23" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D142" s="12"/>
     </row>
@@ -3760,10 +3765,10 @@
         <v>138</v>
       </c>
       <c r="B143" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C143" s="23" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D143" s="12"/>
     </row>
@@ -3773,10 +3778,10 @@
         <v>139</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C144" s="23" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D144" s="12"/>
     </row>
@@ -3786,10 +3791,10 @@
         <v>140</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C145" s="23" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D145" s="12"/>
     </row>
@@ -3799,10 +3804,10 @@
         <v>141</v>
       </c>
       <c r="B146" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C146" s="23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D146" s="12"/>
     </row>
@@ -3812,10 +3817,10 @@
         <v>142</v>
       </c>
       <c r="B147" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C147" s="23" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D147" s="12"/>
     </row>
@@ -3825,10 +3830,10 @@
         <v>143</v>
       </c>
       <c r="B148" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C148" s="23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D148" s="12"/>
     </row>
@@ -3838,10 +3843,10 @@
         <v>144</v>
       </c>
       <c r="B149" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C149" s="23" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D149" s="12"/>
     </row>
@@ -3851,10 +3856,10 @@
         <v>145</v>
       </c>
       <c r="B150" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C150" s="23" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D150" s="12"/>
     </row>
@@ -3864,10 +3869,10 @@
         <v>146</v>
       </c>
       <c r="B151" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C151" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D151" s="12"/>
     </row>
@@ -3877,10 +3882,10 @@
         <v>147</v>
       </c>
       <c r="B152" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C152" s="23" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D152" s="12"/>
     </row>
@@ -3890,10 +3895,10 @@
         <v>148</v>
       </c>
       <c r="B153" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C153" s="23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D153" s="12"/>
     </row>
@@ -3903,10 +3908,10 @@
         <v>149</v>
       </c>
       <c r="B154" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C154" s="23" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D154" s="12"/>
     </row>
@@ -3916,10 +3921,10 @@
         <v>150</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C155" s="23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D155" s="12"/>
     </row>
@@ -3929,10 +3934,10 @@
         <v>151</v>
       </c>
       <c r="B156" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C156" s="24" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D156" s="12"/>
     </row>
@@ -3942,10 +3947,10 @@
         <v>152</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C157" s="24" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D157" s="12"/>
     </row>
@@ -3955,10 +3960,10 @@
         <v>153</v>
       </c>
       <c r="B158" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C158" s="23" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D158" s="12"/>
     </row>
@@ -3968,10 +3973,10 @@
         <v>154</v>
       </c>
       <c r="B159" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C159" s="23" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D159" s="12"/>
     </row>
@@ -3981,10 +3986,10 @@
         <v>155</v>
       </c>
       <c r="B160" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C160" s="23" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D160" s="12"/>
     </row>
@@ -3994,10 +3999,10 @@
         <v>156</v>
       </c>
       <c r="B161" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C161" s="23" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D161" s="12"/>
     </row>
@@ -4007,10 +4012,10 @@
         <v>157</v>
       </c>
       <c r="B162" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C162" s="23" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D162" s="12"/>
     </row>
@@ -4020,10 +4025,10 @@
         <v>158</v>
       </c>
       <c r="B163" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C163" s="23" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D163" s="12"/>
     </row>
@@ -4033,10 +4038,10 @@
         <v>159</v>
       </c>
       <c r="B164" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C164" s="23" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D164" s="12"/>
     </row>
@@ -4046,10 +4051,10 @@
         <v>160</v>
       </c>
       <c r="B165" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C165" s="23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D165" s="12"/>
     </row>
@@ -4059,10 +4064,10 @@
         <v>161</v>
       </c>
       <c r="B166" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C166" s="23" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D166" s="12"/>
     </row>
@@ -4072,10 +4077,10 @@
         <v>162</v>
       </c>
       <c r="B167" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C167" s="23" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D167" s="12"/>
     </row>
@@ -4085,10 +4090,10 @@
         <v>163</v>
       </c>
       <c r="B168" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C168" s="23" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D168" s="12"/>
     </row>
@@ -4098,10 +4103,10 @@
         <v>164</v>
       </c>
       <c r="B169" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C169" s="23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D169" s="12"/>
     </row>
@@ -4111,10 +4116,10 @@
         <v>165</v>
       </c>
       <c r="B170" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C170" s="23" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D170" s="12"/>
     </row>
@@ -4124,10 +4129,10 @@
         <v>166</v>
       </c>
       <c r="B171" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C171" s="23" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D171" s="12"/>
     </row>
@@ -4137,10 +4142,10 @@
         <v>167</v>
       </c>
       <c r="B172" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C172" s="23" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D172" s="12"/>
     </row>
@@ -4150,10 +4155,10 @@
         <v>168</v>
       </c>
       <c r="B173" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C173" s="23" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D173" s="12"/>
     </row>
@@ -4163,10 +4168,10 @@
         <v>169</v>
       </c>
       <c r="B174" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C174" s="23" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D174" s="12"/>
     </row>
@@ -4176,10 +4181,10 @@
         <v>170</v>
       </c>
       <c r="B175" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C175" s="23" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D175" s="12"/>
     </row>
@@ -4189,10 +4194,10 @@
         <v>171</v>
       </c>
       <c r="B176" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C176" s="23" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D176" s="12"/>
     </row>
@@ -4202,10 +4207,10 @@
         <v>172</v>
       </c>
       <c r="B177" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C177" s="23" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D177" s="12"/>
     </row>
@@ -4215,10 +4220,10 @@
         <v>173</v>
       </c>
       <c r="B178" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C178" s="23" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D178" s="12"/>
     </row>
@@ -4228,10 +4233,10 @@
         <v>174</v>
       </c>
       <c r="B179" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C179" s="23" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D179" s="12"/>
     </row>
@@ -4241,10 +4246,10 @@
         <v>175</v>
       </c>
       <c r="B180" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C180" s="23" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D180" s="12"/>
     </row>
@@ -4254,10 +4259,10 @@
         <v>176</v>
       </c>
       <c r="B181" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C181" s="23" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D181" s="12"/>
     </row>
@@ -4267,10 +4272,10 @@
         <v>177</v>
       </c>
       <c r="B182" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C182" s="23" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D182" s="12"/>
     </row>
@@ -4280,10 +4285,10 @@
         <v>178</v>
       </c>
       <c r="B183" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C183" s="23" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D183" s="12"/>
     </row>
@@ -4293,10 +4298,10 @@
         <v>179</v>
       </c>
       <c r="B184" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C184" s="23" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D184" s="12"/>
     </row>
@@ -4306,10 +4311,10 @@
         <v>180</v>
       </c>
       <c r="B185" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C185" s="23" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D185" s="12"/>
     </row>
@@ -4319,10 +4324,10 @@
         <v>181</v>
       </c>
       <c r="B186" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C186" s="23" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D186" s="12"/>
     </row>
@@ -4332,10 +4337,10 @@
         <v>182</v>
       </c>
       <c r="B187" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C187" s="23" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D187" s="12"/>
     </row>
@@ -4345,10 +4350,10 @@
         <v>183</v>
       </c>
       <c r="B188" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C188" s="23" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D188" s="12"/>
     </row>
@@ -4358,10 +4363,10 @@
         <v>184</v>
       </c>
       <c r="B189" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C189" s="23" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D189" s="12"/>
     </row>
@@ -4371,10 +4376,10 @@
         <v>185</v>
       </c>
       <c r="B190" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C190" s="23" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D190" s="12"/>
     </row>
@@ -4384,10 +4389,10 @@
         <v>186</v>
       </c>
       <c r="B191" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C191" s="23" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D191" s="12"/>
     </row>
@@ -4397,10 +4402,10 @@
         <v>187</v>
       </c>
       <c r="B192" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C192" s="23" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D192" s="12"/>
     </row>
@@ -4410,10 +4415,10 @@
         <v>188</v>
       </c>
       <c r="B193" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C193" s="23" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D193" s="12"/>
     </row>
@@ -4423,10 +4428,10 @@
         <v>189</v>
       </c>
       <c r="B194" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C194" s="23" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D194" s="12"/>
     </row>
@@ -4436,10 +4441,10 @@
         <v>190</v>
       </c>
       <c r="B195" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C195" s="23" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D195" s="12"/>
     </row>
@@ -4449,10 +4454,10 @@
         <v>191</v>
       </c>
       <c r="B196" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C196" s="23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D196" s="12"/>
     </row>
@@ -4462,10 +4467,10 @@
         <v>192</v>
       </c>
       <c r="B197" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C197" s="23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D197" s="12"/>
     </row>
@@ -4475,10 +4480,10 @@
         <v>193</v>
       </c>
       <c r="B198" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C198" s="23" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D198" s="12"/>
     </row>
@@ -4488,10 +4493,10 @@
         <v>194</v>
       </c>
       <c r="B199" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C199" s="23" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D199" s="12"/>
     </row>
@@ -4501,10 +4506,10 @@
         <v>195</v>
       </c>
       <c r="B200" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C200" s="23" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D200" s="12"/>
     </row>
@@ -4514,10 +4519,10 @@
         <v>196</v>
       </c>
       <c r="B201" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C201" s="23" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D201" s="12"/>
     </row>
@@ -4527,10 +4532,10 @@
         <v>197</v>
       </c>
       <c r="B202" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C202" s="23" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4539,10 +4544,10 @@
         <v>198</v>
       </c>
       <c r="B203" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C203" s="23" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4551,10 +4556,10 @@
         <v>199</v>
       </c>
       <c r="B204" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C204" s="23" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4563,10 +4568,10 @@
         <v>200</v>
       </c>
       <c r="B205" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C205" s="23" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4575,10 +4580,10 @@
         <v>201</v>
       </c>
       <c r="B206" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C206" s="23" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4587,10 +4592,10 @@
         <v>202</v>
       </c>
       <c r="B207" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C207" s="23" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4599,10 +4604,10 @@
         <v>203</v>
       </c>
       <c r="B208" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C208" s="25" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4611,10 +4616,10 @@
         <v>204</v>
       </c>
       <c r="B209" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C209" s="23" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4623,10 +4628,10 @@
         <v>205</v>
       </c>
       <c r="B210" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C210" s="23" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D210" s="12"/>
     </row>
@@ -4636,10 +4641,10 @@
         <v>206</v>
       </c>
       <c r="B211" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C211" s="23" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D211" s="12"/>
     </row>
@@ -4649,10 +4654,10 @@
         <v>207</v>
       </c>
       <c r="B212" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C212" s="23" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D212" s="12"/>
     </row>
@@ -4662,10 +4667,10 @@
         <v>208</v>
       </c>
       <c r="B213" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C213" s="23" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D213" s="12"/>
     </row>
@@ -4675,10 +4680,10 @@
         <v>209</v>
       </c>
       <c r="B214" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C214" s="23" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D214" s="12"/>
     </row>
@@ -4688,10 +4693,10 @@
         <v>210</v>
       </c>
       <c r="B215" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C215" s="23" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D215" s="12"/>
     </row>
@@ -4701,10 +4706,10 @@
         <v>211</v>
       </c>
       <c r="B216" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C216" s="23" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D216" s="12"/>
     </row>
@@ -4714,10 +4719,10 @@
         <v>212</v>
       </c>
       <c r="B217" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C217" s="23" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D217" s="12"/>
     </row>
@@ -4727,10 +4732,10 @@
         <v>213</v>
       </c>
       <c r="B218" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C218" s="23" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D218" s="12"/>
     </row>
@@ -4740,10 +4745,10 @@
         <v>214</v>
       </c>
       <c r="B219" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C219" s="23" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D219" s="12"/>
     </row>
@@ -4753,10 +4758,10 @@
         <v>215</v>
       </c>
       <c r="B220" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C220" s="23" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D220" s="12"/>
     </row>
@@ -4766,10 +4771,10 @@
         <v>216</v>
       </c>
       <c r="B221" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C221" s="23" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D221" s="12"/>
     </row>
@@ -4779,10 +4784,10 @@
         <v>217</v>
       </c>
       <c r="B222" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C222" s="23" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D222" s="12"/>
     </row>
@@ -4792,10 +4797,10 @@
         <v>218</v>
       </c>
       <c r="B223" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C223" s="23" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D223" s="12"/>
     </row>
@@ -4805,10 +4810,10 @@
         <v>219</v>
       </c>
       <c r="B224" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C224" s="23" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D224" s="12"/>
     </row>
@@ -4818,10 +4823,10 @@
         <v>220</v>
       </c>
       <c r="B225" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C225" s="23" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D225" s="12"/>
     </row>
@@ -4831,10 +4836,10 @@
         <v>221</v>
       </c>
       <c r="B226" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C226" s="23" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D226" s="12"/>
     </row>
@@ -4844,10 +4849,10 @@
         <v>222</v>
       </c>
       <c r="B227" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C227" s="23" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D227" s="12"/>
     </row>
@@ -4857,10 +4862,10 @@
         <v>223</v>
       </c>
       <c r="B228" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C228" s="23" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D228" s="12"/>
     </row>
@@ -4870,10 +4875,10 @@
         <v>224</v>
       </c>
       <c r="B229" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C229" s="23" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D229" s="12"/>
     </row>
@@ -4883,10 +4888,10 @@
         <v>225</v>
       </c>
       <c r="B230" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C230" s="23" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D230" s="12"/>
     </row>
@@ -4896,10 +4901,10 @@
         <v>226</v>
       </c>
       <c r="B231" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C231" s="23" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D231" s="12"/>
     </row>
@@ -4909,10 +4914,10 @@
         <v>227</v>
       </c>
       <c r="B232" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C232" s="23" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D232" s="12"/>
     </row>
@@ -4922,10 +4927,10 @@
         <v>228</v>
       </c>
       <c r="B233" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C233" s="23" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D233" s="12"/>
     </row>
@@ -4935,10 +4940,10 @@
         <v>229</v>
       </c>
       <c r="B234" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C234" s="23" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D234" s="12"/>
     </row>
@@ -4948,10 +4953,10 @@
         <v>230</v>
       </c>
       <c r="B235" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C235" s="23" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D235" s="12"/>
     </row>
@@ -4961,10 +4966,10 @@
         <v>231</v>
       </c>
       <c r="B236" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C236" s="23" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D236" s="12"/>
     </row>
@@ -4974,10 +4979,10 @@
         <v>232</v>
       </c>
       <c r="B237" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C237" s="23" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D237" s="12"/>
     </row>
@@ -4987,10 +4992,10 @@
         <v>233</v>
       </c>
       <c r="B238" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C238" s="23" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D238" s="12"/>
     </row>
@@ -5000,10 +5005,10 @@
         <v>234</v>
       </c>
       <c r="B239" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C239" s="23" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D239" s="12"/>
     </row>
@@ -5013,10 +5018,10 @@
         <v>235</v>
       </c>
       <c r="B240" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C240" s="23" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D240" s="12"/>
     </row>
@@ -5026,10 +5031,10 @@
         <v>236</v>
       </c>
       <c r="B241" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C241" s="23" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D241" s="12"/>
     </row>
@@ -5039,10 +5044,10 @@
         <v>237</v>
       </c>
       <c r="B242" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C242" s="23" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D242" s="12"/>
     </row>
@@ -5052,10 +5057,10 @@
         <v>238</v>
       </c>
       <c r="B243" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C243" s="23" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D243" s="12"/>
     </row>
@@ -5065,10 +5070,10 @@
         <v>239</v>
       </c>
       <c r="B244" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C244" s="23" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D244" s="12"/>
     </row>
@@ -5078,10 +5083,10 @@
         <v>240</v>
       </c>
       <c r="B245" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C245" s="23" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D245" s="12"/>
     </row>
@@ -5091,10 +5096,10 @@
         <v>241</v>
       </c>
       <c r="B246" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C246" s="23" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D246" s="12"/>
     </row>
@@ -5104,10 +5109,10 @@
         <v>242</v>
       </c>
       <c r="B247" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C247" s="23" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D247" s="12"/>
     </row>
@@ -5117,10 +5122,10 @@
         <v>243</v>
       </c>
       <c r="B248" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C248" s="23" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D248" s="12"/>
     </row>
@@ -5130,10 +5135,10 @@
         <v>244</v>
       </c>
       <c r="B249" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C249" s="23" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D249" s="12"/>
     </row>
@@ -5143,10 +5148,10 @@
         <v>245</v>
       </c>
       <c r="B250" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C250" s="23" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D250" s="12"/>
     </row>
@@ -5156,10 +5161,10 @@
         <v>246</v>
       </c>
       <c r="B251" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C251" s="23" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D251" s="12"/>
     </row>
@@ -5169,10 +5174,10 @@
         <v>247</v>
       </c>
       <c r="B252" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C252" s="23" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D252" s="12"/>
     </row>
@@ -5182,10 +5187,10 @@
         <v>248</v>
       </c>
       <c r="B253" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C253" s="23" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D253" s="12"/>
     </row>
@@ -5195,10 +5200,10 @@
         <v>249</v>
       </c>
       <c r="B254" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C254" s="23" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D254" s="12"/>
     </row>
@@ -5208,10 +5213,10 @@
         <v>250</v>
       </c>
       <c r="B255" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C255" s="23" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D255" s="12"/>
     </row>
@@ -5221,10 +5226,10 @@
         <v>251</v>
       </c>
       <c r="B256" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C256" s="23" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D256" s="12"/>
     </row>
@@ -5234,10 +5239,10 @@
         <v>252</v>
       </c>
       <c r="B257" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C257" s="23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D257" s="12"/>
     </row>
@@ -5247,10 +5252,10 @@
         <v>253</v>
       </c>
       <c r="B258" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C258" s="23" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D258" s="12"/>
     </row>
@@ -5260,10 +5265,10 @@
         <v>254</v>
       </c>
       <c r="B259" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C259" s="23" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D259" s="12"/>
     </row>
@@ -5273,10 +5278,10 @@
         <v>255</v>
       </c>
       <c r="B260" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C260" s="23" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D260" s="12"/>
     </row>
@@ -5286,10 +5291,10 @@
         <v>256</v>
       </c>
       <c r="B261" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C261" s="23" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D261" s="12"/>
     </row>
@@ -5299,10 +5304,10 @@
         <v>257</v>
       </c>
       <c r="B262" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C262" s="23" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D262" s="12"/>
     </row>
@@ -5312,10 +5317,10 @@
         <v>258</v>
       </c>
       <c r="B263" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C263" s="23" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D263" s="12"/>
     </row>
@@ -5325,10 +5330,10 @@
         <v>259</v>
       </c>
       <c r="B264" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C264" s="23" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D264" s="12"/>
     </row>
@@ -5338,10 +5343,10 @@
         <v>260</v>
       </c>
       <c r="B265" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C265" s="23" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D265" s="12"/>
     </row>
@@ -5351,10 +5356,10 @@
         <v>261</v>
       </c>
       <c r="B266" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C266" s="23" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D266" s="12"/>
     </row>
@@ -5364,10 +5369,10 @@
         <v>262</v>
       </c>
       <c r="B267" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C267" s="23" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D267" s="12"/>
     </row>
@@ -5377,10 +5382,10 @@
         <v>263</v>
       </c>
       <c r="B268" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C268" s="23" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D268" s="12"/>
     </row>
@@ -5390,10 +5395,10 @@
         <v>264</v>
       </c>
       <c r="B269" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C269" s="23" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D269" s="12"/>
     </row>
@@ -5403,10 +5408,10 @@
         <v>265</v>
       </c>
       <c r="B270" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C270" s="23" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D270" s="12"/>
     </row>
@@ -5416,10 +5421,10 @@
         <v>266</v>
       </c>
       <c r="B271" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C271" s="23" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D271" s="12"/>
     </row>
@@ -5429,10 +5434,10 @@
         <v>267</v>
       </c>
       <c r="B272" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C272" s="23" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D272" s="12"/>
     </row>
@@ -5442,10 +5447,10 @@
         <v>268</v>
       </c>
       <c r="B273" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C273" s="23" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D273" s="12"/>
     </row>
@@ -5455,10 +5460,10 @@
         <v>269</v>
       </c>
       <c r="B274" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C274" s="23" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D274" s="12"/>
     </row>
@@ -5468,10 +5473,10 @@
         <v>270</v>
       </c>
       <c r="B275" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C275" s="23" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D275" s="12"/>
     </row>
@@ -5481,10 +5486,10 @@
         <v>271</v>
       </c>
       <c r="B276" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C276" s="23" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D276" s="12"/>
     </row>
@@ -5494,10 +5499,10 @@
         <v>272</v>
       </c>
       <c r="B277" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C277" s="23" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D277" s="12"/>
     </row>
@@ -5507,10 +5512,10 @@
         <v>273</v>
       </c>
       <c r="B278" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C278" s="23" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D278" s="12"/>
     </row>
@@ -5520,10 +5525,10 @@
         <v>274</v>
       </c>
       <c r="B279" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C279" s="23" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D279" s="12"/>
     </row>
@@ -5533,10 +5538,10 @@
         <v>275</v>
       </c>
       <c r="B280" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C280" s="23" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D280" s="12"/>
     </row>
@@ -5546,10 +5551,10 @@
         <v>276</v>
       </c>
       <c r="B281" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C281" s="23" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D281" s="12"/>
     </row>
@@ -5559,10 +5564,10 @@
         <v>277</v>
       </c>
       <c r="B282" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C282" s="23" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D282" s="12"/>
     </row>
@@ -5572,10 +5577,10 @@
         <v>278</v>
       </c>
       <c r="B283" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C283" s="23" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D283" s="12"/>
     </row>
@@ -5585,10 +5590,10 @@
         <v>279</v>
       </c>
       <c r="B284" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C284" s="23" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D284" s="12"/>
     </row>
@@ -5598,10 +5603,10 @@
         <v>280</v>
       </c>
       <c r="B285" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C285" s="23" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D285" s="12"/>
     </row>
@@ -5611,10 +5616,10 @@
         <v>281</v>
       </c>
       <c r="B286" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C286" s="23" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D286" s="12"/>
     </row>
@@ -5624,10 +5629,10 @@
         <v>282</v>
       </c>
       <c r="B287" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C287" s="23" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D287" s="12"/>
     </row>
@@ -5637,10 +5642,10 @@
         <v>283</v>
       </c>
       <c r="B288" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C288" s="23" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D288" s="12"/>
     </row>
@@ -5650,10 +5655,10 @@
         <v>284</v>
       </c>
       <c r="B289" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C289" s="23" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D289" s="12"/>
     </row>
@@ -5663,10 +5668,10 @@
         <v>285</v>
       </c>
       <c r="B290" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C290" s="23" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D290" s="12"/>
     </row>
@@ -5676,10 +5681,10 @@
         <v>286</v>
       </c>
       <c r="B291" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C291" s="25" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D291" s="12"/>
     </row>
@@ -5689,10 +5694,10 @@
         <v>287</v>
       </c>
       <c r="B292" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C292" s="23" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D292" s="12"/>
     </row>
@@ -5702,10 +5707,10 @@
         <v>288</v>
       </c>
       <c r="B293" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C293" s="23" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D293" s="12"/>
     </row>
@@ -5715,10 +5720,10 @@
         <v>289</v>
       </c>
       <c r="B294" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C294" s="23" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D294" s="12"/>
     </row>
@@ -5728,10 +5733,10 @@
         <v>290</v>
       </c>
       <c r="B295" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C295" s="23" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D295" s="12"/>
     </row>
@@ -5741,10 +5746,10 @@
         <v>291</v>
       </c>
       <c r="B296" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C296" s="23" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D296" s="12"/>
     </row>
@@ -5754,10 +5759,10 @@
         <v>292</v>
       </c>
       <c r="B297" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C297" s="23" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D297" s="12"/>
     </row>
@@ -5767,10 +5772,10 @@
         <v>293</v>
       </c>
       <c r="B298" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C298" s="23" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D298" s="12"/>
     </row>
@@ -5780,10 +5785,10 @@
         <v>294</v>
       </c>
       <c r="B299" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C299" s="23" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D299" s="12"/>
     </row>
@@ -5793,10 +5798,10 @@
         <v>295</v>
       </c>
       <c r="B300" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C300" s="23" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D300" s="12"/>
     </row>
@@ -5806,10 +5811,10 @@
         <v>296</v>
       </c>
       <c r="B301" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C301" s="23" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D301" s="12"/>
     </row>
@@ -5819,10 +5824,10 @@
         <v>297</v>
       </c>
       <c r="B302" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C302" s="23" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D302" s="12"/>
     </row>
@@ -5832,10 +5837,10 @@
         <v>298</v>
       </c>
       <c r="B303" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C303" s="23" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D303" s="12"/>
     </row>
@@ -5845,10 +5850,10 @@
         <v>299</v>
       </c>
       <c r="B304" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C304" s="23" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D304" s="12"/>
     </row>
@@ -5858,10 +5863,10 @@
         <v>300</v>
       </c>
       <c r="B305" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C305" s="23" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D305" s="12"/>
     </row>
@@ -5871,10 +5876,10 @@
         <v>301</v>
       </c>
       <c r="B306" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C306" s="23" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D306" s="12"/>
     </row>
@@ -5884,10 +5889,10 @@
         <v>302</v>
       </c>
       <c r="B307" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C307" s="23" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D307" s="12"/>
     </row>
@@ -5897,10 +5902,10 @@
         <v>303</v>
       </c>
       <c r="B308" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C308" s="23" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D308" s="12"/>
     </row>
@@ -5910,10 +5915,10 @@
         <v>304</v>
       </c>
       <c r="B309" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C309" s="23" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D309" s="12"/>
     </row>
@@ -5923,10 +5928,10 @@
         <v>305</v>
       </c>
       <c r="B310" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C310" s="23" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D310" s="12"/>
     </row>
@@ -5936,10 +5941,10 @@
         <v>306</v>
       </c>
       <c r="B311" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C311" s="23" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D311" s="12"/>
     </row>
@@ -5949,10 +5954,10 @@
         <v>307</v>
       </c>
       <c r="B312" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C312" s="23" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D312" s="12"/>
     </row>
@@ -5962,10 +5967,10 @@
         <v>308</v>
       </c>
       <c r="B313" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C313" s="23" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D313" s="12"/>
     </row>
@@ -5975,10 +5980,10 @@
         <v>309</v>
       </c>
       <c r="B314" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C314" s="23" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D314" s="12"/>
     </row>
@@ -5988,10 +5993,10 @@
         <v>310</v>
       </c>
       <c r="B315" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C315" s="23" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D315" s="12"/>
     </row>
@@ -6001,10 +6006,10 @@
         <v>311</v>
       </c>
       <c r="B316" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C316" s="23" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D316" s="12"/>
     </row>
@@ -6014,10 +6019,10 @@
         <v>312</v>
       </c>
       <c r="B317" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C317" s="23" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D317" s="12"/>
     </row>
@@ -6027,10 +6032,10 @@
         <v>313</v>
       </c>
       <c r="B318" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C318" s="23" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D318" s="12"/>
     </row>
@@ -6040,10 +6045,10 @@
         <v>314</v>
       </c>
       <c r="B319" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C319" s="23" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D319" s="12"/>
     </row>
@@ -6053,10 +6058,10 @@
         <v>315</v>
       </c>
       <c r="B320" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C320" s="23" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D320" s="12"/>
     </row>
@@ -6066,10 +6071,10 @@
         <v>316</v>
       </c>
       <c r="B321" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C321" s="23" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D321" s="12"/>
     </row>
@@ -6079,10 +6084,10 @@
         <v>317</v>
       </c>
       <c r="B322" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C322" s="23" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D322" s="12"/>
     </row>
@@ -6092,10 +6097,10 @@
         <v>318</v>
       </c>
       <c r="B323" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C323" s="23" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D323" s="12"/>
     </row>
@@ -6105,10 +6110,10 @@
         <v>319</v>
       </c>
       <c r="B324" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C324" s="25" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D324" s="12"/>
     </row>
@@ -6118,10 +6123,10 @@
         <v>320</v>
       </c>
       <c r="B325" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C325" s="23" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D325" s="12"/>
     </row>
@@ -6131,10 +6136,10 @@
         <v>321</v>
       </c>
       <c r="B326" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C326" s="23" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D326" s="12"/>
     </row>
@@ -6144,10 +6149,10 @@
         <v>322</v>
       </c>
       <c r="B327" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C327" s="23" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D327" s="12"/>
     </row>
@@ -6157,10 +6162,10 @@
         <v>323</v>
       </c>
       <c r="B328" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C328" s="23" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D328" s="12"/>
     </row>
@@ -6170,10 +6175,10 @@
         <v>324</v>
       </c>
       <c r="B329" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C329" s="23" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D329" s="12"/>
     </row>
@@ -6183,10 +6188,10 @@
         <v>325</v>
       </c>
       <c r="B330" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C330" s="23" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D330" s="12"/>
     </row>
@@ -6196,10 +6201,10 @@
         <v>326</v>
       </c>
       <c r="B331" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C331" s="23" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D331" s="12"/>
     </row>
@@ -6209,10 +6214,10 @@
         <v>327</v>
       </c>
       <c r="B332" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C332" s="23" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D332" s="12"/>
     </row>
@@ -6222,10 +6227,10 @@
         <v>328</v>
       </c>
       <c r="B333" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C333" s="23" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D333" s="12"/>
     </row>
@@ -6235,10 +6240,10 @@
         <v>329</v>
       </c>
       <c r="B334" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C334" s="23" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D334" s="12"/>
     </row>
@@ -6248,10 +6253,10 @@
         <v>330</v>
       </c>
       <c r="B335" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C335" s="23" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D335" s="12"/>
     </row>
@@ -6261,10 +6266,10 @@
         <v>331</v>
       </c>
       <c r="B336" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C336" s="23" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D336" s="12"/>
     </row>
@@ -6274,10 +6279,10 @@
         <v>332</v>
       </c>
       <c r="B337" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C337" s="23" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D337" s="12"/>
     </row>
@@ -6287,10 +6292,10 @@
         <v>333</v>
       </c>
       <c r="B338" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C338" s="23" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D338" s="12"/>
     </row>
@@ -6300,10 +6305,10 @@
         <v>334</v>
       </c>
       <c r="B339" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C339" s="23" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D339" s="12"/>
     </row>
@@ -6313,10 +6318,10 @@
         <v>335</v>
       </c>
       <c r="B340" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C340" s="23" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D340" s="12"/>
     </row>
@@ -6326,10 +6331,10 @@
         <v>336</v>
       </c>
       <c r="B341" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C341" s="23" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D341" s="12"/>
     </row>
@@ -6339,10 +6344,10 @@
         <v>337</v>
       </c>
       <c r="B342" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C342" s="23" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D342" s="12"/>
     </row>
@@ -6352,10 +6357,10 @@
         <v>338</v>
       </c>
       <c r="B343" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C343" s="23" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D343" s="12"/>
     </row>
@@ -6365,10 +6370,10 @@
         <v>339</v>
       </c>
       <c r="B344" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C344" s="23" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D344" s="12"/>
     </row>
@@ -6378,10 +6383,10 @@
         <v>340</v>
       </c>
       <c r="B345" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C345" s="23" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D345" s="12"/>
     </row>
@@ -6391,10 +6396,10 @@
         <v>341</v>
       </c>
       <c r="B346" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C346" s="23" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D346" s="12"/>
     </row>
@@ -6404,10 +6409,10 @@
         <v>342</v>
       </c>
       <c r="B347" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C347" s="23" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D347" s="12"/>
     </row>
@@ -6417,10 +6422,10 @@
         <v>343</v>
       </c>
       <c r="B348" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C348" s="23" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D348" s="12"/>
     </row>
@@ -6430,10 +6435,10 @@
         <v>344</v>
       </c>
       <c r="B349" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C349" s="23" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D349" s="12"/>
     </row>
@@ -6443,10 +6448,10 @@
         <v>345</v>
       </c>
       <c r="B350" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C350" s="23" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D350" s="12"/>
     </row>
@@ -6456,10 +6461,10 @@
         <v>346</v>
       </c>
       <c r="B351" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C351" s="23" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D351" s="12"/>
     </row>
@@ -6469,10 +6474,10 @@
         <v>347</v>
       </c>
       <c r="B352" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C352" s="23" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D352" s="12"/>
     </row>
@@ -6482,10 +6487,10 @@
         <v>348</v>
       </c>
       <c r="B353" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C353" s="23" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D353" s="12"/>
     </row>
@@ -6495,10 +6500,10 @@
         <v>349</v>
       </c>
       <c r="B354" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C354" s="23" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D354" s="12"/>
     </row>
@@ -6508,10 +6513,10 @@
         <v>350</v>
       </c>
       <c r="B355" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C355" s="23" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D355" s="12"/>
     </row>
@@ -6521,10 +6526,10 @@
         <v>351</v>
       </c>
       <c r="B356" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C356" s="23" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D356" s="12"/>
     </row>
@@ -6534,10 +6539,10 @@
         <v>352</v>
       </c>
       <c r="B357" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C357" s="23" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D357" s="12"/>
     </row>
@@ -6547,10 +6552,10 @@
         <v>353</v>
       </c>
       <c r="B358" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C358" s="23" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D358" s="12"/>
     </row>
@@ -6560,10 +6565,10 @@
         <v>354</v>
       </c>
       <c r="B359" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C359" s="23" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D359" s="12"/>
     </row>
@@ -6573,10 +6578,10 @@
         <v>355</v>
       </c>
       <c r="B360" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C360" s="23" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D360" s="12"/>
     </row>
@@ -6586,10 +6591,10 @@
         <v>356</v>
       </c>
       <c r="B361" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C361" s="23" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D361" s="12"/>
     </row>
@@ -6599,10 +6604,10 @@
         <v>357</v>
       </c>
       <c r="B362" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C362" s="23" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D362" s="12"/>
     </row>
@@ -6612,10 +6617,10 @@
         <v>358</v>
       </c>
       <c r="B363" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C363" s="23" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D363" s="12"/>
     </row>
@@ -6625,10 +6630,10 @@
         <v>359</v>
       </c>
       <c r="B364" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C364" s="23" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D364" s="12"/>
     </row>
@@ -6638,10 +6643,10 @@
         <v>360</v>
       </c>
       <c r="B365" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C365" s="23" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D365" s="12"/>
     </row>
@@ -6651,10 +6656,10 @@
         <v>361</v>
       </c>
       <c r="B366" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C366" s="23" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D366" s="12"/>
     </row>
@@ -6664,10 +6669,10 @@
         <v>362</v>
       </c>
       <c r="B367" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C367" s="23" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D367" s="12"/>
     </row>
@@ -6677,10 +6682,10 @@
         <v>363</v>
       </c>
       <c r="B368" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C368" s="23" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D368" s="12"/>
     </row>
@@ -6690,10 +6695,10 @@
         <v>364</v>
       </c>
       <c r="B369" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C369" s="23" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D369" s="12"/>
     </row>
@@ -6703,10 +6708,10 @@
         <v>365</v>
       </c>
       <c r="B370" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C370" s="23" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D370" s="12"/>
     </row>
@@ -6716,10 +6721,10 @@
         <v>366</v>
       </c>
       <c r="B371" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C371" s="23" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D371" s="12"/>
     </row>
@@ -6729,10 +6734,10 @@
         <v>367</v>
       </c>
       <c r="B372" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C372" s="23" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D372" s="12"/>
     </row>
@@ -6742,10 +6747,10 @@
         <v>368</v>
       </c>
       <c r="B373" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C373" s="23" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D373" s="12"/>
     </row>
@@ -6755,10 +6760,10 @@
         <v>369</v>
       </c>
       <c r="B374" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C374" s="23" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D374" s="12"/>
     </row>
@@ -6768,10 +6773,10 @@
         <v>370</v>
       </c>
       <c r="B375" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C375" s="23" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D375" s="12"/>
     </row>
@@ -6781,10 +6786,10 @@
         <v>371</v>
       </c>
       <c r="B376" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C376" s="23" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D376" s="12"/>
     </row>
@@ -6794,10 +6799,10 @@
         <v>372</v>
       </c>
       <c r="B377" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C377" s="23" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D377" s="12"/>
     </row>
@@ -6807,10 +6812,10 @@
         <v>373</v>
       </c>
       <c r="B378" s="10" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C378" s="23" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D378" s="12"/>
     </row>
@@ -6820,10 +6825,10 @@
         <v>374</v>
       </c>
       <c r="B379" s="10" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C379" s="23" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D379" s="12"/>
     </row>
@@ -6833,10 +6838,10 @@
         <v>375</v>
       </c>
       <c r="B380" s="10" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C380" s="23" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D380" s="12"/>
     </row>
@@ -6846,10 +6851,10 @@
         <v>376</v>
       </c>
       <c r="B381" s="10" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C381" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D381" s="12"/>
     </row>
@@ -6859,10 +6864,10 @@
         <v>377</v>
       </c>
       <c r="B382" s="10" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C382" s="23" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D382" s="12"/>
     </row>
@@ -6872,10 +6877,10 @@
         <v>378</v>
       </c>
       <c r="B383" s="10" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C383" s="23" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D383" s="12"/>
     </row>
@@ -6885,10 +6890,10 @@
         <v>379</v>
       </c>
       <c r="B384" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C384" s="23" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D384" s="12"/>
     </row>
@@ -6898,10 +6903,10 @@
         <v>380</v>
       </c>
       <c r="B385" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C385" s="23" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D385" s="12"/>
     </row>
@@ -6911,10 +6916,10 @@
         <v>381</v>
       </c>
       <c r="B386" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C386" s="23" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D386" s="12"/>
     </row>
@@ -6924,10 +6929,10 @@
         <v>382</v>
       </c>
       <c r="B387" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C387" s="23" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D387" s="12"/>
     </row>
@@ -6937,10 +6942,10 @@
         <v>383</v>
       </c>
       <c r="B388" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C388" s="23" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D388" s="12"/>
     </row>
@@ -6950,10 +6955,10 @@
         <v>384</v>
       </c>
       <c r="B389" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C389" s="23" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D389" s="12"/>
     </row>
@@ -6963,10 +6968,10 @@
         <v>385</v>
       </c>
       <c r="B390" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C390" s="23" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D390" s="12"/>
     </row>
@@ -6976,10 +6981,10 @@
         <v>386</v>
       </c>
       <c r="B391" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C391" s="23" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D391" s="12"/>
     </row>
@@ -6989,10 +6994,10 @@
         <v>387</v>
       </c>
       <c r="B392" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C392" s="23" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D392" s="12"/>
     </row>
@@ -7002,10 +7007,10 @@
         <v>388</v>
       </c>
       <c r="B393" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C393" s="23" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D393" s="12"/>
     </row>
@@ -7015,10 +7020,10 @@
         <v>389</v>
       </c>
       <c r="B394" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C394" s="23" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D394" s="12"/>
     </row>
@@ -7028,10 +7033,10 @@
         <v>390</v>
       </c>
       <c r="B395" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C395" s="23" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D395" s="12"/>
     </row>
@@ -7041,10 +7046,10 @@
         <v>391</v>
       </c>
       <c r="B396" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C396" s="23" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D396" s="12"/>
     </row>
@@ -7054,10 +7059,10 @@
         <v>392</v>
       </c>
       <c r="B397" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C397" s="23" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D397" s="12"/>
     </row>
@@ -7067,10 +7072,10 @@
         <v>393</v>
       </c>
       <c r="B398" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C398" s="23" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D398" s="12"/>
     </row>
@@ -7080,10 +7085,10 @@
         <v>394</v>
       </c>
       <c r="B399" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C399" s="23" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D399" s="12"/>
     </row>
@@ -7093,10 +7098,10 @@
         <v>395</v>
       </c>
       <c r="B400" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C400" s="23" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D400" s="12"/>
     </row>
@@ -7106,10 +7111,10 @@
         <v>396</v>
       </c>
       <c r="B401" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C401" s="23" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D401" s="12"/>
     </row>
@@ -7119,10 +7124,10 @@
         <v>397</v>
       </c>
       <c r="B402" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C402" s="23" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D402" s="12"/>
     </row>
@@ -7132,10 +7137,10 @@
         <v>398</v>
       </c>
       <c r="B403" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C403" s="23" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D403" s="12"/>
     </row>
@@ -7145,10 +7150,10 @@
         <v>399</v>
       </c>
       <c r="B404" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C404" s="23" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D404" s="12"/>
     </row>
@@ -7158,10 +7163,10 @@
         <v>400</v>
       </c>
       <c r="B405" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C405" s="23" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D405" s="12"/>
     </row>
@@ -7171,10 +7176,10 @@
         <v>401</v>
       </c>
       <c r="B406" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C406" s="23" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D406" s="12"/>
     </row>
@@ -7184,10 +7189,10 @@
         <v>402</v>
       </c>
       <c r="B407" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C407" s="23" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D407" s="12"/>
     </row>
@@ -7197,10 +7202,10 @@
         <v>403</v>
       </c>
       <c r="B408" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C408" s="23" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D408" s="12"/>
     </row>
@@ -7210,10 +7215,10 @@
         <v>404</v>
       </c>
       <c r="B409" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C409" s="23" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D409" s="12"/>
     </row>
@@ -7223,10 +7228,10 @@
         <v>405</v>
       </c>
       <c r="B410" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C410" s="23" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D410" s="12"/>
     </row>
@@ -7236,10 +7241,10 @@
         <v>406</v>
       </c>
       <c r="B411" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C411" s="23" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D411" s="12"/>
     </row>
@@ -7249,10 +7254,10 @@
         <v>407</v>
       </c>
       <c r="B412" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C412" s="23" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D412" s="12"/>
     </row>
@@ -7262,10 +7267,10 @@
         <v>408</v>
       </c>
       <c r="B413" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C413" s="23" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D413" s="12"/>
     </row>
@@ -7275,10 +7280,10 @@
         <v>409</v>
       </c>
       <c r="B414" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C414" s="23" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D414" s="12"/>
     </row>
@@ -7288,10 +7293,10 @@
         <v>410</v>
       </c>
       <c r="B415" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C415" s="23" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D415" s="12"/>
     </row>
@@ -7301,10 +7306,10 @@
         <v>411</v>
       </c>
       <c r="B416" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C416" s="23" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D416" s="12"/>
     </row>
@@ -7314,10 +7319,10 @@
         <v>412</v>
       </c>
       <c r="B417" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C417" s="23" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D417" s="12"/>
     </row>
@@ -7327,10 +7332,10 @@
         <v>413</v>
       </c>
       <c r="B418" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C418" s="23" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D418" s="12"/>
     </row>
@@ -7340,10 +7345,10 @@
         <v>414</v>
       </c>
       <c r="B419" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C419" s="23" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D419" s="12"/>
     </row>
@@ -7353,10 +7358,10 @@
         <v>415</v>
       </c>
       <c r="B420" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C420" s="23" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D420" s="12"/>
     </row>
@@ -7366,10 +7371,10 @@
         <v>416</v>
       </c>
       <c r="B421" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C421" s="23" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D421" s="12"/>
     </row>
@@ -7379,10 +7384,10 @@
         <v>417</v>
       </c>
       <c r="B422" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C422" s="23" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D422" s="12"/>
     </row>
@@ -7392,10 +7397,10 @@
         <v>418</v>
       </c>
       <c r="B423" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C423" s="23" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D423" s="12"/>
     </row>
@@ -7405,10 +7410,10 @@
         <v>419</v>
       </c>
       <c r="B424" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C424" s="23" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D424" s="12"/>
     </row>
@@ -7418,10 +7423,10 @@
         <v>420</v>
       </c>
       <c r="B425" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C425" s="23" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D425" s="12"/>
     </row>
@@ -7431,10 +7436,10 @@
         <v>421</v>
       </c>
       <c r="B426" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C426" s="23" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D426" s="12"/>
     </row>
@@ -7444,10 +7449,10 @@
         <v>422</v>
       </c>
       <c r="B427" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C427" s="23" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D427" s="12"/>
     </row>
@@ -7457,10 +7462,10 @@
         <v>423</v>
       </c>
       <c r="B428" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C428" s="23" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D428" s="12"/>
     </row>
@@ -7470,10 +7475,10 @@
         <v>424</v>
       </c>
       <c r="B429" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C429" s="23" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D429" s="12"/>
     </row>
@@ -7483,10 +7488,10 @@
         <v>425</v>
       </c>
       <c r="B430" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C430" s="23" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D430" s="12"/>
     </row>
@@ -7496,10 +7501,10 @@
         <v>426</v>
       </c>
       <c r="B431" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C431" s="23" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D431" s="12"/>
     </row>
@@ -7509,10 +7514,10 @@
         <v>427</v>
       </c>
       <c r="B432" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C432" s="23" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D432" s="12"/>
     </row>
@@ -7522,10 +7527,10 @@
         <v>428</v>
       </c>
       <c r="B433" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C433" s="23" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D433" s="12"/>
     </row>
@@ -7535,10 +7540,10 @@
         <v>429</v>
       </c>
       <c r="B434" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C434" s="23" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D434" s="12"/>
     </row>
@@ -7548,10 +7553,10 @@
         <v>430</v>
       </c>
       <c r="B435" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C435" s="23" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D435" s="12"/>
     </row>
@@ -7561,10 +7566,10 @@
         <v>431</v>
       </c>
       <c r="B436" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C436" s="23" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D436" s="12"/>
     </row>
@@ -7574,10 +7579,10 @@
         <v>432</v>
       </c>
       <c r="B437" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C437" s="23" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D437" s="12"/>
     </row>
@@ -7587,10 +7592,10 @@
         <v>433</v>
       </c>
       <c r="B438" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C438" s="23" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D438" s="12"/>
     </row>
@@ -7600,10 +7605,10 @@
         <v>434</v>
       </c>
       <c r="B439" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C439" s="23" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D439" s="12"/>
     </row>
@@ -7613,10 +7618,10 @@
         <v>435</v>
       </c>
       <c r="B440" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C440" s="23" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D440" s="12"/>
     </row>
@@ -7626,10 +7631,10 @@
         <v>436</v>
       </c>
       <c r="B441" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C441" s="23" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D441" s="12"/>
     </row>
@@ -7639,10 +7644,10 @@
         <v>437</v>
       </c>
       <c r="B442" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C442" s="23" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D442" s="12"/>
     </row>
@@ -7652,10 +7657,10 @@
         <v>438</v>
       </c>
       <c r="B443" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C443" s="23" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D443" s="12"/>
     </row>
@@ -7665,10 +7670,10 @@
         <v>439</v>
       </c>
       <c r="B444" s="10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C444" s="23" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D444" s="12"/>
     </row>
@@ -7678,10 +7683,10 @@
         <v>440</v>
       </c>
       <c r="B445" s="10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C445" s="23" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D445" s="12"/>
     </row>
@@ -7691,10 +7696,10 @@
         <v>441</v>
       </c>
       <c r="B446" s="10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C446" s="23" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D446" s="12"/>
     </row>
@@ -7704,10 +7709,10 @@
         <v>442</v>
       </c>
       <c r="B447" s="10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C447" s="23" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D447" s="12"/>
     </row>
@@ -7717,10 +7722,10 @@
         <v>443</v>
       </c>
       <c r="B448" s="10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C448" s="23" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D448" s="12"/>
     </row>
@@ -7730,10 +7735,10 @@
         <v>444</v>
       </c>
       <c r="B449" s="10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C449" s="23" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D449" s="12"/>
     </row>
@@ -7743,10 +7748,10 @@
         <v>445</v>
       </c>
       <c r="B450" s="10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C450" s="23" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D450" s="12"/>
     </row>
@@ -7756,10 +7761,10 @@
         <v>446</v>
       </c>
       <c r="B451" s="10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C451" s="23" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D451" s="12"/>
     </row>
@@ -7769,10 +7774,10 @@
         <v>447</v>
       </c>
       <c r="B452" s="10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C452" s="23" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D452" s="12"/>
     </row>
@@ -7782,10 +7787,10 @@
         <v>448</v>
       </c>
       <c r="B453" s="10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C453" s="23" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D453" s="12"/>
     </row>

</xml_diff>

<commit_message>
Q64 corrected MAJOR FLAWS src: stackoverflow
</commit_message>
<xml_diff>
--- a/DSA_450_LoveBabbar.xlsx
+++ b/DSA_450_LoveBabbar.xlsx
@@ -322,7 +322,26 @@
     <t xml:space="preserve">Rabin Karp Algo</t>
   </si>
   <si>
-    <t xml:space="preserve">doubt: Why mod = 1e9+7 gave the wrong answer, but 1e5+7 worked fine</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">doubt: Why mod = 1e9+7 gave the wrong answer, but 1e5+7 worked fine </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[ANSWERED]</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">KMP Algo</t>
@@ -1937,10 +1956,10 @@
   <dimension ref="A1:D467"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D70" activeCellId="0" sqref="D70"/>
+      <selection pane="topLeft" activeCell="D68" activeCellId="0" sqref="D68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.79296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.24"/>
@@ -7917,7 +7936,7 @@
     <hyperlink ref="C67" r:id="rId62" display="Balanced Parenthesis problem.[Imp]"/>
     <hyperlink ref="C68" r:id="rId63" display="Word break Problem[ Very Imp]"/>
     <hyperlink ref="C69" r:id="rId64" display="Rabin Karp Algo"/>
-    <hyperlink ref="D69" r:id="rId65" display="doubt"/>
+    <hyperlink ref="D69" r:id="rId65" display="doubt: Why mod = 1e9+7 gave the wrong answer, but 1e5+7 worked fine"/>
     <hyperlink ref="C70" r:id="rId66" display="KMP Algo"/>
     <hyperlink ref="C71" r:id="rId67" display="Convert a Sentence into its equivalent mobile numeric keypad sequence."/>
     <hyperlink ref="C72" r:id="rId68" display="Minimum number of bracket reversals needed to make an expression balanced."/>

</xml_diff>

<commit_message>
done Q65 Knuth Morris Pratt pattern searching
</commit_message>
<xml_diff>
--- a/DSA_450_LoveBabbar.xlsx
+++ b/DSA_450_LoveBabbar.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="474">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -322,29 +322,13 @@
     <t xml:space="preserve">Rabin Karp Algo</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">doubt: Why mod = 1e9+7 gave the wrong answer, but 1e5+7 worked fine </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00A933"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[ANSWERED]</t>
-    </r>
+    <t xml:space="preserve">doubt: Why mod = 1e9+7 gave the wrong answer, but 1e5+7 worked fine [ANSWERED]</t>
   </si>
   <si>
     <t xml:space="preserve">KMP Algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V.Important</t>
   </si>
   <si>
     <t xml:space="preserve">Convert a Sentence into its equivalent mobile numeric keypad sequence.</t>
@@ -1955,11 +1939,11 @@
   </sheetPr>
   <dimension ref="A1:D467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D68" activeCellId="0" sqref="D68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C71" activeCellId="0" sqref="C71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.79296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.24"/>
@@ -2852,10 +2836,12 @@
       <c r="B70" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C70" s="24" t="s">
+      <c r="C70" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="D70" s="12"/>
+      <c r="D70" s="21" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="n">
@@ -2866,7 +2852,7 @@
         <v>56</v>
       </c>
       <c r="C71" s="24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D71" s="12"/>
     </row>
@@ -2879,7 +2865,7 @@
         <v>56</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D72" s="12"/>
     </row>
@@ -2892,7 +2878,7 @@
         <v>56</v>
       </c>
       <c r="C73" s="24" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D73" s="12"/>
     </row>
@@ -2905,7 +2891,7 @@
         <v>56</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D74" s="12"/>
     </row>
@@ -2918,7 +2904,7 @@
         <v>56</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D75" s="12"/>
     </row>
@@ -2931,7 +2917,7 @@
         <v>56</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D76" s="12"/>
     </row>
@@ -2944,7 +2930,7 @@
         <v>56</v>
       </c>
       <c r="C77" s="24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D77" s="12"/>
     </row>
@@ -2957,7 +2943,7 @@
         <v>56</v>
       </c>
       <c r="C78" s="24" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D78" s="12"/>
     </row>
@@ -2970,7 +2956,7 @@
         <v>56</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D79" s="12"/>
     </row>
@@ -2983,7 +2969,7 @@
         <v>56</v>
       </c>
       <c r="C80" s="24" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D80" s="12"/>
     </row>
@@ -2996,7 +2982,7 @@
         <v>56</v>
       </c>
       <c r="C81" s="24" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D81" s="12"/>
     </row>
@@ -3009,7 +2995,7 @@
         <v>56</v>
       </c>
       <c r="C82" s="24" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D82" s="12"/>
     </row>
@@ -3022,7 +3008,7 @@
         <v>56</v>
       </c>
       <c r="C83" s="24" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D83" s="12"/>
     </row>
@@ -3035,7 +3021,7 @@
         <v>56</v>
       </c>
       <c r="C84" s="24" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D84" s="12"/>
     </row>
@@ -3048,7 +3034,7 @@
         <v>56</v>
       </c>
       <c r="C85" s="24" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D85" s="12"/>
     </row>
@@ -3061,7 +3047,7 @@
         <v>56</v>
       </c>
       <c r="C86" s="24" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D86" s="12"/>
     </row>
@@ -3074,7 +3060,7 @@
         <v>56</v>
       </c>
       <c r="C87" s="24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D87" s="12"/>
     </row>
@@ -3087,7 +3073,7 @@
         <v>56</v>
       </c>
       <c r="C88" s="24" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D88" s="12"/>
     </row>
@@ -3100,7 +3086,7 @@
         <v>56</v>
       </c>
       <c r="C89" s="24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D89" s="12"/>
     </row>
@@ -3113,7 +3099,7 @@
         <v>56</v>
       </c>
       <c r="C90" s="24" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D90" s="12"/>
     </row>
@@ -3126,7 +3112,7 @@
         <v>56</v>
       </c>
       <c r="C91" s="24" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D91" s="12"/>
     </row>
@@ -3139,7 +3125,7 @@
         <v>56</v>
       </c>
       <c r="C92" s="24" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D92" s="12"/>
     </row>
@@ -3152,7 +3138,7 @@
         <v>56</v>
       </c>
       <c r="C93" s="24" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D93" s="12"/>
     </row>
@@ -3165,7 +3151,7 @@
         <v>56</v>
       </c>
       <c r="C94" s="24" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D94" s="12"/>
     </row>
@@ -3175,10 +3161,10 @@
         <v>90</v>
       </c>
       <c r="B95" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C95" s="24" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D95" s="12"/>
     </row>
@@ -3188,10 +3174,10 @@
         <v>91</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C96" s="24" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D96" s="12"/>
     </row>
@@ -3201,10 +3187,10 @@
         <v>92</v>
       </c>
       <c r="B97" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C97" s="24" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D97" s="12"/>
     </row>
@@ -3214,10 +3200,10 @@
         <v>93</v>
       </c>
       <c r="B98" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C98" s="24" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D98" s="12"/>
     </row>
@@ -3227,10 +3213,10 @@
         <v>94</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C99" s="24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D99" s="12"/>
     </row>
@@ -3240,10 +3226,10 @@
         <v>95</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C100" s="24" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D100" s="12"/>
     </row>
@@ -3253,10 +3239,10 @@
         <v>96</v>
       </c>
       <c r="B101" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C101" s="24" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D101" s="12"/>
     </row>
@@ -3266,10 +3252,10 @@
         <v>97</v>
       </c>
       <c r="B102" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C102" s="24" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D102" s="12"/>
     </row>
@@ -3279,10 +3265,10 @@
         <v>98</v>
       </c>
       <c r="B103" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C103" s="24" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D103" s="12"/>
     </row>
@@ -3292,10 +3278,10 @@
         <v>99</v>
       </c>
       <c r="B104" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C104" s="24" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D104" s="12"/>
     </row>
@@ -3305,10 +3291,10 @@
         <v>100</v>
       </c>
       <c r="B105" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C105" s="24" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D105" s="12"/>
     </row>
@@ -3318,10 +3304,10 @@
         <v>101</v>
       </c>
       <c r="B106" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C106" s="24" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D106" s="12"/>
     </row>
@@ -3331,10 +3317,10 @@
         <v>102</v>
       </c>
       <c r="B107" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C107" s="24" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D107" s="12"/>
     </row>
@@ -3344,10 +3330,10 @@
         <v>103</v>
       </c>
       <c r="B108" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C108" s="24" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D108" s="12"/>
     </row>
@@ -3357,10 +3343,10 @@
         <v>104</v>
       </c>
       <c r="B109" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C109" s="24" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D109" s="12"/>
     </row>
@@ -3370,10 +3356,10 @@
         <v>105</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C110" s="24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D110" s="12"/>
     </row>
@@ -3383,10 +3369,10 @@
         <v>106</v>
       </c>
       <c r="B111" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C111" s="24" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D111" s="12"/>
     </row>
@@ -3396,10 +3382,10 @@
         <v>107</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C112" s="24" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D112" s="12"/>
     </row>
@@ -3409,10 +3395,10 @@
         <v>108</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C113" s="24" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D113" s="12"/>
     </row>
@@ -3422,10 +3408,10 @@
         <v>109</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C114" s="24" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D114" s="12"/>
     </row>
@@ -3435,10 +3421,10 @@
         <v>110</v>
       </c>
       <c r="B115" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C115" s="24" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D115" s="12"/>
     </row>
@@ -3448,10 +3434,10 @@
         <v>111</v>
       </c>
       <c r="B116" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C116" s="24" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D116" s="12"/>
     </row>
@@ -3461,10 +3447,10 @@
         <v>112</v>
       </c>
       <c r="B117" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C117" s="24" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D117" s="12"/>
     </row>
@@ -3474,10 +3460,10 @@
         <v>113</v>
       </c>
       <c r="B118" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C118" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D118" s="12"/>
     </row>
@@ -3487,10 +3473,10 @@
         <v>114</v>
       </c>
       <c r="B119" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C119" s="24" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D119" s="12"/>
     </row>
@@ -3500,10 +3486,10 @@
         <v>115</v>
       </c>
       <c r="B120" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C120" s="24" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D120" s="12"/>
     </row>
@@ -3513,10 +3499,10 @@
         <v>116</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C121" s="24" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D121" s="12"/>
     </row>
@@ -3526,10 +3512,10 @@
         <v>117</v>
       </c>
       <c r="B122" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C122" s="24" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D122" s="12"/>
     </row>
@@ -3539,10 +3525,10 @@
         <v>118</v>
       </c>
       <c r="B123" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C123" s="24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D123" s="12"/>
     </row>
@@ -3552,10 +3538,10 @@
         <v>119</v>
       </c>
       <c r="B124" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C124" s="24" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D124" s="12"/>
     </row>
@@ -3565,10 +3551,10 @@
         <v>120</v>
       </c>
       <c r="B125" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C125" s="24" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D125" s="12"/>
     </row>
@@ -3578,10 +3564,10 @@
         <v>121</v>
       </c>
       <c r="B126" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C126" s="24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D126" s="12"/>
     </row>
@@ -3591,10 +3577,10 @@
         <v>122</v>
       </c>
       <c r="B127" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C127" s="24" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D127" s="12"/>
     </row>
@@ -3604,10 +3590,10 @@
         <v>123</v>
       </c>
       <c r="B128" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C128" s="24" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D128" s="12"/>
     </row>
@@ -3617,10 +3603,10 @@
         <v>124</v>
       </c>
       <c r="B129" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C129" s="24" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D129" s="12"/>
     </row>
@@ -3630,10 +3616,10 @@
         <v>125</v>
       </c>
       <c r="B130" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C130" s="24" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D130" s="12"/>
     </row>
@@ -3643,10 +3629,10 @@
         <v>126</v>
       </c>
       <c r="B131" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C131" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D131" s="12"/>
     </row>
@@ -3656,10 +3642,10 @@
         <v>127</v>
       </c>
       <c r="B132" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C132" s="24" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D132" s="12"/>
     </row>
@@ -3669,10 +3655,10 @@
         <v>128</v>
       </c>
       <c r="B133" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C133" s="24" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D133" s="12"/>
     </row>
@@ -3682,10 +3668,10 @@
         <v>129</v>
       </c>
       <c r="B134" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C134" s="24" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D134" s="12"/>
     </row>
@@ -3695,10 +3681,10 @@
         <v>130</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C135" s="24" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D135" s="12"/>
     </row>
@@ -3708,10 +3694,10 @@
         <v>131</v>
       </c>
       <c r="B136" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C136" s="24" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D136" s="12"/>
     </row>
@@ -3721,10 +3707,10 @@
         <v>132</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C137" s="24" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D137" s="12"/>
     </row>
@@ -3734,10 +3720,10 @@
         <v>133</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C138" s="24" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D138" s="12"/>
     </row>
@@ -3747,10 +3733,10 @@
         <v>134</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C139" s="24" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D139" s="12"/>
     </row>
@@ -3760,10 +3746,10 @@
         <v>135</v>
       </c>
       <c r="B140" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C140" s="24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D140" s="12"/>
     </row>
@@ -3773,10 +3759,10 @@
         <v>136</v>
       </c>
       <c r="B141" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C141" s="24" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D141" s="12"/>
     </row>
@@ -3786,10 +3772,10 @@
         <v>137</v>
       </c>
       <c r="B142" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C142" s="24" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D142" s="12"/>
     </row>
@@ -3799,10 +3785,10 @@
         <v>138</v>
       </c>
       <c r="B143" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C143" s="24" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D143" s="12"/>
     </row>
@@ -3812,10 +3798,10 @@
         <v>139</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C144" s="24" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D144" s="12"/>
     </row>
@@ -3825,10 +3811,10 @@
         <v>140</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C145" s="24" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D145" s="12"/>
     </row>
@@ -3838,10 +3824,10 @@
         <v>141</v>
       </c>
       <c r="B146" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C146" s="24" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D146" s="12"/>
     </row>
@@ -3851,10 +3837,10 @@
         <v>142</v>
       </c>
       <c r="B147" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C147" s="24" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D147" s="12"/>
     </row>
@@ -3864,10 +3850,10 @@
         <v>143</v>
       </c>
       <c r="B148" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C148" s="24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D148" s="12"/>
     </row>
@@ -3877,10 +3863,10 @@
         <v>144</v>
       </c>
       <c r="B149" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C149" s="24" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D149" s="12"/>
     </row>
@@ -3890,10 +3876,10 @@
         <v>145</v>
       </c>
       <c r="B150" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C150" s="24" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D150" s="12"/>
     </row>
@@ -3903,10 +3889,10 @@
         <v>146</v>
       </c>
       <c r="B151" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C151" s="24" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D151" s="12"/>
     </row>
@@ -3916,10 +3902,10 @@
         <v>147</v>
       </c>
       <c r="B152" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C152" s="24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D152" s="12"/>
     </row>
@@ -3929,10 +3915,10 @@
         <v>148</v>
       </c>
       <c r="B153" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C153" s="24" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D153" s="12"/>
     </row>
@@ -3942,10 +3928,10 @@
         <v>149</v>
       </c>
       <c r="B154" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C154" s="24" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D154" s="12"/>
     </row>
@@ -3955,10 +3941,10 @@
         <v>150</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C155" s="24" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D155" s="12"/>
     </row>
@@ -3968,10 +3954,10 @@
         <v>151</v>
       </c>
       <c r="B156" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C156" s="25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D156" s="12"/>
     </row>
@@ -3981,10 +3967,10 @@
         <v>152</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C157" s="25" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D157" s="12"/>
     </row>
@@ -3994,10 +3980,10 @@
         <v>153</v>
       </c>
       <c r="B158" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C158" s="24" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D158" s="12"/>
     </row>
@@ -4007,10 +3993,10 @@
         <v>154</v>
       </c>
       <c r="B159" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C159" s="24" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D159" s="12"/>
     </row>
@@ -4020,10 +4006,10 @@
         <v>155</v>
       </c>
       <c r="B160" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C160" s="24" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D160" s="12"/>
     </row>
@@ -4033,10 +4019,10 @@
         <v>156</v>
       </c>
       <c r="B161" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C161" s="24" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D161" s="12"/>
     </row>
@@ -4046,10 +4032,10 @@
         <v>157</v>
       </c>
       <c r="B162" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C162" s="24" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D162" s="12"/>
     </row>
@@ -4059,10 +4045,10 @@
         <v>158</v>
       </c>
       <c r="B163" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C163" s="24" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D163" s="12"/>
     </row>
@@ -4072,10 +4058,10 @@
         <v>159</v>
       </c>
       <c r="B164" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C164" s="24" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D164" s="12"/>
     </row>
@@ -4085,10 +4071,10 @@
         <v>160</v>
       </c>
       <c r="B165" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C165" s="24" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D165" s="12"/>
     </row>
@@ -4098,10 +4084,10 @@
         <v>161</v>
       </c>
       <c r="B166" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C166" s="24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D166" s="12"/>
     </row>
@@ -4111,10 +4097,10 @@
         <v>162</v>
       </c>
       <c r="B167" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C167" s="24" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D167" s="12"/>
     </row>
@@ -4124,10 +4110,10 @@
         <v>163</v>
       </c>
       <c r="B168" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C168" s="24" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D168" s="12"/>
     </row>
@@ -4137,10 +4123,10 @@
         <v>164</v>
       </c>
       <c r="B169" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C169" s="24" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D169" s="12"/>
     </row>
@@ -4150,10 +4136,10 @@
         <v>165</v>
       </c>
       <c r="B170" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C170" s="24" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D170" s="12"/>
     </row>
@@ -4163,10 +4149,10 @@
         <v>166</v>
       </c>
       <c r="B171" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C171" s="24" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D171" s="12"/>
     </row>
@@ -4176,10 +4162,10 @@
         <v>167</v>
       </c>
       <c r="B172" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C172" s="24" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D172" s="12"/>
     </row>
@@ -4189,10 +4175,10 @@
         <v>168</v>
       </c>
       <c r="B173" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C173" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D173" s="12"/>
     </row>
@@ -4202,10 +4188,10 @@
         <v>169</v>
       </c>
       <c r="B174" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C174" s="24" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D174" s="12"/>
     </row>
@@ -4215,10 +4201,10 @@
         <v>170</v>
       </c>
       <c r="B175" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C175" s="24" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D175" s="12"/>
     </row>
@@ -4228,10 +4214,10 @@
         <v>171</v>
       </c>
       <c r="B176" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C176" s="24" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D176" s="12"/>
     </row>
@@ -4241,10 +4227,10 @@
         <v>172</v>
       </c>
       <c r="B177" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C177" s="24" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D177" s="12"/>
     </row>
@@ -4254,10 +4240,10 @@
         <v>173</v>
       </c>
       <c r="B178" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C178" s="24" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D178" s="12"/>
     </row>
@@ -4267,10 +4253,10 @@
         <v>174</v>
       </c>
       <c r="B179" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C179" s="24" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D179" s="12"/>
     </row>
@@ -4280,10 +4266,10 @@
         <v>175</v>
       </c>
       <c r="B180" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C180" s="24" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D180" s="12"/>
     </row>
@@ -4293,10 +4279,10 @@
         <v>176</v>
       </c>
       <c r="B181" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C181" s="24" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D181" s="12"/>
     </row>
@@ -4306,10 +4292,10 @@
         <v>177</v>
       </c>
       <c r="B182" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C182" s="24" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D182" s="12"/>
     </row>
@@ -4319,10 +4305,10 @@
         <v>178</v>
       </c>
       <c r="B183" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C183" s="24" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D183" s="12"/>
     </row>
@@ -4332,10 +4318,10 @@
         <v>179</v>
       </c>
       <c r="B184" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C184" s="24" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D184" s="12"/>
     </row>
@@ -4345,10 +4331,10 @@
         <v>180</v>
       </c>
       <c r="B185" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C185" s="24" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D185" s="12"/>
     </row>
@@ -4358,10 +4344,10 @@
         <v>181</v>
       </c>
       <c r="B186" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C186" s="24" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D186" s="12"/>
     </row>
@@ -4371,10 +4357,10 @@
         <v>182</v>
       </c>
       <c r="B187" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C187" s="24" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D187" s="12"/>
     </row>
@@ -4384,10 +4370,10 @@
         <v>183</v>
       </c>
       <c r="B188" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C188" s="24" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D188" s="12"/>
     </row>
@@ -4397,10 +4383,10 @@
         <v>184</v>
       </c>
       <c r="B189" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C189" s="24" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D189" s="12"/>
     </row>
@@ -4410,10 +4396,10 @@
         <v>185</v>
       </c>
       <c r="B190" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C190" s="24" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D190" s="12"/>
     </row>
@@ -4423,10 +4409,10 @@
         <v>186</v>
       </c>
       <c r="B191" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C191" s="24" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D191" s="12"/>
     </row>
@@ -4436,10 +4422,10 @@
         <v>187</v>
       </c>
       <c r="B192" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C192" s="24" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D192" s="12"/>
     </row>
@@ -4449,10 +4435,10 @@
         <v>188</v>
       </c>
       <c r="B193" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C193" s="24" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D193" s="12"/>
     </row>
@@ -4462,10 +4448,10 @@
         <v>189</v>
       </c>
       <c r="B194" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C194" s="24" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D194" s="12"/>
     </row>
@@ -4475,10 +4461,10 @@
         <v>190</v>
       </c>
       <c r="B195" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C195" s="24" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D195" s="12"/>
     </row>
@@ -4488,10 +4474,10 @@
         <v>191</v>
       </c>
       <c r="B196" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C196" s="24" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D196" s="12"/>
     </row>
@@ -4501,10 +4487,10 @@
         <v>192</v>
       </c>
       <c r="B197" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C197" s="24" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D197" s="12"/>
     </row>
@@ -4514,10 +4500,10 @@
         <v>193</v>
       </c>
       <c r="B198" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C198" s="24" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D198" s="12"/>
     </row>
@@ -4527,10 +4513,10 @@
         <v>194</v>
       </c>
       <c r="B199" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C199" s="24" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D199" s="12"/>
     </row>
@@ -4540,10 +4526,10 @@
         <v>195</v>
       </c>
       <c r="B200" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C200" s="24" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D200" s="12"/>
     </row>
@@ -4553,10 +4539,10 @@
         <v>196</v>
       </c>
       <c r="B201" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C201" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D201" s="12"/>
     </row>
@@ -4566,10 +4552,10 @@
         <v>197</v>
       </c>
       <c r="B202" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C202" s="24" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4578,10 +4564,10 @@
         <v>198</v>
       </c>
       <c r="B203" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C203" s="24" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4590,10 +4576,10 @@
         <v>199</v>
       </c>
       <c r="B204" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C204" s="24" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4602,10 +4588,10 @@
         <v>200</v>
       </c>
       <c r="B205" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C205" s="24" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4614,10 +4600,10 @@
         <v>201</v>
       </c>
       <c r="B206" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C206" s="24" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4626,10 +4612,10 @@
         <v>202</v>
       </c>
       <c r="B207" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C207" s="24" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4638,10 +4624,10 @@
         <v>203</v>
       </c>
       <c r="B208" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C208" s="26" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4650,10 +4636,10 @@
         <v>204</v>
       </c>
       <c r="B209" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C209" s="24" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4662,10 +4648,10 @@
         <v>205</v>
       </c>
       <c r="B210" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C210" s="24" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D210" s="12"/>
     </row>
@@ -4675,10 +4661,10 @@
         <v>206</v>
       </c>
       <c r="B211" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C211" s="24" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D211" s="12"/>
     </row>
@@ -4688,10 +4674,10 @@
         <v>207</v>
       </c>
       <c r="B212" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C212" s="24" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D212" s="12"/>
     </row>
@@ -4701,10 +4687,10 @@
         <v>208</v>
       </c>
       <c r="B213" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C213" s="24" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D213" s="12"/>
     </row>
@@ -4714,10 +4700,10 @@
         <v>209</v>
       </c>
       <c r="B214" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C214" s="24" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D214" s="12"/>
     </row>
@@ -4727,10 +4713,10 @@
         <v>210</v>
       </c>
       <c r="B215" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C215" s="24" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D215" s="12"/>
     </row>
@@ -4740,10 +4726,10 @@
         <v>211</v>
       </c>
       <c r="B216" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C216" s="24" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D216" s="12"/>
     </row>
@@ -4753,10 +4739,10 @@
         <v>212</v>
       </c>
       <c r="B217" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C217" s="24" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D217" s="12"/>
     </row>
@@ -4766,10 +4752,10 @@
         <v>213</v>
       </c>
       <c r="B218" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C218" s="24" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D218" s="12"/>
     </row>
@@ -4779,10 +4765,10 @@
         <v>214</v>
       </c>
       <c r="B219" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C219" s="24" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D219" s="12"/>
     </row>
@@ -4792,10 +4778,10 @@
         <v>215</v>
       </c>
       <c r="B220" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C220" s="24" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D220" s="12"/>
     </row>
@@ -4805,10 +4791,10 @@
         <v>216</v>
       </c>
       <c r="B221" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C221" s="24" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D221" s="12"/>
     </row>
@@ -4818,10 +4804,10 @@
         <v>217</v>
       </c>
       <c r="B222" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C222" s="24" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D222" s="12"/>
     </row>
@@ -4831,10 +4817,10 @@
         <v>218</v>
       </c>
       <c r="B223" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C223" s="24" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D223" s="12"/>
     </row>
@@ -4844,10 +4830,10 @@
         <v>219</v>
       </c>
       <c r="B224" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C224" s="24" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D224" s="12"/>
     </row>
@@ -4857,10 +4843,10 @@
         <v>220</v>
       </c>
       <c r="B225" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C225" s="24" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D225" s="12"/>
     </row>
@@ -4870,10 +4856,10 @@
         <v>221</v>
       </c>
       <c r="B226" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C226" s="24" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D226" s="12"/>
     </row>
@@ -4883,10 +4869,10 @@
         <v>222</v>
       </c>
       <c r="B227" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C227" s="24" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D227" s="12"/>
     </row>
@@ -4896,10 +4882,10 @@
         <v>223</v>
       </c>
       <c r="B228" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C228" s="24" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D228" s="12"/>
     </row>
@@ -4909,10 +4895,10 @@
         <v>224</v>
       </c>
       <c r="B229" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C229" s="24" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D229" s="12"/>
     </row>
@@ -4922,10 +4908,10 @@
         <v>225</v>
       </c>
       <c r="B230" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C230" s="24" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D230" s="12"/>
     </row>
@@ -4935,10 +4921,10 @@
         <v>226</v>
       </c>
       <c r="B231" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C231" s="24" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D231" s="12"/>
     </row>
@@ -4948,10 +4934,10 @@
         <v>227</v>
       </c>
       <c r="B232" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C232" s="24" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D232" s="12"/>
     </row>
@@ -4961,10 +4947,10 @@
         <v>228</v>
       </c>
       <c r="B233" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C233" s="24" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D233" s="12"/>
     </row>
@@ -4974,10 +4960,10 @@
         <v>229</v>
       </c>
       <c r="B234" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C234" s="24" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D234" s="12"/>
     </row>
@@ -4987,10 +4973,10 @@
         <v>230</v>
       </c>
       <c r="B235" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C235" s="24" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D235" s="12"/>
     </row>
@@ -5000,10 +4986,10 @@
         <v>231</v>
       </c>
       <c r="B236" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C236" s="24" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D236" s="12"/>
     </row>
@@ -5013,10 +4999,10 @@
         <v>232</v>
       </c>
       <c r="B237" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C237" s="24" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D237" s="12"/>
     </row>
@@ -5026,10 +5012,10 @@
         <v>233</v>
       </c>
       <c r="B238" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C238" s="24" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D238" s="12"/>
     </row>
@@ -5039,10 +5025,10 @@
         <v>234</v>
       </c>
       <c r="B239" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C239" s="24" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D239" s="12"/>
     </row>
@@ -5052,10 +5038,10 @@
         <v>235</v>
       </c>
       <c r="B240" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C240" s="24" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D240" s="12"/>
     </row>
@@ -5065,10 +5051,10 @@
         <v>236</v>
       </c>
       <c r="B241" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C241" s="24" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D241" s="12"/>
     </row>
@@ -5078,10 +5064,10 @@
         <v>237</v>
       </c>
       <c r="B242" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C242" s="24" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D242" s="12"/>
     </row>
@@ -5091,10 +5077,10 @@
         <v>238</v>
       </c>
       <c r="B243" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C243" s="24" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D243" s="12"/>
     </row>
@@ -5104,10 +5090,10 @@
         <v>239</v>
       </c>
       <c r="B244" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C244" s="24" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D244" s="12"/>
     </row>
@@ -5117,10 +5103,10 @@
         <v>240</v>
       </c>
       <c r="B245" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C245" s="24" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D245" s="12"/>
     </row>
@@ -5130,10 +5116,10 @@
         <v>241</v>
       </c>
       <c r="B246" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C246" s="24" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D246" s="12"/>
     </row>
@@ -5143,10 +5129,10 @@
         <v>242</v>
       </c>
       <c r="B247" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C247" s="24" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D247" s="12"/>
     </row>
@@ -5156,10 +5142,10 @@
         <v>243</v>
       </c>
       <c r="B248" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C248" s="24" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D248" s="12"/>
     </row>
@@ -5169,10 +5155,10 @@
         <v>244</v>
       </c>
       <c r="B249" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C249" s="24" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D249" s="12"/>
     </row>
@@ -5182,10 +5168,10 @@
         <v>245</v>
       </c>
       <c r="B250" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C250" s="24" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D250" s="12"/>
     </row>
@@ -5195,10 +5181,10 @@
         <v>246</v>
       </c>
       <c r="B251" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C251" s="24" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D251" s="12"/>
     </row>
@@ -5208,10 +5194,10 @@
         <v>247</v>
       </c>
       <c r="B252" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C252" s="24" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D252" s="12"/>
     </row>
@@ -5221,10 +5207,10 @@
         <v>248</v>
       </c>
       <c r="B253" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C253" s="24" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D253" s="12"/>
     </row>
@@ -5234,10 +5220,10 @@
         <v>249</v>
       </c>
       <c r="B254" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C254" s="24" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D254" s="12"/>
     </row>
@@ -5247,10 +5233,10 @@
         <v>250</v>
       </c>
       <c r="B255" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C255" s="24" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D255" s="12"/>
     </row>
@@ -5260,10 +5246,10 @@
         <v>251</v>
       </c>
       <c r="B256" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C256" s="24" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D256" s="12"/>
     </row>
@@ -5273,10 +5259,10 @@
         <v>252</v>
       </c>
       <c r="B257" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C257" s="24" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D257" s="12"/>
     </row>
@@ -5286,10 +5272,10 @@
         <v>253</v>
       </c>
       <c r="B258" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C258" s="24" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D258" s="12"/>
     </row>
@@ -5299,10 +5285,10 @@
         <v>254</v>
       </c>
       <c r="B259" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C259" s="24" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D259" s="12"/>
     </row>
@@ -5312,10 +5298,10 @@
         <v>255</v>
       </c>
       <c r="B260" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C260" s="24" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D260" s="12"/>
     </row>
@@ -5325,10 +5311,10 @@
         <v>256</v>
       </c>
       <c r="B261" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C261" s="24" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D261" s="12"/>
     </row>
@@ -5338,10 +5324,10 @@
         <v>257</v>
       </c>
       <c r="B262" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C262" s="24" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D262" s="12"/>
     </row>
@@ -5351,10 +5337,10 @@
         <v>258</v>
       </c>
       <c r="B263" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C263" s="24" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D263" s="12"/>
     </row>
@@ -5364,10 +5350,10 @@
         <v>259</v>
       </c>
       <c r="B264" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C264" s="24" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D264" s="12"/>
     </row>
@@ -5377,10 +5363,10 @@
         <v>260</v>
       </c>
       <c r="B265" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C265" s="24" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D265" s="12"/>
     </row>
@@ -5390,10 +5376,10 @@
         <v>261</v>
       </c>
       <c r="B266" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C266" s="24" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D266" s="12"/>
     </row>
@@ -5403,10 +5389,10 @@
         <v>262</v>
       </c>
       <c r="B267" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C267" s="24" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D267" s="12"/>
     </row>
@@ -5416,10 +5402,10 @@
         <v>263</v>
       </c>
       <c r="B268" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C268" s="24" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D268" s="12"/>
     </row>
@@ -5429,10 +5415,10 @@
         <v>264</v>
       </c>
       <c r="B269" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C269" s="24" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D269" s="12"/>
     </row>
@@ -5442,10 +5428,10 @@
         <v>265</v>
       </c>
       <c r="B270" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C270" s="24" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D270" s="12"/>
     </row>
@@ -5455,10 +5441,10 @@
         <v>266</v>
       </c>
       <c r="B271" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C271" s="24" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D271" s="12"/>
     </row>
@@ -5468,10 +5454,10 @@
         <v>267</v>
       </c>
       <c r="B272" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C272" s="24" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D272" s="12"/>
     </row>
@@ -5481,10 +5467,10 @@
         <v>268</v>
       </c>
       <c r="B273" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C273" s="24" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D273" s="12"/>
     </row>
@@ -5494,10 +5480,10 @@
         <v>269</v>
       </c>
       <c r="B274" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C274" s="24" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D274" s="12"/>
     </row>
@@ -5507,10 +5493,10 @@
         <v>270</v>
       </c>
       <c r="B275" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C275" s="24" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D275" s="12"/>
     </row>
@@ -5520,10 +5506,10 @@
         <v>271</v>
       </c>
       <c r="B276" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C276" s="24" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D276" s="12"/>
     </row>
@@ -5533,10 +5519,10 @@
         <v>272</v>
       </c>
       <c r="B277" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C277" s="24" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D277" s="12"/>
     </row>
@@ -5546,10 +5532,10 @@
         <v>273</v>
       </c>
       <c r="B278" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C278" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D278" s="12"/>
     </row>
@@ -5559,10 +5545,10 @@
         <v>274</v>
       </c>
       <c r="B279" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C279" s="24" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D279" s="12"/>
     </row>
@@ -5572,10 +5558,10 @@
         <v>275</v>
       </c>
       <c r="B280" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C280" s="24" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D280" s="12"/>
     </row>
@@ -5585,10 +5571,10 @@
         <v>276</v>
       </c>
       <c r="B281" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C281" s="24" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D281" s="12"/>
     </row>
@@ -5598,10 +5584,10 @@
         <v>277</v>
       </c>
       <c r="B282" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C282" s="24" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D282" s="12"/>
     </row>
@@ -5611,10 +5597,10 @@
         <v>278</v>
       </c>
       <c r="B283" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C283" s="24" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D283" s="12"/>
     </row>
@@ -5624,10 +5610,10 @@
         <v>279</v>
       </c>
       <c r="B284" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C284" s="24" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D284" s="12"/>
     </row>
@@ -5637,10 +5623,10 @@
         <v>280</v>
       </c>
       <c r="B285" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C285" s="24" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D285" s="12"/>
     </row>
@@ -5650,10 +5636,10 @@
         <v>281</v>
       </c>
       <c r="B286" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C286" s="24" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D286" s="12"/>
     </row>
@@ -5663,10 +5649,10 @@
         <v>282</v>
       </c>
       <c r="B287" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C287" s="24" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D287" s="12"/>
     </row>
@@ -5676,10 +5662,10 @@
         <v>283</v>
       </c>
       <c r="B288" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C288" s="24" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D288" s="12"/>
     </row>
@@ -5689,10 +5675,10 @@
         <v>284</v>
       </c>
       <c r="B289" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C289" s="24" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D289" s="12"/>
     </row>
@@ -5702,10 +5688,10 @@
         <v>285</v>
       </c>
       <c r="B290" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C290" s="24" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D290" s="12"/>
     </row>
@@ -5715,10 +5701,10 @@
         <v>286</v>
       </c>
       <c r="B291" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C291" s="26" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D291" s="12"/>
     </row>
@@ -5728,10 +5714,10 @@
         <v>287</v>
       </c>
       <c r="B292" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C292" s="24" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D292" s="12"/>
     </row>
@@ -5741,10 +5727,10 @@
         <v>288</v>
       </c>
       <c r="B293" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C293" s="24" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D293" s="12"/>
     </row>
@@ -5754,10 +5740,10 @@
         <v>289</v>
       </c>
       <c r="B294" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C294" s="24" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D294" s="12"/>
     </row>
@@ -5767,10 +5753,10 @@
         <v>290</v>
       </c>
       <c r="B295" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C295" s="24" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D295" s="12"/>
     </row>
@@ -5780,10 +5766,10 @@
         <v>291</v>
       </c>
       <c r="B296" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C296" s="24" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D296" s="12"/>
     </row>
@@ -5793,10 +5779,10 @@
         <v>292</v>
       </c>
       <c r="B297" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C297" s="24" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D297" s="12"/>
     </row>
@@ -5806,10 +5792,10 @@
         <v>293</v>
       </c>
       <c r="B298" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C298" s="24" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D298" s="12"/>
     </row>
@@ -5819,10 +5805,10 @@
         <v>294</v>
       </c>
       <c r="B299" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C299" s="24" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D299" s="12"/>
     </row>
@@ -5832,10 +5818,10 @@
         <v>295</v>
       </c>
       <c r="B300" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C300" s="24" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D300" s="12"/>
     </row>
@@ -5845,10 +5831,10 @@
         <v>296</v>
       </c>
       <c r="B301" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C301" s="24" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D301" s="12"/>
     </row>
@@ -5858,10 +5844,10 @@
         <v>297</v>
       </c>
       <c r="B302" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C302" s="24" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D302" s="12"/>
     </row>
@@ -5871,10 +5857,10 @@
         <v>298</v>
       </c>
       <c r="B303" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C303" s="24" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D303" s="12"/>
     </row>
@@ -5884,10 +5870,10 @@
         <v>299</v>
       </c>
       <c r="B304" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C304" s="24" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D304" s="12"/>
     </row>
@@ -5897,10 +5883,10 @@
         <v>300</v>
       </c>
       <c r="B305" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C305" s="24" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D305" s="12"/>
     </row>
@@ -5910,10 +5896,10 @@
         <v>301</v>
       </c>
       <c r="B306" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C306" s="24" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D306" s="12"/>
     </row>
@@ -5923,10 +5909,10 @@
         <v>302</v>
       </c>
       <c r="B307" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C307" s="24" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D307" s="12"/>
     </row>
@@ -5936,10 +5922,10 @@
         <v>303</v>
       </c>
       <c r="B308" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C308" s="24" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D308" s="12"/>
     </row>
@@ -5949,10 +5935,10 @@
         <v>304</v>
       </c>
       <c r="B309" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C309" s="24" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D309" s="12"/>
     </row>
@@ -5962,10 +5948,10 @@
         <v>305</v>
       </c>
       <c r="B310" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C310" s="24" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D310" s="12"/>
     </row>
@@ -5975,10 +5961,10 @@
         <v>306</v>
       </c>
       <c r="B311" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C311" s="24" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D311" s="12"/>
     </row>
@@ -5988,10 +5974,10 @@
         <v>307</v>
       </c>
       <c r="B312" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C312" s="24" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D312" s="12"/>
     </row>
@@ -6001,10 +5987,10 @@
         <v>308</v>
       </c>
       <c r="B313" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C313" s="24" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D313" s="12"/>
     </row>
@@ -6014,10 +6000,10 @@
         <v>309</v>
       </c>
       <c r="B314" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C314" s="24" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D314" s="12"/>
     </row>
@@ -6027,10 +6013,10 @@
         <v>310</v>
       </c>
       <c r="B315" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C315" s="24" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D315" s="12"/>
     </row>
@@ -6040,10 +6026,10 @@
         <v>311</v>
       </c>
       <c r="B316" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C316" s="24" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D316" s="12"/>
     </row>
@@ -6053,10 +6039,10 @@
         <v>312</v>
       </c>
       <c r="B317" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C317" s="24" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D317" s="12"/>
     </row>
@@ -6066,10 +6052,10 @@
         <v>313</v>
       </c>
       <c r="B318" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C318" s="24" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D318" s="12"/>
     </row>
@@ -6079,10 +6065,10 @@
         <v>314</v>
       </c>
       <c r="B319" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C319" s="24" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D319" s="12"/>
     </row>
@@ -6092,10 +6078,10 @@
         <v>315</v>
       </c>
       <c r="B320" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C320" s="24" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D320" s="12"/>
     </row>
@@ -6105,10 +6091,10 @@
         <v>316</v>
       </c>
       <c r="B321" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C321" s="24" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D321" s="12"/>
     </row>
@@ -6118,10 +6104,10 @@
         <v>317</v>
       </c>
       <c r="B322" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C322" s="24" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D322" s="12"/>
     </row>
@@ -6131,10 +6117,10 @@
         <v>318</v>
       </c>
       <c r="B323" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C323" s="24" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D323" s="12"/>
     </row>
@@ -6144,10 +6130,10 @@
         <v>319</v>
       </c>
       <c r="B324" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C324" s="26" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D324" s="12"/>
     </row>
@@ -6157,10 +6143,10 @@
         <v>320</v>
       </c>
       <c r="B325" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C325" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D325" s="12"/>
     </row>
@@ -6170,10 +6156,10 @@
         <v>321</v>
       </c>
       <c r="B326" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C326" s="24" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D326" s="12"/>
     </row>
@@ -6183,10 +6169,10 @@
         <v>322</v>
       </c>
       <c r="B327" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C327" s="24" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D327" s="12"/>
     </row>
@@ -6196,10 +6182,10 @@
         <v>323</v>
       </c>
       <c r="B328" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C328" s="24" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D328" s="12"/>
     </row>
@@ -6209,10 +6195,10 @@
         <v>324</v>
       </c>
       <c r="B329" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C329" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D329" s="12"/>
     </row>
@@ -6222,10 +6208,10 @@
         <v>325</v>
       </c>
       <c r="B330" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C330" s="24" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D330" s="12"/>
     </row>
@@ -6235,10 +6221,10 @@
         <v>326</v>
       </c>
       <c r="B331" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C331" s="24" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D331" s="12"/>
     </row>
@@ -6248,10 +6234,10 @@
         <v>327</v>
       </c>
       <c r="B332" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C332" s="24" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D332" s="12"/>
     </row>
@@ -6261,10 +6247,10 @@
         <v>328</v>
       </c>
       <c r="B333" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C333" s="24" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D333" s="12"/>
     </row>
@@ -6274,10 +6260,10 @@
         <v>329</v>
       </c>
       <c r="B334" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C334" s="24" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D334" s="12"/>
     </row>
@@ -6287,10 +6273,10 @@
         <v>330</v>
       </c>
       <c r="B335" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C335" s="24" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D335" s="12"/>
     </row>
@@ -6300,10 +6286,10 @@
         <v>331</v>
       </c>
       <c r="B336" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C336" s="24" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D336" s="12"/>
     </row>
@@ -6313,10 +6299,10 @@
         <v>332</v>
       </c>
       <c r="B337" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C337" s="24" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D337" s="12"/>
     </row>
@@ -6326,10 +6312,10 @@
         <v>333</v>
       </c>
       <c r="B338" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C338" s="24" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D338" s="12"/>
     </row>
@@ -6339,10 +6325,10 @@
         <v>334</v>
       </c>
       <c r="B339" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C339" s="24" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D339" s="12"/>
     </row>
@@ -6352,10 +6338,10 @@
         <v>335</v>
       </c>
       <c r="B340" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C340" s="24" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D340" s="12"/>
     </row>
@@ -6365,10 +6351,10 @@
         <v>336</v>
       </c>
       <c r="B341" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C341" s="24" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D341" s="12"/>
     </row>
@@ -6378,10 +6364,10 @@
         <v>337</v>
       </c>
       <c r="B342" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C342" s="24" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D342" s="12"/>
     </row>
@@ -6391,10 +6377,10 @@
         <v>338</v>
       </c>
       <c r="B343" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C343" s="24" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D343" s="12"/>
     </row>
@@ -6404,10 +6390,10 @@
         <v>339</v>
       </c>
       <c r="B344" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C344" s="24" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D344" s="12"/>
     </row>
@@ -6417,10 +6403,10 @@
         <v>340</v>
       </c>
       <c r="B345" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C345" s="24" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D345" s="12"/>
     </row>
@@ -6430,10 +6416,10 @@
         <v>341</v>
       </c>
       <c r="B346" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C346" s="24" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D346" s="12"/>
     </row>
@@ -6443,10 +6429,10 @@
         <v>342</v>
       </c>
       <c r="B347" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C347" s="24" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D347" s="12"/>
     </row>
@@ -6456,10 +6442,10 @@
         <v>343</v>
       </c>
       <c r="B348" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C348" s="24" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D348" s="12"/>
     </row>
@@ -6469,10 +6455,10 @@
         <v>344</v>
       </c>
       <c r="B349" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C349" s="24" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D349" s="12"/>
     </row>
@@ -6482,10 +6468,10 @@
         <v>345</v>
       </c>
       <c r="B350" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C350" s="24" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D350" s="12"/>
     </row>
@@ -6495,10 +6481,10 @@
         <v>346</v>
       </c>
       <c r="B351" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C351" s="24" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D351" s="12"/>
     </row>
@@ -6508,10 +6494,10 @@
         <v>347</v>
       </c>
       <c r="B352" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C352" s="24" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D352" s="12"/>
     </row>
@@ -6521,10 +6507,10 @@
         <v>348</v>
       </c>
       <c r="B353" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C353" s="24" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D353" s="12"/>
     </row>
@@ -6534,10 +6520,10 @@
         <v>349</v>
       </c>
       <c r="B354" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C354" s="24" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D354" s="12"/>
     </row>
@@ -6547,10 +6533,10 @@
         <v>350</v>
       </c>
       <c r="B355" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C355" s="24" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D355" s="12"/>
     </row>
@@ -6560,10 +6546,10 @@
         <v>351</v>
       </c>
       <c r="B356" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C356" s="24" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D356" s="12"/>
     </row>
@@ -6573,10 +6559,10 @@
         <v>352</v>
       </c>
       <c r="B357" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C357" s="24" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D357" s="12"/>
     </row>
@@ -6586,10 +6572,10 @@
         <v>353</v>
       </c>
       <c r="B358" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C358" s="24" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D358" s="12"/>
     </row>
@@ -6599,10 +6585,10 @@
         <v>354</v>
       </c>
       <c r="B359" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C359" s="24" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D359" s="12"/>
     </row>
@@ -6612,10 +6598,10 @@
         <v>355</v>
       </c>
       <c r="B360" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C360" s="24" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D360" s="12"/>
     </row>
@@ -6625,10 +6611,10 @@
         <v>356</v>
       </c>
       <c r="B361" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C361" s="24" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D361" s="12"/>
     </row>
@@ -6638,10 +6624,10 @@
         <v>357</v>
       </c>
       <c r="B362" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C362" s="24" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D362" s="12"/>
     </row>
@@ -6651,10 +6637,10 @@
         <v>358</v>
       </c>
       <c r="B363" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C363" s="24" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D363" s="12"/>
     </row>
@@ -6664,10 +6650,10 @@
         <v>359</v>
       </c>
       <c r="B364" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C364" s="24" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D364" s="12"/>
     </row>
@@ -6677,10 +6663,10 @@
         <v>360</v>
       </c>
       <c r="B365" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C365" s="24" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D365" s="12"/>
     </row>
@@ -6690,10 +6676,10 @@
         <v>361</v>
       </c>
       <c r="B366" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C366" s="24" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D366" s="12"/>
     </row>
@@ -6703,10 +6689,10 @@
         <v>362</v>
       </c>
       <c r="B367" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C367" s="24" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D367" s="12"/>
     </row>
@@ -6716,10 +6702,10 @@
         <v>363</v>
       </c>
       <c r="B368" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C368" s="24" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D368" s="12"/>
     </row>
@@ -6729,10 +6715,10 @@
         <v>364</v>
       </c>
       <c r="B369" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C369" s="24" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D369" s="12"/>
     </row>
@@ -6742,10 +6728,10 @@
         <v>365</v>
       </c>
       <c r="B370" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C370" s="24" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D370" s="12"/>
     </row>
@@ -6755,10 +6741,10 @@
         <v>366</v>
       </c>
       <c r="B371" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C371" s="24" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D371" s="12"/>
     </row>
@@ -6768,10 +6754,10 @@
         <v>367</v>
       </c>
       <c r="B372" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C372" s="24" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D372" s="12"/>
     </row>
@@ -6781,10 +6767,10 @@
         <v>368</v>
       </c>
       <c r="B373" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C373" s="24" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D373" s="12"/>
     </row>
@@ -6794,10 +6780,10 @@
         <v>369</v>
       </c>
       <c r="B374" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C374" s="24" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D374" s="12"/>
     </row>
@@ -6807,10 +6793,10 @@
         <v>370</v>
       </c>
       <c r="B375" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C375" s="24" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D375" s="12"/>
     </row>
@@ -6820,10 +6806,10 @@
         <v>371</v>
       </c>
       <c r="B376" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C376" s="24" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D376" s="12"/>
     </row>
@@ -6833,10 +6819,10 @@
         <v>372</v>
       </c>
       <c r="B377" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C377" s="24" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D377" s="12"/>
     </row>
@@ -6846,10 +6832,10 @@
         <v>373</v>
       </c>
       <c r="B378" s="10" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C378" s="24" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D378" s="12"/>
     </row>
@@ -6859,10 +6845,10 @@
         <v>374</v>
       </c>
       <c r="B379" s="10" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C379" s="24" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D379" s="12"/>
     </row>
@@ -6872,10 +6858,10 @@
         <v>375</v>
       </c>
       <c r="B380" s="10" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C380" s="24" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D380" s="12"/>
     </row>
@@ -6885,10 +6871,10 @@
         <v>376</v>
       </c>
       <c r="B381" s="10" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C381" s="24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D381" s="12"/>
     </row>
@@ -6898,10 +6884,10 @@
         <v>377</v>
       </c>
       <c r="B382" s="10" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C382" s="24" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D382" s="12"/>
     </row>
@@ -6911,10 +6897,10 @@
         <v>378</v>
       </c>
       <c r="B383" s="10" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C383" s="24" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D383" s="12"/>
     </row>
@@ -6924,10 +6910,10 @@
         <v>379</v>
       </c>
       <c r="B384" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C384" s="24" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D384" s="12"/>
     </row>
@@ -6937,10 +6923,10 @@
         <v>380</v>
       </c>
       <c r="B385" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C385" s="24" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D385" s="12"/>
     </row>
@@ -6950,10 +6936,10 @@
         <v>381</v>
       </c>
       <c r="B386" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C386" s="24" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D386" s="12"/>
     </row>
@@ -6963,10 +6949,10 @@
         <v>382</v>
       </c>
       <c r="B387" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C387" s="24" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D387" s="12"/>
     </row>
@@ -6976,10 +6962,10 @@
         <v>383</v>
       </c>
       <c r="B388" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C388" s="24" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D388" s="12"/>
     </row>
@@ -6989,10 +6975,10 @@
         <v>384</v>
       </c>
       <c r="B389" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C389" s="24" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D389" s="12"/>
     </row>
@@ -7002,10 +6988,10 @@
         <v>385</v>
       </c>
       <c r="B390" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C390" s="24" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D390" s="12"/>
     </row>
@@ -7015,10 +7001,10 @@
         <v>386</v>
       </c>
       <c r="B391" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C391" s="24" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D391" s="12"/>
     </row>
@@ -7028,10 +7014,10 @@
         <v>387</v>
       </c>
       <c r="B392" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C392" s="24" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D392" s="12"/>
     </row>
@@ -7041,10 +7027,10 @@
         <v>388</v>
       </c>
       <c r="B393" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C393" s="24" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D393" s="12"/>
     </row>
@@ -7054,10 +7040,10 @@
         <v>389</v>
       </c>
       <c r="B394" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C394" s="24" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D394" s="12"/>
     </row>
@@ -7067,10 +7053,10 @@
         <v>390</v>
       </c>
       <c r="B395" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C395" s="24" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D395" s="12"/>
     </row>
@@ -7080,10 +7066,10 @@
         <v>391</v>
       </c>
       <c r="B396" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C396" s="24" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D396" s="12"/>
     </row>
@@ -7093,10 +7079,10 @@
         <v>392</v>
       </c>
       <c r="B397" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C397" s="24" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D397" s="12"/>
     </row>
@@ -7106,10 +7092,10 @@
         <v>393</v>
       </c>
       <c r="B398" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C398" s="24" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D398" s="12"/>
     </row>
@@ -7119,10 +7105,10 @@
         <v>394</v>
       </c>
       <c r="B399" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C399" s="24" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D399" s="12"/>
     </row>
@@ -7132,10 +7118,10 @@
         <v>395</v>
       </c>
       <c r="B400" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C400" s="24" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D400" s="12"/>
     </row>
@@ -7145,10 +7131,10 @@
         <v>396</v>
       </c>
       <c r="B401" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C401" s="24" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D401" s="12"/>
     </row>
@@ -7158,10 +7144,10 @@
         <v>397</v>
       </c>
       <c r="B402" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C402" s="24" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D402" s="12"/>
     </row>
@@ -7171,10 +7157,10 @@
         <v>398</v>
       </c>
       <c r="B403" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C403" s="24" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D403" s="12"/>
     </row>
@@ -7184,10 +7170,10 @@
         <v>399</v>
       </c>
       <c r="B404" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C404" s="24" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D404" s="12"/>
     </row>
@@ -7197,10 +7183,10 @@
         <v>400</v>
       </c>
       <c r="B405" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C405" s="24" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D405" s="12"/>
     </row>
@@ -7210,10 +7196,10 @@
         <v>401</v>
       </c>
       <c r="B406" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C406" s="24" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D406" s="12"/>
     </row>
@@ -7223,10 +7209,10 @@
         <v>402</v>
       </c>
       <c r="B407" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C407" s="24" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D407" s="12"/>
     </row>
@@ -7236,10 +7222,10 @@
         <v>403</v>
       </c>
       <c r="B408" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C408" s="24" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D408" s="12"/>
     </row>
@@ -7249,10 +7235,10 @@
         <v>404</v>
       </c>
       <c r="B409" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C409" s="24" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D409" s="12"/>
     </row>
@@ -7262,10 +7248,10 @@
         <v>405</v>
       </c>
       <c r="B410" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C410" s="24" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D410" s="12"/>
     </row>
@@ -7275,10 +7261,10 @@
         <v>406</v>
       </c>
       <c r="B411" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C411" s="24" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D411" s="12"/>
     </row>
@@ -7288,10 +7274,10 @@
         <v>407</v>
       </c>
       <c r="B412" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C412" s="24" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D412" s="12"/>
     </row>
@@ -7301,10 +7287,10 @@
         <v>408</v>
       </c>
       <c r="B413" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C413" s="24" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D413" s="12"/>
     </row>
@@ -7314,10 +7300,10 @@
         <v>409</v>
       </c>
       <c r="B414" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C414" s="24" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D414" s="12"/>
     </row>
@@ -7327,10 +7313,10 @@
         <v>410</v>
       </c>
       <c r="B415" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C415" s="24" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D415" s="12"/>
     </row>
@@ -7340,10 +7326,10 @@
         <v>411</v>
       </c>
       <c r="B416" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C416" s="24" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D416" s="12"/>
     </row>
@@ -7353,10 +7339,10 @@
         <v>412</v>
       </c>
       <c r="B417" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C417" s="24" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D417" s="12"/>
     </row>
@@ -7366,10 +7352,10 @@
         <v>413</v>
       </c>
       <c r="B418" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C418" s="24" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D418" s="12"/>
     </row>
@@ -7379,10 +7365,10 @@
         <v>414</v>
       </c>
       <c r="B419" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C419" s="24" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D419" s="12"/>
     </row>
@@ -7392,10 +7378,10 @@
         <v>415</v>
       </c>
       <c r="B420" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C420" s="24" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D420" s="12"/>
     </row>
@@ -7405,10 +7391,10 @@
         <v>416</v>
       </c>
       <c r="B421" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C421" s="24" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D421" s="12"/>
     </row>
@@ -7418,10 +7404,10 @@
         <v>417</v>
       </c>
       <c r="B422" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C422" s="24" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D422" s="12"/>
     </row>
@@ -7431,10 +7417,10 @@
         <v>418</v>
       </c>
       <c r="B423" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C423" s="24" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D423" s="12"/>
     </row>
@@ -7444,10 +7430,10 @@
         <v>419</v>
       </c>
       <c r="B424" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C424" s="24" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D424" s="12"/>
     </row>
@@ -7457,10 +7443,10 @@
         <v>420</v>
       </c>
       <c r="B425" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C425" s="24" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D425" s="12"/>
     </row>
@@ -7470,10 +7456,10 @@
         <v>421</v>
       </c>
       <c r="B426" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C426" s="24" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D426" s="12"/>
     </row>
@@ -7483,10 +7469,10 @@
         <v>422</v>
       </c>
       <c r="B427" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C427" s="24" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D427" s="12"/>
     </row>
@@ -7496,10 +7482,10 @@
         <v>423</v>
       </c>
       <c r="B428" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C428" s="24" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D428" s="12"/>
     </row>
@@ -7509,10 +7495,10 @@
         <v>424</v>
       </c>
       <c r="B429" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C429" s="24" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D429" s="12"/>
     </row>
@@ -7522,10 +7508,10 @@
         <v>425</v>
       </c>
       <c r="B430" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C430" s="24" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D430" s="12"/>
     </row>
@@ -7535,10 +7521,10 @@
         <v>426</v>
       </c>
       <c r="B431" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C431" s="24" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D431" s="12"/>
     </row>
@@ -7548,10 +7534,10 @@
         <v>427</v>
       </c>
       <c r="B432" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C432" s="24" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D432" s="12"/>
     </row>
@@ -7561,10 +7547,10 @@
         <v>428</v>
       </c>
       <c r="B433" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C433" s="24" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D433" s="12"/>
     </row>
@@ -7574,10 +7560,10 @@
         <v>429</v>
       </c>
       <c r="B434" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C434" s="24" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D434" s="12"/>
     </row>
@@ -7587,10 +7573,10 @@
         <v>430</v>
       </c>
       <c r="B435" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C435" s="24" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D435" s="12"/>
     </row>
@@ -7600,10 +7586,10 @@
         <v>431</v>
       </c>
       <c r="B436" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C436" s="24" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D436" s="12"/>
     </row>
@@ -7613,10 +7599,10 @@
         <v>432</v>
       </c>
       <c r="B437" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C437" s="24" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D437" s="12"/>
     </row>
@@ -7626,10 +7612,10 @@
         <v>433</v>
       </c>
       <c r="B438" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C438" s="24" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D438" s="12"/>
     </row>
@@ -7639,10 +7625,10 @@
         <v>434</v>
       </c>
       <c r="B439" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C439" s="24" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D439" s="12"/>
     </row>
@@ -7652,10 +7638,10 @@
         <v>435</v>
       </c>
       <c r="B440" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C440" s="24" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D440" s="12"/>
     </row>
@@ -7665,10 +7651,10 @@
         <v>436</v>
       </c>
       <c r="B441" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C441" s="24" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D441" s="12"/>
     </row>
@@ -7678,10 +7664,10 @@
         <v>437</v>
       </c>
       <c r="B442" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C442" s="24" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D442" s="12"/>
     </row>
@@ -7691,10 +7677,10 @@
         <v>438</v>
       </c>
       <c r="B443" s="15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C443" s="24" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D443" s="12"/>
     </row>
@@ -7704,10 +7690,10 @@
         <v>439</v>
       </c>
       <c r="B444" s="10" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C444" s="24" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D444" s="12"/>
     </row>
@@ -7717,10 +7703,10 @@
         <v>440</v>
       </c>
       <c r="B445" s="10" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C445" s="24" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D445" s="12"/>
     </row>
@@ -7730,10 +7716,10 @@
         <v>441</v>
       </c>
       <c r="B446" s="10" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C446" s="24" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D446" s="12"/>
     </row>
@@ -7743,10 +7729,10 @@
         <v>442</v>
       </c>
       <c r="B447" s="10" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C447" s="24" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D447" s="12"/>
     </row>
@@ -7756,10 +7742,10 @@
         <v>443</v>
       </c>
       <c r="B448" s="10" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C448" s="24" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D448" s="12"/>
     </row>
@@ -7769,10 +7755,10 @@
         <v>444</v>
       </c>
       <c r="B449" s="10" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C449" s="24" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D449" s="12"/>
     </row>
@@ -7782,10 +7768,10 @@
         <v>445</v>
       </c>
       <c r="B450" s="10" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C450" s="24" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D450" s="12"/>
     </row>
@@ -7795,10 +7781,10 @@
         <v>446</v>
       </c>
       <c r="B451" s="10" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C451" s="24" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D451" s="12"/>
     </row>
@@ -7808,10 +7794,10 @@
         <v>447</v>
       </c>
       <c r="B452" s="10" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C452" s="24" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D452" s="12"/>
     </row>
@@ -7821,10 +7807,10 @@
         <v>448</v>
       </c>
       <c r="B453" s="10" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C453" s="24" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D453" s="12"/>
     </row>
@@ -7936,7 +7922,7 @@
     <hyperlink ref="C67" r:id="rId62" display="Balanced Parenthesis problem.[Imp]"/>
     <hyperlink ref="C68" r:id="rId63" display="Word break Problem[ Very Imp]"/>
     <hyperlink ref="C69" r:id="rId64" display="Rabin Karp Algo"/>
-    <hyperlink ref="D69" r:id="rId65" display="doubt: Why mod = 1e9+7 gave the wrong answer, but 1e5+7 worked fine"/>
+    <hyperlink ref="D69" r:id="rId65" display="doubt: Why mod = 1e9+7 gave the wrong answer, but 1e5+7 worked fine [ANSWERED]"/>
     <hyperlink ref="C70" r:id="rId66" display="KMP Algo"/>
     <hyperlink ref="C71" r:id="rId67" display="Convert a Sentence into its equivalent mobile numeric keypad sequence."/>
     <hyperlink ref="C72" r:id="rId68" display="Minimum number of bracket reversals needed to make an expression balanced."/>

</xml_diff>

<commit_message>
done Q66 convert string into numeric keypad
</commit_message>
<xml_diff>
--- a/DSA_450_LoveBabbar.xlsx
+++ b/DSA_450_LoveBabbar.xlsx
@@ -1939,11 +1939,11 @@
   </sheetPr>
   <dimension ref="A1:D467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C71" activeCellId="0" sqref="C71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.24"/>
@@ -2851,7 +2851,7 @@
       <c r="B71" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C71" s="24" t="s">
+      <c r="C71" s="13" t="s">
         <v>83</v>
       </c>
       <c r="D71" s="12"/>

</xml_diff>

<commit_message>
done Q67 minimum number of bracket reversals
</commit_message>
<xml_diff>
--- a/DSA_450_LoveBabbar.xlsx
+++ b/DSA_450_LoveBabbar.xlsx
@@ -1940,10 +1940,10 @@
   <dimension ref="A1:D467"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C71" activeCellId="0" sqref="C71"/>
+      <selection pane="topLeft" activeCell="C72" activeCellId="0" sqref="C72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.24"/>
@@ -2864,7 +2864,7 @@
       <c r="B72" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C72" s="24" t="s">
+      <c r="C72" s="11" t="s">
         <v>84</v>
       </c>
       <c r="D72" s="12"/>

</xml_diff>

<commit_message>
done Q68 count palindromic subsequences in n2^n
</commit_message>
<xml_diff>
--- a/DSA_450_LoveBabbar.xlsx
+++ b/DSA_450_LoveBabbar.xlsx
@@ -1939,8 +1939,8 @@
   </sheetPr>
   <dimension ref="A1:D467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C72" activeCellId="0" sqref="C72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C74" activeCellId="0" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2877,7 +2877,7 @@
       <c r="B73" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C73" s="24" t="s">
+      <c r="C73" s="11" t="s">
         <v>85</v>
       </c>
       <c r="D73" s="12"/>

</xml_diff>

<commit_message>
optimized Q68 count all palindromic subsequences
</commit_message>
<xml_diff>
--- a/DSA_450_LoveBabbar.xlsx
+++ b/DSA_450_LoveBabbar.xlsx
@@ -174,7 +174,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Can’t solve generalised form MxN in given time
+      <t xml:space="preserve">Can’t solve generalized form MxN in given time
 </t>
     </r>
     <r>
@@ -1940,7 +1940,7 @@
   <dimension ref="A1:D467"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C74" activeCellId="0" sqref="C74"/>
+      <selection pane="topLeft" activeCell="D70" activeCellId="0" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8308,7 +8308,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
done Q69 count of given string in 2d char array
</commit_message>
<xml_diff>
--- a/DSA_450_LoveBabbar.xlsx
+++ b/DSA_450_LoveBabbar.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="475">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t xml:space="preserve">Count of number of given string in 2D character array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POTENTIAL CROSSWORD SOLVER ? Checkout the resources folder for what I made before solving this</t>
   </si>
   <si>
     <t xml:space="preserve">Search a Word in a 2D Grid of characters.</t>
@@ -1939,8 +1942,8 @@
   </sheetPr>
   <dimension ref="A1:D467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D70" activeCellId="0" sqref="D70"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D76" activeCellId="0" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2890,10 +2893,12 @@
       <c r="B74" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C74" s="24" t="s">
+      <c r="C74" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D74" s="12"/>
+      <c r="D74" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="n">
@@ -2904,7 +2909,7 @@
         <v>56</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D75" s="12"/>
     </row>
@@ -2917,7 +2922,7 @@
         <v>56</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D76" s="12"/>
     </row>
@@ -2930,7 +2935,7 @@
         <v>56</v>
       </c>
       <c r="C77" s="24" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D77" s="12"/>
     </row>
@@ -2943,7 +2948,7 @@
         <v>56</v>
       </c>
       <c r="C78" s="24" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D78" s="12"/>
     </row>
@@ -2956,7 +2961,7 @@
         <v>56</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D79" s="12"/>
     </row>
@@ -2969,7 +2974,7 @@
         <v>56</v>
       </c>
       <c r="C80" s="24" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D80" s="12"/>
     </row>
@@ -2982,7 +2987,7 @@
         <v>56</v>
       </c>
       <c r="C81" s="24" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D81" s="12"/>
     </row>
@@ -2995,7 +3000,7 @@
         <v>56</v>
       </c>
       <c r="C82" s="24" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D82" s="12"/>
     </row>
@@ -3008,7 +3013,7 @@
         <v>56</v>
       </c>
       <c r="C83" s="24" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D83" s="12"/>
     </row>
@@ -3021,7 +3026,7 @@
         <v>56</v>
       </c>
       <c r="C84" s="24" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D84" s="12"/>
     </row>
@@ -3034,7 +3039,7 @@
         <v>56</v>
       </c>
       <c r="C85" s="24" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D85" s="12"/>
     </row>
@@ -3047,7 +3052,7 @@
         <v>56</v>
       </c>
       <c r="C86" s="24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D86" s="12"/>
     </row>
@@ -3060,7 +3065,7 @@
         <v>56</v>
       </c>
       <c r="C87" s="24" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D87" s="12"/>
     </row>
@@ -3073,7 +3078,7 @@
         <v>56</v>
       </c>
       <c r="C88" s="24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D88" s="12"/>
     </row>
@@ -3086,7 +3091,7 @@
         <v>56</v>
       </c>
       <c r="C89" s="24" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D89" s="12"/>
     </row>
@@ -3099,7 +3104,7 @@
         <v>56</v>
       </c>
       <c r="C90" s="24" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D90" s="12"/>
     </row>
@@ -3112,7 +3117,7 @@
         <v>56</v>
       </c>
       <c r="C91" s="24" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D91" s="12"/>
     </row>
@@ -3125,7 +3130,7 @@
         <v>56</v>
       </c>
       <c r="C92" s="24" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D92" s="12"/>
     </row>
@@ -3138,7 +3143,7 @@
         <v>56</v>
       </c>
       <c r="C93" s="24" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D93" s="12"/>
     </row>
@@ -3151,7 +3156,7 @@
         <v>56</v>
       </c>
       <c r="C94" s="24" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D94" s="12"/>
     </row>
@@ -3161,10 +3166,10 @@
         <v>90</v>
       </c>
       <c r="B95" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C95" s="24" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D95" s="12"/>
     </row>
@@ -3174,10 +3179,10 @@
         <v>91</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C96" s="24" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D96" s="12"/>
     </row>
@@ -3187,10 +3192,10 @@
         <v>92</v>
       </c>
       <c r="B97" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C97" s="24" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D97" s="12"/>
     </row>
@@ -3200,10 +3205,10 @@
         <v>93</v>
       </c>
       <c r="B98" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C98" s="24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D98" s="12"/>
     </row>
@@ -3213,10 +3218,10 @@
         <v>94</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C99" s="24" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D99" s="12"/>
     </row>
@@ -3226,10 +3231,10 @@
         <v>95</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C100" s="24" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D100" s="12"/>
     </row>
@@ -3239,10 +3244,10 @@
         <v>96</v>
       </c>
       <c r="B101" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C101" s="24" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D101" s="12"/>
     </row>
@@ -3252,10 +3257,10 @@
         <v>97</v>
       </c>
       <c r="B102" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C102" s="24" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D102" s="12"/>
     </row>
@@ -3265,10 +3270,10 @@
         <v>98</v>
       </c>
       <c r="B103" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C103" s="24" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D103" s="12"/>
     </row>
@@ -3278,10 +3283,10 @@
         <v>99</v>
       </c>
       <c r="B104" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C104" s="24" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D104" s="12"/>
     </row>
@@ -3291,10 +3296,10 @@
         <v>100</v>
       </c>
       <c r="B105" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C105" s="24" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D105" s="12"/>
     </row>
@@ -3304,10 +3309,10 @@
         <v>101</v>
       </c>
       <c r="B106" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C106" s="24" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D106" s="12"/>
     </row>
@@ -3317,10 +3322,10 @@
         <v>102</v>
       </c>
       <c r="B107" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C107" s="24" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D107" s="12"/>
     </row>
@@ -3330,10 +3335,10 @@
         <v>103</v>
       </c>
       <c r="B108" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C108" s="24" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D108" s="12"/>
     </row>
@@ -3343,10 +3348,10 @@
         <v>104</v>
       </c>
       <c r="B109" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C109" s="24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D109" s="12"/>
     </row>
@@ -3356,10 +3361,10 @@
         <v>105</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C110" s="24" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D110" s="12"/>
     </row>
@@ -3369,10 +3374,10 @@
         <v>106</v>
       </c>
       <c r="B111" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C111" s="24" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D111" s="12"/>
     </row>
@@ -3382,10 +3387,10 @@
         <v>107</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C112" s="24" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D112" s="12"/>
     </row>
@@ -3395,10 +3400,10 @@
         <v>108</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C113" s="24" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D113" s="12"/>
     </row>
@@ -3408,10 +3413,10 @@
         <v>109</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C114" s="24" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D114" s="12"/>
     </row>
@@ -3421,10 +3426,10 @@
         <v>110</v>
       </c>
       <c r="B115" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C115" s="24" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D115" s="12"/>
     </row>
@@ -3434,10 +3439,10 @@
         <v>111</v>
       </c>
       <c r="B116" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C116" s="24" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D116" s="12"/>
     </row>
@@ -3447,10 +3452,10 @@
         <v>112</v>
       </c>
       <c r="B117" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C117" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D117" s="12"/>
     </row>
@@ -3460,10 +3465,10 @@
         <v>113</v>
       </c>
       <c r="B118" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C118" s="24" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D118" s="12"/>
     </row>
@@ -3473,10 +3478,10 @@
         <v>114</v>
       </c>
       <c r="B119" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C119" s="24" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D119" s="12"/>
     </row>
@@ -3486,10 +3491,10 @@
         <v>115</v>
       </c>
       <c r="B120" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C120" s="24" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D120" s="12"/>
     </row>
@@ -3499,10 +3504,10 @@
         <v>116</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C121" s="24" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D121" s="12"/>
     </row>
@@ -3512,10 +3517,10 @@
         <v>117</v>
       </c>
       <c r="B122" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C122" s="24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D122" s="12"/>
     </row>
@@ -3525,10 +3530,10 @@
         <v>118</v>
       </c>
       <c r="B123" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C123" s="24" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D123" s="12"/>
     </row>
@@ -3538,10 +3543,10 @@
         <v>119</v>
       </c>
       <c r="B124" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C124" s="24" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D124" s="12"/>
     </row>
@@ -3551,10 +3556,10 @@
         <v>120</v>
       </c>
       <c r="B125" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C125" s="24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D125" s="12"/>
     </row>
@@ -3564,10 +3569,10 @@
         <v>121</v>
       </c>
       <c r="B126" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C126" s="24" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D126" s="12"/>
     </row>
@@ -3577,10 +3582,10 @@
         <v>122</v>
       </c>
       <c r="B127" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C127" s="24" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D127" s="12"/>
     </row>
@@ -3590,10 +3595,10 @@
         <v>123</v>
       </c>
       <c r="B128" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C128" s="24" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D128" s="12"/>
     </row>
@@ -3603,10 +3608,10 @@
         <v>124</v>
       </c>
       <c r="B129" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C129" s="24" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D129" s="12"/>
     </row>
@@ -3616,10 +3621,10 @@
         <v>125</v>
       </c>
       <c r="B130" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C130" s="24" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D130" s="12"/>
     </row>
@@ -3629,10 +3634,10 @@
         <v>126</v>
       </c>
       <c r="B131" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C131" s="24" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D131" s="12"/>
     </row>
@@ -3642,10 +3647,10 @@
         <v>127</v>
       </c>
       <c r="B132" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C132" s="24" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D132" s="12"/>
     </row>
@@ -3655,10 +3660,10 @@
         <v>128</v>
       </c>
       <c r="B133" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C133" s="24" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D133" s="12"/>
     </row>
@@ -3668,10 +3673,10 @@
         <v>129</v>
       </c>
       <c r="B134" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C134" s="24" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D134" s="12"/>
     </row>
@@ -3681,10 +3686,10 @@
         <v>130</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C135" s="24" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D135" s="12"/>
     </row>
@@ -3694,10 +3699,10 @@
         <v>131</v>
       </c>
       <c r="B136" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C136" s="24" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D136" s="12"/>
     </row>
@@ -3707,10 +3712,10 @@
         <v>132</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C137" s="24" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D137" s="12"/>
     </row>
@@ -3720,10 +3725,10 @@
         <v>133</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C138" s="24" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D138" s="12"/>
     </row>
@@ -3733,10 +3738,10 @@
         <v>134</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C139" s="24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D139" s="12"/>
     </row>
@@ -3746,10 +3751,10 @@
         <v>135</v>
       </c>
       <c r="B140" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C140" s="24" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D140" s="12"/>
     </row>
@@ -3759,10 +3764,10 @@
         <v>136</v>
       </c>
       <c r="B141" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C141" s="24" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D141" s="12"/>
     </row>
@@ -3772,10 +3777,10 @@
         <v>137</v>
       </c>
       <c r="B142" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C142" s="24" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D142" s="12"/>
     </row>
@@ -3785,10 +3790,10 @@
         <v>138</v>
       </c>
       <c r="B143" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C143" s="24" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D143" s="12"/>
     </row>
@@ -3798,10 +3803,10 @@
         <v>139</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C144" s="24" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D144" s="12"/>
     </row>
@@ -3811,10 +3816,10 @@
         <v>140</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C145" s="24" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D145" s="12"/>
     </row>
@@ -3824,10 +3829,10 @@
         <v>141</v>
       </c>
       <c r="B146" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C146" s="24" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D146" s="12"/>
     </row>
@@ -3837,10 +3842,10 @@
         <v>142</v>
       </c>
       <c r="B147" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C147" s="24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D147" s="12"/>
     </row>
@@ -3850,10 +3855,10 @@
         <v>143</v>
       </c>
       <c r="B148" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C148" s="24" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D148" s="12"/>
     </row>
@@ -3863,10 +3868,10 @@
         <v>144</v>
       </c>
       <c r="B149" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C149" s="24" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D149" s="12"/>
     </row>
@@ -3876,10 +3881,10 @@
         <v>145</v>
       </c>
       <c r="B150" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C150" s="24" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D150" s="12"/>
     </row>
@@ -3889,10 +3894,10 @@
         <v>146</v>
       </c>
       <c r="B151" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C151" s="24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D151" s="12"/>
     </row>
@@ -3902,10 +3907,10 @@
         <v>147</v>
       </c>
       <c r="B152" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C152" s="24" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D152" s="12"/>
     </row>
@@ -3915,10 +3920,10 @@
         <v>148</v>
       </c>
       <c r="B153" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C153" s="24" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D153" s="12"/>
     </row>
@@ -3928,10 +3933,10 @@
         <v>149</v>
       </c>
       <c r="B154" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C154" s="24" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D154" s="12"/>
     </row>
@@ -3941,10 +3946,10 @@
         <v>150</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C155" s="24" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D155" s="12"/>
     </row>
@@ -3954,10 +3959,10 @@
         <v>151</v>
       </c>
       <c r="B156" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C156" s="25" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D156" s="12"/>
     </row>
@@ -3967,10 +3972,10 @@
         <v>152</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C157" s="25" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D157" s="12"/>
     </row>
@@ -3980,10 +3985,10 @@
         <v>153</v>
       </c>
       <c r="B158" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C158" s="24" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D158" s="12"/>
     </row>
@@ -3993,10 +3998,10 @@
         <v>154</v>
       </c>
       <c r="B159" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C159" s="24" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D159" s="12"/>
     </row>
@@ -4006,10 +4011,10 @@
         <v>155</v>
       </c>
       <c r="B160" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C160" s="24" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D160" s="12"/>
     </row>
@@ -4019,10 +4024,10 @@
         <v>156</v>
       </c>
       <c r="B161" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C161" s="24" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D161" s="12"/>
     </row>
@@ -4032,10 +4037,10 @@
         <v>157</v>
       </c>
       <c r="B162" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C162" s="24" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D162" s="12"/>
     </row>
@@ -4045,10 +4050,10 @@
         <v>158</v>
       </c>
       <c r="B163" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C163" s="24" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D163" s="12"/>
     </row>
@@ -4058,10 +4063,10 @@
         <v>159</v>
       </c>
       <c r="B164" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C164" s="24" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D164" s="12"/>
     </row>
@@ -4071,10 +4076,10 @@
         <v>160</v>
       </c>
       <c r="B165" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C165" s="24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D165" s="12"/>
     </row>
@@ -4084,10 +4089,10 @@
         <v>161</v>
       </c>
       <c r="B166" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C166" s="24" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D166" s="12"/>
     </row>
@@ -4097,10 +4102,10 @@
         <v>162</v>
       </c>
       <c r="B167" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C167" s="24" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D167" s="12"/>
     </row>
@@ -4110,10 +4115,10 @@
         <v>163</v>
       </c>
       <c r="B168" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C168" s="24" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D168" s="12"/>
     </row>
@@ -4123,10 +4128,10 @@
         <v>164</v>
       </c>
       <c r="B169" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C169" s="24" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D169" s="12"/>
     </row>
@@ -4136,10 +4141,10 @@
         <v>165</v>
       </c>
       <c r="B170" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C170" s="24" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D170" s="12"/>
     </row>
@@ -4149,10 +4154,10 @@
         <v>166</v>
       </c>
       <c r="B171" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C171" s="24" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D171" s="12"/>
     </row>
@@ -4162,10 +4167,10 @@
         <v>167</v>
       </c>
       <c r="B172" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C172" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D172" s="12"/>
     </row>
@@ -4175,10 +4180,10 @@
         <v>168</v>
       </c>
       <c r="B173" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C173" s="24" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D173" s="12"/>
     </row>
@@ -4188,10 +4193,10 @@
         <v>169</v>
       </c>
       <c r="B174" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C174" s="24" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D174" s="12"/>
     </row>
@@ -4201,10 +4206,10 @@
         <v>170</v>
       </c>
       <c r="B175" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C175" s="24" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D175" s="12"/>
     </row>
@@ -4214,10 +4219,10 @@
         <v>171</v>
       </c>
       <c r="B176" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C176" s="24" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D176" s="12"/>
     </row>
@@ -4227,10 +4232,10 @@
         <v>172</v>
       </c>
       <c r="B177" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C177" s="24" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D177" s="12"/>
     </row>
@@ -4240,10 +4245,10 @@
         <v>173</v>
       </c>
       <c r="B178" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C178" s="24" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D178" s="12"/>
     </row>
@@ -4253,10 +4258,10 @@
         <v>174</v>
       </c>
       <c r="B179" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C179" s="24" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D179" s="12"/>
     </row>
@@ -4266,10 +4271,10 @@
         <v>175</v>
       </c>
       <c r="B180" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C180" s="24" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D180" s="12"/>
     </row>
@@ -4279,10 +4284,10 @@
         <v>176</v>
       </c>
       <c r="B181" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C181" s="24" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D181" s="12"/>
     </row>
@@ -4292,10 +4297,10 @@
         <v>177</v>
       </c>
       <c r="B182" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C182" s="24" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D182" s="12"/>
     </row>
@@ -4305,10 +4310,10 @@
         <v>178</v>
       </c>
       <c r="B183" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C183" s="24" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D183" s="12"/>
     </row>
@@ -4318,10 +4323,10 @@
         <v>179</v>
       </c>
       <c r="B184" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C184" s="24" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D184" s="12"/>
     </row>
@@ -4331,10 +4336,10 @@
         <v>180</v>
       </c>
       <c r="B185" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C185" s="24" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D185" s="12"/>
     </row>
@@ -4344,10 +4349,10 @@
         <v>181</v>
       </c>
       <c r="B186" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C186" s="24" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D186" s="12"/>
     </row>
@@ -4357,10 +4362,10 @@
         <v>182</v>
       </c>
       <c r="B187" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C187" s="24" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D187" s="12"/>
     </row>
@@ -4370,10 +4375,10 @@
         <v>183</v>
       </c>
       <c r="B188" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C188" s="24" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D188" s="12"/>
     </row>
@@ -4383,10 +4388,10 @@
         <v>184</v>
       </c>
       <c r="B189" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C189" s="24" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D189" s="12"/>
     </row>
@@ -4396,10 +4401,10 @@
         <v>185</v>
       </c>
       <c r="B190" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C190" s="24" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D190" s="12"/>
     </row>
@@ -4409,10 +4414,10 @@
         <v>186</v>
       </c>
       <c r="B191" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C191" s="24" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D191" s="12"/>
     </row>
@@ -4422,10 +4427,10 @@
         <v>187</v>
       </c>
       <c r="B192" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C192" s="24" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D192" s="12"/>
     </row>
@@ -4435,10 +4440,10 @@
         <v>188</v>
       </c>
       <c r="B193" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C193" s="24" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D193" s="12"/>
     </row>
@@ -4448,10 +4453,10 @@
         <v>189</v>
       </c>
       <c r="B194" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C194" s="24" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D194" s="12"/>
     </row>
@@ -4461,10 +4466,10 @@
         <v>190</v>
       </c>
       <c r="B195" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C195" s="24" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D195" s="12"/>
     </row>
@@ -4474,10 +4479,10 @@
         <v>191</v>
       </c>
       <c r="B196" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C196" s="24" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D196" s="12"/>
     </row>
@@ -4487,10 +4492,10 @@
         <v>192</v>
       </c>
       <c r="B197" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C197" s="24" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D197" s="12"/>
     </row>
@@ -4500,10 +4505,10 @@
         <v>193</v>
       </c>
       <c r="B198" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C198" s="24" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D198" s="12"/>
     </row>
@@ -4513,10 +4518,10 @@
         <v>194</v>
       </c>
       <c r="B199" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C199" s="24" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D199" s="12"/>
     </row>
@@ -4526,10 +4531,10 @@
         <v>195</v>
       </c>
       <c r="B200" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C200" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D200" s="12"/>
     </row>
@@ -4539,10 +4544,10 @@
         <v>196</v>
       </c>
       <c r="B201" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C201" s="24" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D201" s="12"/>
     </row>
@@ -4552,10 +4557,10 @@
         <v>197</v>
       </c>
       <c r="B202" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C202" s="24" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4564,10 +4569,10 @@
         <v>198</v>
       </c>
       <c r="B203" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C203" s="24" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4576,10 +4581,10 @@
         <v>199</v>
       </c>
       <c r="B204" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C204" s="24" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4588,10 +4593,10 @@
         <v>200</v>
       </c>
       <c r="B205" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C205" s="24" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4600,10 +4605,10 @@
         <v>201</v>
       </c>
       <c r="B206" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C206" s="24" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4612,10 +4617,10 @@
         <v>202</v>
       </c>
       <c r="B207" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C207" s="24" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4624,10 +4629,10 @@
         <v>203</v>
       </c>
       <c r="B208" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C208" s="26" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4636,10 +4641,10 @@
         <v>204</v>
       </c>
       <c r="B209" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C209" s="24" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4648,10 +4653,10 @@
         <v>205</v>
       </c>
       <c r="B210" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C210" s="24" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D210" s="12"/>
     </row>
@@ -4661,10 +4666,10 @@
         <v>206</v>
       </c>
       <c r="B211" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C211" s="24" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D211" s="12"/>
     </row>
@@ -4674,10 +4679,10 @@
         <v>207</v>
       </c>
       <c r="B212" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C212" s="24" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D212" s="12"/>
     </row>
@@ -4687,10 +4692,10 @@
         <v>208</v>
       </c>
       <c r="B213" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C213" s="24" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D213" s="12"/>
     </row>
@@ -4700,10 +4705,10 @@
         <v>209</v>
       </c>
       <c r="B214" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C214" s="24" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D214" s="12"/>
     </row>
@@ -4713,10 +4718,10 @@
         <v>210</v>
       </c>
       <c r="B215" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C215" s="24" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D215" s="12"/>
     </row>
@@ -4726,10 +4731,10 @@
         <v>211</v>
       </c>
       <c r="B216" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C216" s="24" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D216" s="12"/>
     </row>
@@ -4739,10 +4744,10 @@
         <v>212</v>
       </c>
       <c r="B217" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C217" s="24" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D217" s="12"/>
     </row>
@@ -4752,10 +4757,10 @@
         <v>213</v>
       </c>
       <c r="B218" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C218" s="24" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D218" s="12"/>
     </row>
@@ -4765,10 +4770,10 @@
         <v>214</v>
       </c>
       <c r="B219" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C219" s="24" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D219" s="12"/>
     </row>
@@ -4778,10 +4783,10 @@
         <v>215</v>
       </c>
       <c r="B220" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C220" s="24" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D220" s="12"/>
     </row>
@@ -4791,10 +4796,10 @@
         <v>216</v>
       </c>
       <c r="B221" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C221" s="24" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D221" s="12"/>
     </row>
@@ -4804,10 +4809,10 @@
         <v>217</v>
       </c>
       <c r="B222" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C222" s="24" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D222" s="12"/>
     </row>
@@ -4817,10 +4822,10 @@
         <v>218</v>
       </c>
       <c r="B223" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C223" s="24" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D223" s="12"/>
     </row>
@@ -4830,10 +4835,10 @@
         <v>219</v>
       </c>
       <c r="B224" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C224" s="24" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D224" s="12"/>
     </row>
@@ -4843,10 +4848,10 @@
         <v>220</v>
       </c>
       <c r="B225" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C225" s="24" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D225" s="12"/>
     </row>
@@ -4856,10 +4861,10 @@
         <v>221</v>
       </c>
       <c r="B226" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C226" s="24" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D226" s="12"/>
     </row>
@@ -4869,10 +4874,10 @@
         <v>222</v>
       </c>
       <c r="B227" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C227" s="24" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D227" s="12"/>
     </row>
@@ -4882,10 +4887,10 @@
         <v>223</v>
       </c>
       <c r="B228" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C228" s="24" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D228" s="12"/>
     </row>
@@ -4895,10 +4900,10 @@
         <v>224</v>
       </c>
       <c r="B229" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C229" s="24" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D229" s="12"/>
     </row>
@@ -4908,10 +4913,10 @@
         <v>225</v>
       </c>
       <c r="B230" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C230" s="24" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D230" s="12"/>
     </row>
@@ -4921,10 +4926,10 @@
         <v>226</v>
       </c>
       <c r="B231" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C231" s="24" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D231" s="12"/>
     </row>
@@ -4934,10 +4939,10 @@
         <v>227</v>
       </c>
       <c r="B232" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C232" s="24" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D232" s="12"/>
     </row>
@@ -4947,10 +4952,10 @@
         <v>228</v>
       </c>
       <c r="B233" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C233" s="24" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D233" s="12"/>
     </row>
@@ -4960,10 +4965,10 @@
         <v>229</v>
       </c>
       <c r="B234" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C234" s="24" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D234" s="12"/>
     </row>
@@ -4973,10 +4978,10 @@
         <v>230</v>
       </c>
       <c r="B235" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C235" s="24" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D235" s="12"/>
     </row>
@@ -4986,10 +4991,10 @@
         <v>231</v>
       </c>
       <c r="B236" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C236" s="24" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D236" s="12"/>
     </row>
@@ -4999,10 +5004,10 @@
         <v>232</v>
       </c>
       <c r="B237" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C237" s="24" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D237" s="12"/>
     </row>
@@ -5012,10 +5017,10 @@
         <v>233</v>
       </c>
       <c r="B238" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C238" s="24" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D238" s="12"/>
     </row>
@@ -5025,10 +5030,10 @@
         <v>234</v>
       </c>
       <c r="B239" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C239" s="24" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D239" s="12"/>
     </row>
@@ -5038,10 +5043,10 @@
         <v>235</v>
       </c>
       <c r="B240" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C240" s="24" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D240" s="12"/>
     </row>
@@ -5051,10 +5056,10 @@
         <v>236</v>
       </c>
       <c r="B241" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C241" s="24" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D241" s="12"/>
     </row>
@@ -5064,10 +5069,10 @@
         <v>237</v>
       </c>
       <c r="B242" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C242" s="24" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D242" s="12"/>
     </row>
@@ -5077,10 +5082,10 @@
         <v>238</v>
       </c>
       <c r="B243" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C243" s="24" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D243" s="12"/>
     </row>
@@ -5090,10 +5095,10 @@
         <v>239</v>
       </c>
       <c r="B244" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C244" s="24" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D244" s="12"/>
     </row>
@@ -5103,10 +5108,10 @@
         <v>240</v>
       </c>
       <c r="B245" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C245" s="24" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D245" s="12"/>
     </row>
@@ -5116,10 +5121,10 @@
         <v>241</v>
       </c>
       <c r="B246" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C246" s="24" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D246" s="12"/>
     </row>
@@ -5129,10 +5134,10 @@
         <v>242</v>
       </c>
       <c r="B247" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C247" s="24" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D247" s="12"/>
     </row>
@@ -5142,10 +5147,10 @@
         <v>243</v>
       </c>
       <c r="B248" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C248" s="24" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D248" s="12"/>
     </row>
@@ -5155,10 +5160,10 @@
         <v>244</v>
       </c>
       <c r="B249" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C249" s="24" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D249" s="12"/>
     </row>
@@ -5168,10 +5173,10 @@
         <v>245</v>
       </c>
       <c r="B250" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C250" s="24" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D250" s="12"/>
     </row>
@@ -5181,10 +5186,10 @@
         <v>246</v>
       </c>
       <c r="B251" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C251" s="24" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D251" s="12"/>
     </row>
@@ -5194,10 +5199,10 @@
         <v>247</v>
       </c>
       <c r="B252" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C252" s="24" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D252" s="12"/>
     </row>
@@ -5207,10 +5212,10 @@
         <v>248</v>
       </c>
       <c r="B253" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C253" s="24" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D253" s="12"/>
     </row>
@@ -5220,10 +5225,10 @@
         <v>249</v>
       </c>
       <c r="B254" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C254" s="24" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D254" s="12"/>
     </row>
@@ -5233,10 +5238,10 @@
         <v>250</v>
       </c>
       <c r="B255" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C255" s="24" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D255" s="12"/>
     </row>
@@ -5246,10 +5251,10 @@
         <v>251</v>
       </c>
       <c r="B256" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C256" s="24" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D256" s="12"/>
     </row>
@@ -5259,10 +5264,10 @@
         <v>252</v>
       </c>
       <c r="B257" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C257" s="24" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D257" s="12"/>
     </row>
@@ -5272,10 +5277,10 @@
         <v>253</v>
       </c>
       <c r="B258" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C258" s="24" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D258" s="12"/>
     </row>
@@ -5285,10 +5290,10 @@
         <v>254</v>
       </c>
       <c r="B259" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C259" s="24" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D259" s="12"/>
     </row>
@@ -5298,10 +5303,10 @@
         <v>255</v>
       </c>
       <c r="B260" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C260" s="24" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D260" s="12"/>
     </row>
@@ -5311,10 +5316,10 @@
         <v>256</v>
       </c>
       <c r="B261" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C261" s="24" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D261" s="12"/>
     </row>
@@ -5324,10 +5329,10 @@
         <v>257</v>
       </c>
       <c r="B262" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C262" s="24" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D262" s="12"/>
     </row>
@@ -5337,10 +5342,10 @@
         <v>258</v>
       </c>
       <c r="B263" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C263" s="24" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D263" s="12"/>
     </row>
@@ -5350,10 +5355,10 @@
         <v>259</v>
       </c>
       <c r="B264" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C264" s="24" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D264" s="12"/>
     </row>
@@ -5363,10 +5368,10 @@
         <v>260</v>
       </c>
       <c r="B265" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C265" s="24" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D265" s="12"/>
     </row>
@@ -5376,10 +5381,10 @@
         <v>261</v>
       </c>
       <c r="B266" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C266" s="24" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D266" s="12"/>
     </row>
@@ -5389,10 +5394,10 @@
         <v>262</v>
       </c>
       <c r="B267" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C267" s="24" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D267" s="12"/>
     </row>
@@ -5402,10 +5407,10 @@
         <v>263</v>
       </c>
       <c r="B268" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C268" s="24" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D268" s="12"/>
     </row>
@@ -5415,10 +5420,10 @@
         <v>264</v>
       </c>
       <c r="B269" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C269" s="24" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D269" s="12"/>
     </row>
@@ -5428,10 +5433,10 @@
         <v>265</v>
       </c>
       <c r="B270" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C270" s="24" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D270" s="12"/>
     </row>
@@ -5441,10 +5446,10 @@
         <v>266</v>
       </c>
       <c r="B271" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C271" s="24" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D271" s="12"/>
     </row>
@@ -5454,10 +5459,10 @@
         <v>267</v>
       </c>
       <c r="B272" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C272" s="24" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D272" s="12"/>
     </row>
@@ -5467,10 +5472,10 @@
         <v>268</v>
       </c>
       <c r="B273" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C273" s="24" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D273" s="12"/>
     </row>
@@ -5480,10 +5485,10 @@
         <v>269</v>
       </c>
       <c r="B274" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C274" s="24" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D274" s="12"/>
     </row>
@@ -5493,10 +5498,10 @@
         <v>270</v>
       </c>
       <c r="B275" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C275" s="24" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D275" s="12"/>
     </row>
@@ -5506,10 +5511,10 @@
         <v>271</v>
       </c>
       <c r="B276" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C276" s="24" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D276" s="12"/>
     </row>
@@ -5519,10 +5524,10 @@
         <v>272</v>
       </c>
       <c r="B277" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C277" s="24" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D277" s="12"/>
     </row>
@@ -5532,10 +5537,10 @@
         <v>273</v>
       </c>
       <c r="B278" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C278" s="24" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D278" s="12"/>
     </row>
@@ -5545,10 +5550,10 @@
         <v>274</v>
       </c>
       <c r="B279" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C279" s="24" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D279" s="12"/>
     </row>
@@ -5558,10 +5563,10 @@
         <v>275</v>
       </c>
       <c r="B280" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C280" s="24" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D280" s="12"/>
     </row>
@@ -5571,10 +5576,10 @@
         <v>276</v>
       </c>
       <c r="B281" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C281" s="24" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D281" s="12"/>
     </row>
@@ -5584,10 +5589,10 @@
         <v>277</v>
       </c>
       <c r="B282" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C282" s="24" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D282" s="12"/>
     </row>
@@ -5597,10 +5602,10 @@
         <v>278</v>
       </c>
       <c r="B283" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C283" s="24" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D283" s="12"/>
     </row>
@@ -5610,10 +5615,10 @@
         <v>279</v>
       </c>
       <c r="B284" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C284" s="24" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D284" s="12"/>
     </row>
@@ -5623,10 +5628,10 @@
         <v>280</v>
       </c>
       <c r="B285" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C285" s="24" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D285" s="12"/>
     </row>
@@ -5636,10 +5641,10 @@
         <v>281</v>
       </c>
       <c r="B286" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C286" s="24" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D286" s="12"/>
     </row>
@@ -5649,10 +5654,10 @@
         <v>282</v>
       </c>
       <c r="B287" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C287" s="24" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D287" s="12"/>
     </row>
@@ -5662,10 +5667,10 @@
         <v>283</v>
       </c>
       <c r="B288" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C288" s="24" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D288" s="12"/>
     </row>
@@ -5675,10 +5680,10 @@
         <v>284</v>
       </c>
       <c r="B289" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C289" s="24" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D289" s="12"/>
     </row>
@@ -5688,10 +5693,10 @@
         <v>285</v>
       </c>
       <c r="B290" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C290" s="24" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D290" s="12"/>
     </row>
@@ -5701,10 +5706,10 @@
         <v>286</v>
       </c>
       <c r="B291" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C291" s="26" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D291" s="12"/>
     </row>
@@ -5714,10 +5719,10 @@
         <v>287</v>
       </c>
       <c r="B292" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C292" s="24" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D292" s="12"/>
     </row>
@@ -5727,10 +5732,10 @@
         <v>288</v>
       </c>
       <c r="B293" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C293" s="24" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D293" s="12"/>
     </row>
@@ -5740,10 +5745,10 @@
         <v>289</v>
       </c>
       <c r="B294" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C294" s="24" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D294" s="12"/>
     </row>
@@ -5753,10 +5758,10 @@
         <v>290</v>
       </c>
       <c r="B295" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C295" s="24" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D295" s="12"/>
     </row>
@@ -5766,10 +5771,10 @@
         <v>291</v>
       </c>
       <c r="B296" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C296" s="24" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D296" s="12"/>
     </row>
@@ -5779,10 +5784,10 @@
         <v>292</v>
       </c>
       <c r="B297" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C297" s="24" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D297" s="12"/>
     </row>
@@ -5792,10 +5797,10 @@
         <v>293</v>
       </c>
       <c r="B298" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C298" s="24" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D298" s="12"/>
     </row>
@@ -5805,10 +5810,10 @@
         <v>294</v>
       </c>
       <c r="B299" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C299" s="24" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D299" s="12"/>
     </row>
@@ -5818,10 +5823,10 @@
         <v>295</v>
       </c>
       <c r="B300" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C300" s="24" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D300" s="12"/>
     </row>
@@ -5831,10 +5836,10 @@
         <v>296</v>
       </c>
       <c r="B301" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C301" s="24" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D301" s="12"/>
     </row>
@@ -5844,10 +5849,10 @@
         <v>297</v>
       </c>
       <c r="B302" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C302" s="24" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D302" s="12"/>
     </row>
@@ -5857,10 +5862,10 @@
         <v>298</v>
       </c>
       <c r="B303" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C303" s="24" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D303" s="12"/>
     </row>
@@ -5870,10 +5875,10 @@
         <v>299</v>
       </c>
       <c r="B304" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C304" s="24" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D304" s="12"/>
     </row>
@@ -5883,10 +5888,10 @@
         <v>300</v>
       </c>
       <c r="B305" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C305" s="24" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D305" s="12"/>
     </row>
@@ -5896,10 +5901,10 @@
         <v>301</v>
       </c>
       <c r="B306" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C306" s="24" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D306" s="12"/>
     </row>
@@ -5909,10 +5914,10 @@
         <v>302</v>
       </c>
       <c r="B307" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C307" s="24" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D307" s="12"/>
     </row>
@@ -5922,10 +5927,10 @@
         <v>303</v>
       </c>
       <c r="B308" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C308" s="24" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D308" s="12"/>
     </row>
@@ -5935,10 +5940,10 @@
         <v>304</v>
       </c>
       <c r="B309" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C309" s="24" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D309" s="12"/>
     </row>
@@ -5948,10 +5953,10 @@
         <v>305</v>
       </c>
       <c r="B310" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C310" s="24" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D310" s="12"/>
     </row>
@@ -5961,10 +5966,10 @@
         <v>306</v>
       </c>
       <c r="B311" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C311" s="24" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D311" s="12"/>
     </row>
@@ -5974,10 +5979,10 @@
         <v>307</v>
       </c>
       <c r="B312" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C312" s="24" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D312" s="12"/>
     </row>
@@ -5987,10 +5992,10 @@
         <v>308</v>
       </c>
       <c r="B313" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C313" s="24" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D313" s="12"/>
     </row>
@@ -6000,10 +6005,10 @@
         <v>309</v>
       </c>
       <c r="B314" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C314" s="24" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D314" s="12"/>
     </row>
@@ -6013,10 +6018,10 @@
         <v>310</v>
       </c>
       <c r="B315" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C315" s="24" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D315" s="12"/>
     </row>
@@ -6026,10 +6031,10 @@
         <v>311</v>
       </c>
       <c r="B316" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C316" s="24" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D316" s="12"/>
     </row>
@@ -6039,10 +6044,10 @@
         <v>312</v>
       </c>
       <c r="B317" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C317" s="24" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D317" s="12"/>
     </row>
@@ -6052,10 +6057,10 @@
         <v>313</v>
       </c>
       <c r="B318" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C318" s="24" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D318" s="12"/>
     </row>
@@ -6065,10 +6070,10 @@
         <v>314</v>
       </c>
       <c r="B319" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C319" s="24" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D319" s="12"/>
     </row>
@@ -6078,10 +6083,10 @@
         <v>315</v>
       </c>
       <c r="B320" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C320" s="24" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D320" s="12"/>
     </row>
@@ -6091,10 +6096,10 @@
         <v>316</v>
       </c>
       <c r="B321" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C321" s="24" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D321" s="12"/>
     </row>
@@ -6104,10 +6109,10 @@
         <v>317</v>
       </c>
       <c r="B322" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C322" s="24" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D322" s="12"/>
     </row>
@@ -6117,10 +6122,10 @@
         <v>318</v>
       </c>
       <c r="B323" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C323" s="24" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D323" s="12"/>
     </row>
@@ -6130,10 +6135,10 @@
         <v>319</v>
       </c>
       <c r="B324" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C324" s="26" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D324" s="12"/>
     </row>
@@ -6143,10 +6148,10 @@
         <v>320</v>
       </c>
       <c r="B325" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C325" s="24" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D325" s="12"/>
     </row>
@@ -6156,10 +6161,10 @@
         <v>321</v>
       </c>
       <c r="B326" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C326" s="24" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D326" s="12"/>
     </row>
@@ -6169,10 +6174,10 @@
         <v>322</v>
       </c>
       <c r="B327" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C327" s="24" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D327" s="12"/>
     </row>
@@ -6182,10 +6187,10 @@
         <v>323</v>
       </c>
       <c r="B328" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C328" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D328" s="12"/>
     </row>
@@ -6195,10 +6200,10 @@
         <v>324</v>
       </c>
       <c r="B329" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C329" s="24" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D329" s="12"/>
     </row>
@@ -6208,10 +6213,10 @@
         <v>325</v>
       </c>
       <c r="B330" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C330" s="24" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D330" s="12"/>
     </row>
@@ -6221,10 +6226,10 @@
         <v>326</v>
       </c>
       <c r="B331" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C331" s="24" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D331" s="12"/>
     </row>
@@ -6234,10 +6239,10 @@
         <v>327</v>
       </c>
       <c r="B332" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C332" s="24" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D332" s="12"/>
     </row>
@@ -6247,10 +6252,10 @@
         <v>328</v>
       </c>
       <c r="B333" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C333" s="24" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D333" s="12"/>
     </row>
@@ -6260,10 +6265,10 @@
         <v>329</v>
       </c>
       <c r="B334" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C334" s="24" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D334" s="12"/>
     </row>
@@ -6273,10 +6278,10 @@
         <v>330</v>
       </c>
       <c r="B335" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C335" s="24" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D335" s="12"/>
     </row>
@@ -6286,10 +6291,10 @@
         <v>331</v>
       </c>
       <c r="B336" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C336" s="24" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D336" s="12"/>
     </row>
@@ -6299,10 +6304,10 @@
         <v>332</v>
       </c>
       <c r="B337" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C337" s="24" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D337" s="12"/>
     </row>
@@ -6312,10 +6317,10 @@
         <v>333</v>
       </c>
       <c r="B338" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C338" s="24" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D338" s="12"/>
     </row>
@@ -6325,10 +6330,10 @@
         <v>334</v>
       </c>
       <c r="B339" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C339" s="24" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D339" s="12"/>
     </row>
@@ -6338,10 +6343,10 @@
         <v>335</v>
       </c>
       <c r="B340" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C340" s="24" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D340" s="12"/>
     </row>
@@ -6351,10 +6356,10 @@
         <v>336</v>
       </c>
       <c r="B341" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C341" s="24" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D341" s="12"/>
     </row>
@@ -6364,10 +6369,10 @@
         <v>337</v>
       </c>
       <c r="B342" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C342" s="24" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D342" s="12"/>
     </row>
@@ -6377,10 +6382,10 @@
         <v>338</v>
       </c>
       <c r="B343" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C343" s="24" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D343" s="12"/>
     </row>
@@ -6390,10 +6395,10 @@
         <v>339</v>
       </c>
       <c r="B344" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C344" s="24" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D344" s="12"/>
     </row>
@@ -6403,10 +6408,10 @@
         <v>340</v>
       </c>
       <c r="B345" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C345" s="24" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D345" s="12"/>
     </row>
@@ -6416,10 +6421,10 @@
         <v>341</v>
       </c>
       <c r="B346" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C346" s="24" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D346" s="12"/>
     </row>
@@ -6429,10 +6434,10 @@
         <v>342</v>
       </c>
       <c r="B347" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C347" s="24" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D347" s="12"/>
     </row>
@@ -6442,10 +6447,10 @@
         <v>343</v>
       </c>
       <c r="B348" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C348" s="24" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D348" s="12"/>
     </row>
@@ -6455,10 +6460,10 @@
         <v>344</v>
       </c>
       <c r="B349" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C349" s="24" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D349" s="12"/>
     </row>
@@ -6468,10 +6473,10 @@
         <v>345</v>
       </c>
       <c r="B350" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C350" s="24" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D350" s="12"/>
     </row>
@@ -6481,10 +6486,10 @@
         <v>346</v>
       </c>
       <c r="B351" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C351" s="24" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D351" s="12"/>
     </row>
@@ -6494,10 +6499,10 @@
         <v>347</v>
       </c>
       <c r="B352" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C352" s="24" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D352" s="12"/>
     </row>
@@ -6507,10 +6512,10 @@
         <v>348</v>
       </c>
       <c r="B353" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C353" s="24" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D353" s="12"/>
     </row>
@@ -6520,10 +6525,10 @@
         <v>349</v>
       </c>
       <c r="B354" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C354" s="24" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D354" s="12"/>
     </row>
@@ -6533,10 +6538,10 @@
         <v>350</v>
       </c>
       <c r="B355" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C355" s="24" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D355" s="12"/>
     </row>
@@ -6546,10 +6551,10 @@
         <v>351</v>
       </c>
       <c r="B356" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C356" s="24" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D356" s="12"/>
     </row>
@@ -6559,10 +6564,10 @@
         <v>352</v>
       </c>
       <c r="B357" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C357" s="24" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D357" s="12"/>
     </row>
@@ -6572,10 +6577,10 @@
         <v>353</v>
       </c>
       <c r="B358" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C358" s="24" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D358" s="12"/>
     </row>
@@ -6585,10 +6590,10 @@
         <v>354</v>
       </c>
       <c r="B359" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C359" s="24" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D359" s="12"/>
     </row>
@@ -6598,10 +6603,10 @@
         <v>355</v>
       </c>
       <c r="B360" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C360" s="24" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D360" s="12"/>
     </row>
@@ -6611,10 +6616,10 @@
         <v>356</v>
       </c>
       <c r="B361" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C361" s="24" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D361" s="12"/>
     </row>
@@ -6624,10 +6629,10 @@
         <v>357</v>
       </c>
       <c r="B362" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C362" s="24" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D362" s="12"/>
     </row>
@@ -6637,10 +6642,10 @@
         <v>358</v>
       </c>
       <c r="B363" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C363" s="24" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D363" s="12"/>
     </row>
@@ -6650,10 +6655,10 @@
         <v>359</v>
       </c>
       <c r="B364" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C364" s="24" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D364" s="12"/>
     </row>
@@ -6663,10 +6668,10 @@
         <v>360</v>
       </c>
       <c r="B365" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C365" s="24" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D365" s="12"/>
     </row>
@@ -6676,10 +6681,10 @@
         <v>361</v>
       </c>
       <c r="B366" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C366" s="24" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D366" s="12"/>
     </row>
@@ -6689,10 +6694,10 @@
         <v>362</v>
       </c>
       <c r="B367" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C367" s="24" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D367" s="12"/>
     </row>
@@ -6702,10 +6707,10 @@
         <v>363</v>
       </c>
       <c r="B368" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C368" s="24" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D368" s="12"/>
     </row>
@@ -6715,10 +6720,10 @@
         <v>364</v>
       </c>
       <c r="B369" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C369" s="24" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D369" s="12"/>
     </row>
@@ -6728,10 +6733,10 @@
         <v>365</v>
       </c>
       <c r="B370" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C370" s="24" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D370" s="12"/>
     </row>
@@ -6741,10 +6746,10 @@
         <v>366</v>
       </c>
       <c r="B371" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C371" s="24" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D371" s="12"/>
     </row>
@@ -6754,10 +6759,10 @@
         <v>367</v>
       </c>
       <c r="B372" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C372" s="24" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D372" s="12"/>
     </row>
@@ -6767,10 +6772,10 @@
         <v>368</v>
       </c>
       <c r="B373" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C373" s="24" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D373" s="12"/>
     </row>
@@ -6780,10 +6785,10 @@
         <v>369</v>
       </c>
       <c r="B374" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C374" s="24" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D374" s="12"/>
     </row>
@@ -6793,10 +6798,10 @@
         <v>370</v>
       </c>
       <c r="B375" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C375" s="24" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D375" s="12"/>
     </row>
@@ -6806,10 +6811,10 @@
         <v>371</v>
       </c>
       <c r="B376" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C376" s="24" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D376" s="12"/>
     </row>
@@ -6819,10 +6824,10 @@
         <v>372</v>
       </c>
       <c r="B377" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C377" s="24" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D377" s="12"/>
     </row>
@@ -6832,10 +6837,10 @@
         <v>373</v>
       </c>
       <c r="B378" s="10" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C378" s="24" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D378" s="12"/>
     </row>
@@ -6845,10 +6850,10 @@
         <v>374</v>
       </c>
       <c r="B379" s="10" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C379" s="24" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D379" s="12"/>
     </row>
@@ -6858,10 +6863,10 @@
         <v>375</v>
       </c>
       <c r="B380" s="10" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C380" s="24" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D380" s="12"/>
     </row>
@@ -6871,10 +6876,10 @@
         <v>376</v>
       </c>
       <c r="B381" s="10" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C381" s="24" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D381" s="12"/>
     </row>
@@ -6884,10 +6889,10 @@
         <v>377</v>
       </c>
       <c r="B382" s="10" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C382" s="24" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D382" s="12"/>
     </row>
@@ -6897,10 +6902,10 @@
         <v>378</v>
       </c>
       <c r="B383" s="10" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C383" s="24" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D383" s="12"/>
     </row>
@@ -6910,10 +6915,10 @@
         <v>379</v>
       </c>
       <c r="B384" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C384" s="24" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D384" s="12"/>
     </row>
@@ -6923,10 +6928,10 @@
         <v>380</v>
       </c>
       <c r="B385" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C385" s="24" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D385" s="12"/>
     </row>
@@ -6936,10 +6941,10 @@
         <v>381</v>
       </c>
       <c r="B386" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C386" s="24" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D386" s="12"/>
     </row>
@@ -6949,10 +6954,10 @@
         <v>382</v>
       </c>
       <c r="B387" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C387" s="24" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D387" s="12"/>
     </row>
@@ -6962,10 +6967,10 @@
         <v>383</v>
       </c>
       <c r="B388" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C388" s="24" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D388" s="12"/>
     </row>
@@ -6975,10 +6980,10 @@
         <v>384</v>
       </c>
       <c r="B389" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C389" s="24" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D389" s="12"/>
     </row>
@@ -6988,10 +6993,10 @@
         <v>385</v>
       </c>
       <c r="B390" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C390" s="24" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D390" s="12"/>
     </row>
@@ -7001,10 +7006,10 @@
         <v>386</v>
       </c>
       <c r="B391" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C391" s="24" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D391" s="12"/>
     </row>
@@ -7014,10 +7019,10 @@
         <v>387</v>
       </c>
       <c r="B392" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C392" s="24" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D392" s="12"/>
     </row>
@@ -7027,10 +7032,10 @@
         <v>388</v>
       </c>
       <c r="B393" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C393" s="24" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D393" s="12"/>
     </row>
@@ -7040,10 +7045,10 @@
         <v>389</v>
       </c>
       <c r="B394" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C394" s="24" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D394" s="12"/>
     </row>
@@ -7053,10 +7058,10 @@
         <v>390</v>
       </c>
       <c r="B395" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C395" s="24" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D395" s="12"/>
     </row>
@@ -7066,10 +7071,10 @@
         <v>391</v>
       </c>
       <c r="B396" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C396" s="24" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D396" s="12"/>
     </row>
@@ -7079,10 +7084,10 @@
         <v>392</v>
       </c>
       <c r="B397" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C397" s="24" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D397" s="12"/>
     </row>
@@ -7092,10 +7097,10 @@
         <v>393</v>
       </c>
       <c r="B398" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C398" s="24" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D398" s="12"/>
     </row>
@@ -7105,10 +7110,10 @@
         <v>394</v>
       </c>
       <c r="B399" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C399" s="24" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D399" s="12"/>
     </row>
@@ -7118,10 +7123,10 @@
         <v>395</v>
       </c>
       <c r="B400" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C400" s="24" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D400" s="12"/>
     </row>
@@ -7131,10 +7136,10 @@
         <v>396</v>
       </c>
       <c r="B401" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C401" s="24" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D401" s="12"/>
     </row>
@@ -7144,10 +7149,10 @@
         <v>397</v>
       </c>
       <c r="B402" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C402" s="24" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D402" s="12"/>
     </row>
@@ -7157,10 +7162,10 @@
         <v>398</v>
       </c>
       <c r="B403" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C403" s="24" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D403" s="12"/>
     </row>
@@ -7170,10 +7175,10 @@
         <v>399</v>
       </c>
       <c r="B404" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C404" s="24" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D404" s="12"/>
     </row>
@@ -7183,10 +7188,10 @@
         <v>400</v>
       </c>
       <c r="B405" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C405" s="24" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D405" s="12"/>
     </row>
@@ -7196,10 +7201,10 @@
         <v>401</v>
       </c>
       <c r="B406" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C406" s="24" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D406" s="12"/>
     </row>
@@ -7209,10 +7214,10 @@
         <v>402</v>
       </c>
       <c r="B407" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C407" s="24" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D407" s="12"/>
     </row>
@@ -7222,10 +7227,10 @@
         <v>403</v>
       </c>
       <c r="B408" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C408" s="24" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D408" s="12"/>
     </row>
@@ -7235,10 +7240,10 @@
         <v>404</v>
       </c>
       <c r="B409" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C409" s="24" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D409" s="12"/>
     </row>
@@ -7248,10 +7253,10 @@
         <v>405</v>
       </c>
       <c r="B410" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C410" s="24" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D410" s="12"/>
     </row>
@@ -7261,10 +7266,10 @@
         <v>406</v>
       </c>
       <c r="B411" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C411" s="24" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D411" s="12"/>
     </row>
@@ -7274,10 +7279,10 @@
         <v>407</v>
       </c>
       <c r="B412" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C412" s="24" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D412" s="12"/>
     </row>
@@ -7287,10 +7292,10 @@
         <v>408</v>
       </c>
       <c r="B413" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C413" s="24" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D413" s="12"/>
     </row>
@@ -7300,10 +7305,10 @@
         <v>409</v>
       </c>
       <c r="B414" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C414" s="24" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D414" s="12"/>
     </row>
@@ -7313,10 +7318,10 @@
         <v>410</v>
       </c>
       <c r="B415" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C415" s="24" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D415" s="12"/>
     </row>
@@ -7326,10 +7331,10 @@
         <v>411</v>
       </c>
       <c r="B416" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C416" s="24" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D416" s="12"/>
     </row>
@@ -7339,10 +7344,10 @@
         <v>412</v>
       </c>
       <c r="B417" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C417" s="24" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D417" s="12"/>
     </row>
@@ -7352,10 +7357,10 @@
         <v>413</v>
       </c>
       <c r="B418" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C418" s="24" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D418" s="12"/>
     </row>
@@ -7365,10 +7370,10 @@
         <v>414</v>
       </c>
       <c r="B419" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C419" s="24" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D419" s="12"/>
     </row>
@@ -7378,10 +7383,10 @@
         <v>415</v>
       </c>
       <c r="B420" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C420" s="24" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D420" s="12"/>
     </row>
@@ -7391,10 +7396,10 @@
         <v>416</v>
       </c>
       <c r="B421" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C421" s="24" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D421" s="12"/>
     </row>
@@ -7404,10 +7409,10 @@
         <v>417</v>
       </c>
       <c r="B422" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C422" s="24" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D422" s="12"/>
     </row>
@@ -7417,10 +7422,10 @@
         <v>418</v>
       </c>
       <c r="B423" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C423" s="24" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D423" s="12"/>
     </row>
@@ -7430,10 +7435,10 @@
         <v>419</v>
       </c>
       <c r="B424" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C424" s="24" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D424" s="12"/>
     </row>
@@ -7443,10 +7448,10 @@
         <v>420</v>
       </c>
       <c r="B425" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C425" s="24" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D425" s="12"/>
     </row>
@@ -7456,10 +7461,10 @@
         <v>421</v>
       </c>
       <c r="B426" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C426" s="24" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D426" s="12"/>
     </row>
@@ -7469,10 +7474,10 @@
         <v>422</v>
       </c>
       <c r="B427" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C427" s="24" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D427" s="12"/>
     </row>
@@ -7482,10 +7487,10 @@
         <v>423</v>
       </c>
       <c r="B428" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C428" s="24" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D428" s="12"/>
     </row>
@@ -7495,10 +7500,10 @@
         <v>424</v>
       </c>
       <c r="B429" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C429" s="24" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D429" s="12"/>
     </row>
@@ -7508,10 +7513,10 @@
         <v>425</v>
       </c>
       <c r="B430" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C430" s="24" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D430" s="12"/>
     </row>
@@ -7521,10 +7526,10 @@
         <v>426</v>
       </c>
       <c r="B431" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C431" s="24" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D431" s="12"/>
     </row>
@@ -7534,10 +7539,10 @@
         <v>427</v>
       </c>
       <c r="B432" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C432" s="24" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D432" s="12"/>
     </row>
@@ -7547,10 +7552,10 @@
         <v>428</v>
       </c>
       <c r="B433" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C433" s="24" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D433" s="12"/>
     </row>
@@ -7560,10 +7565,10 @@
         <v>429</v>
       </c>
       <c r="B434" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C434" s="24" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D434" s="12"/>
     </row>
@@ -7573,10 +7578,10 @@
         <v>430</v>
       </c>
       <c r="B435" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C435" s="24" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D435" s="12"/>
     </row>
@@ -7586,10 +7591,10 @@
         <v>431</v>
       </c>
       <c r="B436" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C436" s="24" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D436" s="12"/>
     </row>
@@ -7599,10 +7604,10 @@
         <v>432</v>
       </c>
       <c r="B437" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C437" s="24" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D437" s="12"/>
     </row>
@@ -7612,10 +7617,10 @@
         <v>433</v>
       </c>
       <c r="B438" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C438" s="24" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D438" s="12"/>
     </row>
@@ -7625,10 +7630,10 @@
         <v>434</v>
       </c>
       <c r="B439" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C439" s="24" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D439" s="12"/>
     </row>
@@ -7638,10 +7643,10 @@
         <v>435</v>
       </c>
       <c r="B440" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C440" s="24" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D440" s="12"/>
     </row>
@@ -7651,10 +7656,10 @@
         <v>436</v>
       </c>
       <c r="B441" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C441" s="24" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D441" s="12"/>
     </row>
@@ -7664,10 +7669,10 @@
         <v>437</v>
       </c>
       <c r="B442" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C442" s="24" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D442" s="12"/>
     </row>
@@ -7677,10 +7682,10 @@
         <v>438</v>
       </c>
       <c r="B443" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C443" s="24" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D443" s="12"/>
     </row>
@@ -7690,10 +7695,10 @@
         <v>439</v>
       </c>
       <c r="B444" s="10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C444" s="24" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D444" s="12"/>
     </row>
@@ -7703,10 +7708,10 @@
         <v>440</v>
       </c>
       <c r="B445" s="10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C445" s="24" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D445" s="12"/>
     </row>
@@ -7716,10 +7721,10 @@
         <v>441</v>
       </c>
       <c r="B446" s="10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C446" s="24" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D446" s="12"/>
     </row>
@@ -7729,10 +7734,10 @@
         <v>442</v>
       </c>
       <c r="B447" s="10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C447" s="24" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D447" s="12"/>
     </row>
@@ -7742,10 +7747,10 @@
         <v>443</v>
       </c>
       <c r="B448" s="10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C448" s="24" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D448" s="12"/>
     </row>
@@ -7755,10 +7760,10 @@
         <v>444</v>
       </c>
       <c r="B449" s="10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C449" s="24" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D449" s="12"/>
     </row>
@@ -7768,10 +7773,10 @@
         <v>445</v>
       </c>
       <c r="B450" s="10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C450" s="24" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D450" s="12"/>
     </row>
@@ -7781,10 +7786,10 @@
         <v>446</v>
       </c>
       <c r="B451" s="10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C451" s="24" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D451" s="12"/>
     </row>
@@ -7794,10 +7799,10 @@
         <v>447</v>
       </c>
       <c r="B452" s="10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C452" s="24" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D452" s="12"/>
     </row>
@@ -7807,10 +7812,10 @@
         <v>448</v>
       </c>
       <c r="B453" s="10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C453" s="24" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D453" s="12"/>
     </row>

</xml_diff>

<commit_message>
done Q70 search a word in 2d character grid
</commit_message>
<xml_diff>
--- a/DSA_450_LoveBabbar.xlsx
+++ b/DSA_450_LoveBabbar.xlsx
@@ -1942,11 +1942,11 @@
   </sheetPr>
   <dimension ref="A1:D467"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D76" activeCellId="0" sqref="D76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A62" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C76" activeCellId="0" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.24"/>
@@ -2900,7 +2900,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="n">
         <f aca="false">A74 + 1</f>
         <v>70</v>
@@ -2908,7 +2908,7 @@
       <c r="B75" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C75" s="24" t="s">
+      <c r="C75" s="13" t="s">
         <v>88</v>
       </c>
       <c r="D75" s="12"/>
@@ -8313,7 +8313,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>